<commit_message>
Fixed the s county codes
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/il_courts.xlsx
+++ b/docassemble/ILAO/data/sources/il_courts.xlsx
@@ -1759,106 +1759,106 @@
     <t xml:space="preserve">Harrisburg</t>
   </si>
   <si>
+    <t xml:space="preserve">Saline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sangamon County Courthouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(217) 753-6674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 South 9th Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Springfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sangamon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://co.sangamon.il.us/courts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sangamon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schuyler County Courthouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(217) 322-4633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102 S. Congress Street, Suite 103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rushville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schuyler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schuyler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scott County Courthouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(217) 742-5217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35 E Market St</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Winchester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelby County Courthouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(217) 774-4212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">301 E. MainSt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelbyville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Clair County Courthouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(618) 277-6600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Public Square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belleville</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Clair</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.co.st-clair.il.us</t>
+  </si>
+  <si>
     <t xml:space="preserve">stclair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sangamon County Courthouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(217) 753-6674</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200 South 9th Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Springfield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://co.sangamon.il.us/courts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schuyler County Courthouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(217) 322-4633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">102 S. Congress Street, Suite 103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rushville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sangamon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sangmon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scott County Courthouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(217) 742-5217</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35 E Market St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Winchester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schuyler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schuyler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shelby County Courthouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(217) 774-4212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">301 E. MainSt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shelbyville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scott</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scott</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Clair County Courthouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(618) 277-6600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 Public Square</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belleville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shelby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.co.st-clair.il.us</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schelby</t>
   </si>
   <si>
     <t xml:space="preserve">Stark County Courthouse</t>
@@ -2219,11 +2219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2247,28 +2243,28 @@
   </sheetPr>
   <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="S19" activeCellId="0" sqref="S19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="R97" activeCellId="0" sqref="R97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="2.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="33.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="110.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18"/>
@@ -2297,7 +2293,7 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
@@ -2306,25 +2302,25 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="0" t="s">
@@ -2350,25 +2346,25 @@
       <c r="C2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="0" t="s">
         <v>25</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="O2" s="0" t="n">
         <v>62301</v>
       </c>
       <c r="P2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="0" t="s">
         <v>28</v>
       </c>
       <c r="R2" s="0" t="s">
@@ -2385,25 +2381,25 @@
       <c r="C3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="0" t="s">
         <v>33</v>
       </c>
       <c r="N3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="1" t="n">
+      <c r="O3" s="0" t="n">
         <v>62914</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="0" t="s">
         <v>35</v>
       </c>
       <c r="R3" s="0" t="s">
@@ -2420,25 +2416,25 @@
       <c r="C4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="0" t="s">
         <v>40</v>
       </c>
       <c r="N4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="1" t="n">
+      <c r="O4" s="0" t="n">
         <v>62246</v>
       </c>
       <c r="P4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R4" s="0" t="s">
@@ -2455,25 +2451,25 @@
       <c r="C5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="0" t="s">
         <v>47</v>
       </c>
       <c r="N5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="1" t="n">
+      <c r="O5" s="0" t="n">
         <v>61008</v>
       </c>
       <c r="P5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="0" t="s">
         <v>49</v>
       </c>
       <c r="R5" s="0" t="s">
@@ -2490,25 +2486,25 @@
       <c r="C6" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="0" t="s">
         <v>54</v>
       </c>
       <c r="N6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="1" t="n">
+      <c r="O6" s="0" t="n">
         <v>62353</v>
       </c>
       <c r="P6" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="0" t="s">
         <v>56</v>
       </c>
       <c r="R6" s="0" t="s">
@@ -2525,25 +2521,25 @@
       <c r="C7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="0" t="s">
         <v>61</v>
       </c>
       <c r="N7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="1" t="n">
+      <c r="O7" s="0" t="n">
         <v>61356</v>
       </c>
       <c r="P7" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="0" t="s">
         <v>63</v>
       </c>
       <c r="R7" s="0" t="s">
@@ -2560,25 +2556,25 @@
       <c r="C8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="0" t="s">
         <v>68</v>
       </c>
       <c r="N8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="1" t="n">
+      <c r="O8" s="0" t="n">
         <v>62047</v>
       </c>
       <c r="P8" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="0" t="s">
         <v>56</v>
       </c>
       <c r="R8" s="0" t="s">
@@ -2595,25 +2591,25 @@
       <c r="C9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="0" t="s">
         <v>74</v>
       </c>
       <c r="N9" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="1" t="n">
+      <c r="O9" s="0" t="n">
         <v>61053</v>
       </c>
       <c r="P9" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="0" t="s">
         <v>76</v>
       </c>
       <c r="R9" s="0" t="s">
@@ -2630,25 +2626,25 @@
       <c r="C10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="0" t="s">
         <v>81</v>
       </c>
       <c r="N10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="1" t="n">
+      <c r="O10" s="0" t="n">
         <v>62691</v>
       </c>
       <c r="P10" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="0" t="s">
         <v>56</v>
       </c>
       <c r="R10" s="0" t="s">
@@ -2665,25 +2661,25 @@
       <c r="C11" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="0" t="s">
         <v>87</v>
       </c>
       <c r="N11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="1" t="n">
+      <c r="O11" s="0" t="n">
         <v>61801</v>
       </c>
       <c r="P11" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="0" t="s">
         <v>89</v>
       </c>
       <c r="R11" s="0" t="s">
@@ -2700,25 +2696,25 @@
       <c r="C12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="0" t="s">
         <v>94</v>
       </c>
       <c r="N12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="1" t="n">
+      <c r="O12" s="0" t="n">
         <v>62568</v>
       </c>
       <c r="P12" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R12" s="0" t="s">
@@ -2735,25 +2731,25 @@
       <c r="C13" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M13" s="0" t="s">
         <v>101</v>
       </c>
       <c r="N13" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="1" t="n">
+      <c r="O13" s="0" t="n">
         <v>62441</v>
       </c>
       <c r="P13" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" s="0" t="s">
         <v>103</v>
       </c>
       <c r="R13" s="0" t="s">
@@ -2770,25 +2766,25 @@
       <c r="C14" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M14" s="0" t="s">
         <v>108</v>
       </c>
       <c r="N14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="1" t="n">
+      <c r="O14" s="0" t="n">
         <v>62858</v>
       </c>
       <c r="P14" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R14" s="0" t="s">
@@ -2805,25 +2801,25 @@
       <c r="C15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="M15" s="0" t="s">
         <v>114</v>
       </c>
       <c r="N15" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O15" s="1" t="n">
+      <c r="O15" s="0" t="n">
         <v>62231</v>
       </c>
       <c r="P15" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="Q15" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R15" s="0" t="s">
@@ -2840,25 +2836,25 @@
       <c r="C16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="M16" s="0" t="s">
         <v>120</v>
       </c>
       <c r="N16" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="1" t="n">
+      <c r="O16" s="0" t="n">
         <v>61920</v>
       </c>
       <c r="P16" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" s="0" t="s">
         <v>103</v>
       </c>
       <c r="R16" s="0" t="s">
@@ -2878,25 +2874,25 @@
       <c r="D17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="M17" s="0" t="s">
         <v>126</v>
       </c>
       <c r="N17" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O17" s="1" t="n">
+      <c r="O17" s="0" t="n">
         <v>60602</v>
       </c>
       <c r="P17" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" s="0" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2913,25 +2909,25 @@
       <c r="D18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="M18" s="0" t="s">
         <v>132</v>
       </c>
       <c r="N18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="1" t="n">
+      <c r="O18" s="0" t="n">
         <v>60077</v>
       </c>
       <c r="P18" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" s="0" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2948,25 +2944,25 @@
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M19" s="0" t="s">
         <v>137</v>
       </c>
       <c r="N19" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O19" s="1" t="n">
+      <c r="O19" s="0" t="n">
         <v>60008</v>
       </c>
       <c r="P19" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q19" s="0" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2983,25 +2979,25 @@
       <c r="D20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M20" s="0" t="s">
         <v>142</v>
       </c>
       <c r="N20" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O20" s="1" t="n">
+      <c r="O20" s="0" t="n">
         <v>60153</v>
       </c>
       <c r="P20" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="Q20" s="0" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3018,25 +3014,25 @@
       <c r="D21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K21" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="M21" s="0" t="s">
         <v>147</v>
       </c>
       <c r="N21" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O21" s="1" t="n">
+      <c r="O21" s="0" t="n">
         <v>60455</v>
       </c>
       <c r="P21" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="Q21" s="0" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3053,25 +3049,25 @@
       <c r="D22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K22" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="M22" s="0" t="s">
         <v>152</v>
       </c>
       <c r="N22" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O22" s="1" t="n">
+      <c r="O22" s="0" t="n">
         <v>60428</v>
       </c>
       <c r="P22" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="0" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3085,25 +3081,25 @@
       <c r="C23" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K23" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M23" s="0" t="s">
         <v>126</v>
       </c>
       <c r="N23" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O23" s="1" t="n">
+      <c r="O23" s="0" t="n">
         <v>60607</v>
       </c>
       <c r="P23" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="Q23" s="0" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3117,25 +3113,25 @@
       <c r="C24" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K24" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M24" s="0" t="s">
         <v>126</v>
       </c>
       <c r="N24" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O24" s="1" t="n">
+      <c r="O24" s="0" t="n">
         <v>60608</v>
       </c>
       <c r="P24" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q24" s="0" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3149,25 +3145,25 @@
       <c r="C25" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K25" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M25" s="0" t="s">
         <v>126</v>
       </c>
       <c r="N25" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O25" s="1" t="n">
+      <c r="O25" s="0" t="n">
         <v>60612</v>
       </c>
       <c r="P25" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q25" s="0" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3181,25 +3177,25 @@
       <c r="C26" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K26" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="M26" s="0" t="s">
         <v>166</v>
       </c>
       <c r="N26" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O26" s="1" t="n">
+      <c r="O26" s="0" t="n">
         <v>62454</v>
       </c>
       <c r="P26" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="Q26" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R26" s="0" t="s">
@@ -3216,25 +3212,25 @@
       <c r="C27" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="K27" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="M27" s="0" t="s">
         <v>173</v>
       </c>
       <c r="N27" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O27" s="1" t="n">
+      <c r="O27" s="0" t="n">
         <v>62468</v>
       </c>
       <c r="P27" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" s="0" t="s">
         <v>103</v>
       </c>
       <c r="R27" s="0" t="s">
@@ -3251,25 +3247,25 @@
       <c r="C28" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="K28" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="M28" s="0" t="s">
         <v>179</v>
       </c>
       <c r="N28" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O28" s="1" t="n">
+      <c r="O28" s="0" t="n">
         <v>60178</v>
       </c>
       <c r="P28" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="Q28" s="0" t="s">
         <v>181</v>
       </c>
       <c r="R28" s="0" t="s">
@@ -3286,25 +3282,25 @@
       <c r="C29" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="K29" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="M29" s="0" t="s">
         <v>115</v>
       </c>
       <c r="N29" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="1" t="n">
+      <c r="O29" s="0" t="n">
         <v>61727</v>
       </c>
       <c r="P29" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="Q29" s="0" t="s">
         <v>187</v>
       </c>
       <c r="R29" s="0" t="s">
@@ -3321,25 +3317,25 @@
       <c r="C30" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="K30" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="M30" s="0" t="s">
         <v>192</v>
       </c>
       <c r="N30" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O30" s="1" t="n">
+      <c r="O30" s="0" t="n">
         <v>61953</v>
       </c>
       <c r="P30" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="Q30" s="0" t="s">
         <v>187</v>
       </c>
       <c r="R30" s="0" t="s">
@@ -3356,25 +3352,25 @@
       <c r="C31" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="K31" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="M31" s="0" t="s">
         <v>198</v>
       </c>
       <c r="N31" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O31" s="1" t="n">
+      <c r="O31" s="0" t="n">
         <v>60187</v>
       </c>
       <c r="P31" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="Q31" s="0" t="s">
         <v>200</v>
       </c>
       <c r="R31" s="0" t="s">
@@ -3391,25 +3387,25 @@
       <c r="C32" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="K32" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="M32" s="0" t="s">
         <v>205</v>
       </c>
       <c r="N32" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O32" s="1" t="n">
+      <c r="O32" s="0" t="n">
         <v>61944</v>
       </c>
       <c r="P32" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q32" s="0" t="s">
         <v>103</v>
       </c>
       <c r="R32" s="0" t="s">
@@ -3426,25 +3422,25 @@
       <c r="C33" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="K33" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="M33" s="0" t="s">
         <v>211</v>
       </c>
       <c r="N33" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O33" s="1" t="n">
+      <c r="O33" s="0" t="n">
         <v>62806</v>
       </c>
       <c r="P33" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="Q33" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R33" s="0" t="s">
@@ -3461,25 +3457,25 @@
       <c r="C34" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="K34" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="M34" s="0" t="s">
         <v>217</v>
       </c>
       <c r="N34" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O34" s="1" t="n">
+      <c r="O34" s="0" t="n">
         <v>62401</v>
       </c>
       <c r="P34" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="Q34" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R34" s="0" t="s">
@@ -3496,25 +3492,25 @@
       <c r="C35" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="K35" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="M35" s="0" t="s">
         <v>222</v>
       </c>
       <c r="N35" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O35" s="1" t="n">
+      <c r="O35" s="0" t="n">
         <v>62471</v>
       </c>
       <c r="P35" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="Q35" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R35" s="0" t="s">
@@ -3531,25 +3527,25 @@
       <c r="C36" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H36" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="K36" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="M36" s="0" t="s">
         <v>228</v>
       </c>
       <c r="N36" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O36" s="1" t="n">
+      <c r="O36" s="0" t="n">
         <v>60957</v>
       </c>
       <c r="P36" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="Q36" s="0" t="s">
         <v>230</v>
       </c>
       <c r="R36" s="0" t="s">
@@ -3566,25 +3562,25 @@
       <c r="C37" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H37" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="K37" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="M37" s="0" t="s">
         <v>235</v>
       </c>
       <c r="N37" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O37" s="1" t="n">
+      <c r="O37" s="0" t="n">
         <v>62812</v>
       </c>
       <c r="P37" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="Q37" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R37" s="0" t="s">
@@ -3601,25 +3597,25 @@
       <c r="C38" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="K38" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="M38" s="0" t="s">
         <v>241</v>
       </c>
       <c r="N38" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O38" s="1" t="n">
+      <c r="O38" s="0" t="n">
         <v>61542</v>
       </c>
       <c r="P38" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="Q38" s="0" t="s">
         <v>243</v>
       </c>
       <c r="R38" s="0" t="s">
@@ -3636,25 +3632,25 @@
       <c r="C39" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="K39" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="M39" s="0" t="s">
         <v>248</v>
       </c>
       <c r="N39" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O39" s="1" t="n">
+      <c r="O39" s="0" t="n">
         <v>62984</v>
       </c>
       <c r="P39" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="Q39" s="1" t="s">
+      <c r="Q39" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R39" s="0" t="s">
@@ -3671,25 +3667,25 @@
       <c r="C40" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="K40" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="M40" s="0" t="s">
         <v>254</v>
       </c>
       <c r="N40" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O40" s="1" t="n">
+      <c r="O40" s="0" t="n">
         <v>62016</v>
       </c>
       <c r="P40" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="Q40" s="0" t="s">
         <v>256</v>
       </c>
       <c r="R40" s="0" t="s">
@@ -3706,25 +3702,25 @@
       <c r="C41" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="K41" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="M41" s="0" t="s">
         <v>261</v>
       </c>
       <c r="N41" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O41" s="1" t="n">
+      <c r="O41" s="0" t="n">
         <v>60450</v>
       </c>
       <c r="P41" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="Q41" s="1" t="s">
+      <c r="Q41" s="0" t="s">
         <v>263</v>
       </c>
       <c r="R41" s="0" t="s">
@@ -3741,25 +3737,25 @@
       <c r="C42" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="K42" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="M42" s="0" t="s">
         <v>268</v>
       </c>
       <c r="N42" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O42" s="1" t="n">
+      <c r="O42" s="0" t="n">
         <v>62859</v>
       </c>
       <c r="P42" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="Q42" s="1" t="s">
+      <c r="Q42" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R42" s="0" t="s">
@@ -3776,25 +3772,25 @@
       <c r="C43" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="K43" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="M43" s="0" t="s">
         <v>274</v>
       </c>
       <c r="N43" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O43" s="1" t="n">
+      <c r="O43" s="0" t="n">
         <v>62321</v>
       </c>
       <c r="P43" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="Q43" s="0" t="s">
         <v>276</v>
       </c>
       <c r="R43" s="0" t="s">
@@ -3811,25 +3807,25 @@
       <c r="C44" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="K44" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="M44" s="0" t="s">
         <v>281</v>
       </c>
       <c r="N44" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O44" s="1" t="n">
+      <c r="O44" s="0" t="n">
         <v>62931</v>
       </c>
       <c r="P44" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="Q44" s="1" t="s">
+      <c r="Q44" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R44" s="0" t="s">
@@ -3846,25 +3842,25 @@
       <c r="C45" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="K45" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="M45" s="0" t="s">
         <v>286</v>
       </c>
       <c r="N45" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O45" s="1" t="n">
+      <c r="O45" s="0" t="n">
         <v>61469</v>
       </c>
       <c r="P45" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="Q45" s="0" t="s">
         <v>288</v>
       </c>
       <c r="R45" s="0" t="s">
@@ -3881,25 +3877,25 @@
       <c r="C46" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="K46" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="M46" s="0" t="s">
         <v>293</v>
       </c>
       <c r="N46" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O46" s="1" t="n">
+      <c r="O46" s="0" t="n">
         <v>61238</v>
       </c>
       <c r="P46" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="Q46" s="1" t="s">
+      <c r="Q46" s="0" t="s">
         <v>295</v>
       </c>
       <c r="R46" s="0" t="s">
@@ -3916,25 +3912,25 @@
       <c r="C47" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="K47" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="M47" s="0" t="s">
         <v>300</v>
       </c>
       <c r="N47" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O47" s="1" t="n">
+      <c r="O47" s="0" t="n">
         <v>60970</v>
       </c>
       <c r="P47" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="Q47" s="1" t="s">
+      <c r="Q47" s="0" t="s">
         <v>302</v>
       </c>
       <c r="R47" s="0" t="s">
@@ -3951,25 +3947,25 @@
       <c r="C48" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="K48" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="M48" s="0" t="s">
         <v>307</v>
       </c>
       <c r="N48" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O48" s="1" t="n">
+      <c r="O48" s="0" t="n">
         <v>62966</v>
       </c>
       <c r="P48" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="Q48" s="1" t="s">
+      <c r="Q48" s="0" t="s">
         <v>35</v>
       </c>
       <c r="R48" s="0" t="s">
@@ -3986,25 +3982,25 @@
       <c r="C49" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H49" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="K49" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="M49" s="0" t="s">
         <v>313</v>
       </c>
       <c r="N49" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O49" s="1" t="n">
+      <c r="O49" s="0" t="n">
         <v>62448</v>
       </c>
       <c r="P49" s="0" t="s">
         <v>314</v>
       </c>
-      <c r="Q49" s="1" t="s">
+      <c r="Q49" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R49" s="0" t="s">
@@ -4021,25 +4017,25 @@
       <c r="C50" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H50" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="K50" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="M50" s="0" t="s">
         <v>319</v>
       </c>
       <c r="N50" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O50" s="1" t="n">
+      <c r="O50" s="0" t="n">
         <v>62864</v>
       </c>
       <c r="P50" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="Q50" s="1" t="s">
+      <c r="Q50" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R50" s="0" t="s">
@@ -4056,25 +4052,25 @@
       <c r="C51" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H51" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="K51" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="M51" s="1" t="s">
+      <c r="M51" s="0" t="s">
         <v>325</v>
       </c>
       <c r="N51" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O51" s="1" t="n">
+      <c r="O51" s="0" t="n">
         <v>62052</v>
       </c>
       <c r="P51" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="Q51" s="1" t="s">
+      <c r="Q51" s="0" t="s">
         <v>256</v>
       </c>
       <c r="R51" s="0" t="s">
@@ -4091,25 +4087,25 @@
       <c r="C52" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="H52" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="K52" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="M52" s="1" t="s">
+      <c r="M52" s="0" t="s">
         <v>331</v>
       </c>
       <c r="N52" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O52" s="1" t="n">
+      <c r="O52" s="0" t="n">
         <v>61036</v>
       </c>
       <c r="P52" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="Q52" s="1" t="s">
+      <c r="Q52" s="0" t="s">
         <v>76</v>
       </c>
       <c r="R52" s="0" t="s">
@@ -4126,25 +4122,25 @@
       <c r="C53" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="H53" s="0" t="s">
         <v>335</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="K53" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="M53" s="1" t="s">
+      <c r="M53" s="0" t="s">
         <v>337</v>
       </c>
       <c r="N53" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O53" s="1" t="n">
+      <c r="O53" s="0" t="n">
         <v>62995</v>
       </c>
       <c r="P53" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="Q53" s="1" t="s">
+      <c r="Q53" s="0" t="s">
         <v>35</v>
       </c>
       <c r="R53" s="0" t="s">
@@ -4161,25 +4157,25 @@
       <c r="C54" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" s="0" t="s">
         <v>341</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="K54" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="M54" s="1" t="s">
+      <c r="M54" s="0" t="s">
         <v>343</v>
       </c>
       <c r="N54" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O54" s="1" t="n">
+      <c r="O54" s="0" t="n">
         <v>60174</v>
       </c>
       <c r="P54" s="0" t="s">
         <v>344</v>
       </c>
-      <c r="Q54" s="1" t="s">
+      <c r="Q54" s="0" t="s">
         <v>345</v>
       </c>
       <c r="R54" s="0" t="s">
@@ -4196,25 +4192,25 @@
       <c r="C55" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H55" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="K55" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="M55" s="1" t="s">
+      <c r="M55" s="0" t="s">
         <v>350</v>
       </c>
       <c r="N55" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O55" s="1" t="n">
+      <c r="O55" s="0" t="n">
         <v>60901</v>
       </c>
       <c r="P55" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="Q55" s="1" t="s">
+      <c r="Q55" s="0" t="s">
         <v>302</v>
       </c>
       <c r="R55" s="0" t="s">
@@ -4231,25 +4227,25 @@
       <c r="C56" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="K56" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="M56" s="1" t="s">
+      <c r="M56" s="0" t="s">
         <v>355</v>
       </c>
       <c r="N56" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O56" s="1" t="n">
+      <c r="O56" s="0" t="n">
         <v>60543</v>
       </c>
       <c r="P56" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="Q56" s="1" t="s">
+      <c r="Q56" s="0" t="s">
         <v>357</v>
       </c>
       <c r="R56" s="0" t="s">
@@ -4266,25 +4262,25 @@
       <c r="C57" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="H57" s="0" t="s">
         <v>360</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="K57" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="M57" s="1" t="s">
+      <c r="M57" s="0" t="s">
         <v>362</v>
       </c>
       <c r="N57" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O57" s="1" t="n">
+      <c r="O57" s="0" t="n">
         <v>61401</v>
       </c>
       <c r="P57" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="Q57" s="1" t="s">
+      <c r="Q57" s="0" t="s">
         <v>364</v>
       </c>
       <c r="R57" s="0" t="s">
@@ -4301,25 +4297,25 @@
       <c r="C58" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="H58" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="K58" s="0" t="s">
         <v>368</v>
       </c>
-      <c r="M58" s="1" t="s">
+      <c r="M58" s="0" t="s">
         <v>369</v>
       </c>
       <c r="N58" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O58" s="1" t="n">
+      <c r="O58" s="0" t="n">
         <v>60085</v>
       </c>
       <c r="P58" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="Q58" s="1" t="s">
+      <c r="Q58" s="0" t="s">
         <v>371</v>
       </c>
       <c r="R58" s="0" t="s">
@@ -4336,19 +4332,19 @@
       <c r="C59" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="H59" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="K59" s="0" t="s">
         <v>375</v>
       </c>
-      <c r="M59" s="1" t="s">
+      <c r="M59" s="0" t="s">
         <v>376</v>
       </c>
       <c r="N59" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O59" s="1" t="n">
+      <c r="O59" s="0" t="n">
         <v>61350</v>
       </c>
       <c r="P59" s="0" t="s">
@@ -4368,25 +4364,25 @@
       <c r="C60" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H60" s="1" t="s">
+      <c r="H60" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="K60" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="M60" s="1" t="s">
+      <c r="M60" s="0" t="s">
         <v>382</v>
       </c>
       <c r="N60" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O60" s="1" t="n">
+      <c r="O60" s="0" t="n">
         <v>62439</v>
       </c>
       <c r="P60" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="Q60" s="1" t="s">
+      <c r="Q60" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R60" s="0" t="s">
@@ -4403,25 +4399,25 @@
       <c r="C61" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="H61" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="K61" s="0" t="s">
         <v>387</v>
       </c>
-      <c r="M61" s="1" t="s">
+      <c r="M61" s="0" t="s">
         <v>388</v>
       </c>
       <c r="N61" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O61" s="1" t="n">
+      <c r="O61" s="0" t="n">
         <v>61021</v>
       </c>
       <c r="P61" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="Q61" s="1" t="s">
+      <c r="Q61" s="0" t="s">
         <v>390</v>
       </c>
       <c r="R61" s="0" t="s">
@@ -4438,25 +4434,25 @@
       <c r="C62" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="H62" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="K62" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="M62" s="1" t="s">
+      <c r="M62" s="0" t="s">
         <v>395</v>
       </c>
       <c r="N62" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O62" s="1" t="n">
+      <c r="O62" s="0" t="n">
         <v>61764</v>
       </c>
       <c r="P62" s="0" t="s">
         <v>396</v>
       </c>
-      <c r="Q62" s="1" t="s">
+      <c r="Q62" s="0" t="s">
         <v>397</v>
       </c>
       <c r="R62" s="0" t="s">
@@ -4473,25 +4469,25 @@
       <c r="C63" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="H63" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="K63" s="1" t="s">
+      <c r="K63" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="M63" s="1" t="s">
+      <c r="M63" s="0" t="s">
         <v>402</v>
       </c>
       <c r="N63" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O63" s="1" t="n">
+      <c r="O63" s="0" t="n">
         <v>62656</v>
       </c>
       <c r="P63" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="Q63" s="1" t="s">
+      <c r="Q63" s="0" t="s">
         <v>230</v>
       </c>
       <c r="R63" s="0" t="s">
@@ -4508,25 +4504,25 @@
       <c r="C64" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="H64" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="K64" s="1" t="s">
+      <c r="K64" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="M64" s="1" t="s">
+      <c r="M64" s="0" t="s">
         <v>408</v>
       </c>
       <c r="N64" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O64" s="1" t="n">
+      <c r="O64" s="0" t="n">
         <v>62523</v>
       </c>
       <c r="P64" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="Q64" s="1" t="s">
+      <c r="Q64" s="0" t="s">
         <v>187</v>
       </c>
       <c r="R64" s="0" t="s">
@@ -4543,25 +4539,25 @@
       <c r="C65" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="H65" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="K65" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="M65" s="1" t="s">
+      <c r="M65" s="0" t="s">
         <v>414</v>
       </c>
       <c r="N65" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O65" s="1" t="n">
+      <c r="O65" s="0" t="n">
         <v>62626</v>
       </c>
       <c r="P65" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="Q65" s="1" t="s">
+      <c r="Q65" s="0" t="s">
         <v>256</v>
       </c>
       <c r="R65" s="0" t="s">
@@ -4578,25 +4574,25 @@
       <c r="C66" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="H66" s="0" t="s">
         <v>418</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="K66" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="M66" s="1" t="s">
+      <c r="M66" s="0" t="s">
         <v>420</v>
       </c>
       <c r="N66" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O66" s="1" t="n">
+      <c r="O66" s="0" t="n">
         <v>62025</v>
       </c>
       <c r="P66" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="Q66" s="1" t="s">
+      <c r="Q66" s="0" t="s">
         <v>422</v>
       </c>
       <c r="R66" s="0" t="s">
@@ -4613,25 +4609,25 @@
       <c r="C67" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H67" s="1" t="s">
+      <c r="H67" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="K67" s="1" t="s">
+      <c r="K67" s="0" t="s">
         <v>426</v>
       </c>
-      <c r="M67" s="1" t="s">
+      <c r="M67" s="0" t="s">
         <v>427</v>
       </c>
       <c r="N67" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O67" s="1" t="n">
+      <c r="O67" s="0" t="n">
         <v>62881</v>
       </c>
       <c r="P67" s="0" t="s">
         <v>428</v>
       </c>
-      <c r="Q67" s="1" t="s">
+      <c r="Q67" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R67" s="0" t="s">
@@ -4648,25 +4644,25 @@
       <c r="C68" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="H68" s="0" t="s">
         <v>431</v>
       </c>
-      <c r="K68" s="1" t="s">
+      <c r="K68" s="0" t="s">
         <v>432</v>
       </c>
-      <c r="M68" s="1" t="s">
+      <c r="M68" s="0" t="s">
         <v>433</v>
       </c>
       <c r="N68" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O68" s="1" t="n">
+      <c r="O68" s="0" t="n">
         <v>61540</v>
       </c>
       <c r="P68" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="Q68" s="1" t="s">
+      <c r="Q68" s="0" t="s">
         <v>434</v>
       </c>
       <c r="R68" s="0" t="s">
@@ -4683,25 +4679,25 @@
       <c r="C69" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="H69" s="0" t="s">
         <v>437</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="K69" s="0" t="s">
         <v>438</v>
       </c>
-      <c r="M69" s="1" t="s">
+      <c r="M69" s="0" t="s">
         <v>439</v>
       </c>
       <c r="N69" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O69" s="1" t="n">
+      <c r="O69" s="0" t="n">
         <v>62644</v>
       </c>
       <c r="P69" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="Q69" s="1" t="s">
+      <c r="Q69" s="0" t="s">
         <v>56</v>
       </c>
       <c r="R69" s="0" t="s">
@@ -4718,25 +4714,25 @@
       <c r="C70" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H70" s="0" t="s">
         <v>443</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="K70" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="M70" s="1" t="s">
+      <c r="M70" s="0" t="s">
         <v>445</v>
       </c>
       <c r="N70" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O70" s="1" t="n">
+      <c r="O70" s="0" t="n">
         <v>62960</v>
       </c>
       <c r="P70" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="Q70" s="1" t="s">
+      <c r="Q70" s="0" t="s">
         <v>35</v>
       </c>
       <c r="R70" s="0" t="s">
@@ -4753,25 +4749,25 @@
       <c r="C71" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="H71" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="K71" s="1" t="s">
+      <c r="K71" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="M71" s="1" t="s">
+      <c r="M71" s="0" t="s">
         <v>451</v>
       </c>
       <c r="N71" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O71" s="1" t="n">
+      <c r="O71" s="0" t="n">
         <v>61455</v>
       </c>
       <c r="P71" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="Q71" s="1" t="s">
+      <c r="Q71" s="0" t="s">
         <v>453</v>
       </c>
       <c r="R71" s="0" t="s">
@@ -4788,25 +4784,25 @@
       <c r="C72" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="H72" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="K72" s="1" t="s">
+      <c r="K72" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="M72" s="1" t="s">
+      <c r="M72" s="0" t="s">
         <v>458</v>
       </c>
       <c r="N72" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O72" s="1" t="n">
+      <c r="O72" s="0" t="n">
         <v>60098</v>
       </c>
       <c r="P72" s="0" t="s">
         <v>459</v>
       </c>
-      <c r="Q72" s="1" t="s">
+      <c r="Q72" s="0" t="s">
         <v>460</v>
       </c>
       <c r="R72" s="0" t="s">
@@ -4823,25 +4819,25 @@
       <c r="C73" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="H73" s="0" t="s">
         <v>463</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="K73" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="M73" s="1" t="s">
+      <c r="M73" s="0" t="s">
         <v>465</v>
       </c>
       <c r="N73" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O73" s="1" t="n">
+      <c r="O73" s="0" t="n">
         <v>61701</v>
       </c>
       <c r="P73" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="Q73" s="1" t="s">
+      <c r="Q73" s="0" t="s">
         <v>467</v>
       </c>
       <c r="R73" s="0" t="s">
@@ -4858,25 +4854,25 @@
       <c r="C74" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="H74" s="0" t="s">
         <v>470</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="K74" s="0" t="s">
         <v>471</v>
       </c>
-      <c r="M74" s="1" t="s">
+      <c r="M74" s="0" t="s">
         <v>472</v>
       </c>
       <c r="N74" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O74" s="1" t="n">
+      <c r="O74" s="0" t="n">
         <v>62675</v>
       </c>
       <c r="P74" s="0" t="s">
         <v>473</v>
       </c>
-      <c r="Q74" s="1" t="s">
+      <c r="Q74" s="0" t="s">
         <v>474</v>
       </c>
       <c r="R74" s="0" t="s">
@@ -4893,25 +4889,25 @@
       <c r="C75" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H75" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="K75" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="M75" s="1" t="s">
+      <c r="M75" s="0" t="s">
         <v>479</v>
       </c>
       <c r="N75" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O75" s="1" t="n">
+      <c r="O75" s="0" t="n">
         <v>61231</v>
       </c>
       <c r="P75" s="0" t="s">
         <v>480</v>
       </c>
-      <c r="Q75" s="1" t="s">
+      <c r="Q75" s="0" t="s">
         <v>481</v>
       </c>
       <c r="R75" s="0" t="s">
@@ -4928,19 +4924,19 @@
       <c r="C76" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="H76" s="0" t="s">
         <v>484</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="K76" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="M76" s="1" t="s">
+      <c r="M76" s="0" t="s">
         <v>486</v>
       </c>
       <c r="N76" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O76" s="1" t="n">
+      <c r="O76" s="0" t="n">
         <v>62298</v>
       </c>
       <c r="P76" s="0" t="s">
@@ -4960,25 +4956,25 @@
       <c r="C77" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H77" s="1" t="s">
+      <c r="H77" s="0" t="s">
         <v>490</v>
       </c>
-      <c r="K77" s="1" t="s">
+      <c r="K77" s="0" t="s">
         <v>491</v>
       </c>
-      <c r="M77" s="1" t="s">
+      <c r="M77" s="0" t="s">
         <v>492</v>
       </c>
       <c r="N77" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O77" s="1" t="n">
+      <c r="O77" s="0" t="n">
         <v>62049</v>
       </c>
       <c r="P77" s="0" t="s">
         <v>493</v>
       </c>
-      <c r="Q77" s="1" t="s">
+      <c r="Q77" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R77" s="0" t="s">
@@ -4995,25 +4991,25 @@
       <c r="C78" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H78" s="1" t="s">
+      <c r="H78" s="0" t="s">
         <v>496</v>
       </c>
-      <c r="K78" s="1" t="s">
+      <c r="K78" s="0" t="s">
         <v>497</v>
       </c>
-      <c r="M78" s="1" t="s">
+      <c r="M78" s="0" t="s">
         <v>498</v>
       </c>
       <c r="N78" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O78" s="1" t="n">
+      <c r="O78" s="0" t="n">
         <v>62650</v>
       </c>
       <c r="P78" s="0" t="s">
         <v>499</v>
       </c>
-      <c r="Q78" s="1" t="s">
+      <c r="Q78" s="0" t="s">
         <v>256</v>
       </c>
       <c r="R78" s="0" t="s">
@@ -5030,25 +5026,25 @@
       <c r="C79" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H79" s="0" t="s">
         <v>502</v>
       </c>
-      <c r="K79" s="1" t="s">
+      <c r="K79" s="0" t="s">
         <v>503</v>
       </c>
-      <c r="M79" s="1" t="s">
+      <c r="M79" s="0" t="s">
         <v>504</v>
       </c>
       <c r="N79" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O79" s="1" t="n">
+      <c r="O79" s="0" t="n">
         <v>61951</v>
       </c>
       <c r="P79" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="Q79" s="1" t="s">
+      <c r="Q79" s="0" t="s">
         <v>187</v>
       </c>
       <c r="R79" s="0" t="s">
@@ -5065,25 +5061,25 @@
       <c r="C80" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="H80" s="0" t="s">
         <v>508</v>
       </c>
-      <c r="K80" s="1" t="s">
+      <c r="K80" s="0" t="s">
         <v>509</v>
       </c>
-      <c r="M80" s="1" t="s">
+      <c r="M80" s="0" t="s">
         <v>510</v>
       </c>
       <c r="N80" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O80" s="1" t="n">
+      <c r="O80" s="0" t="n">
         <v>61061</v>
       </c>
       <c r="P80" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="Q80" s="1" t="s">
+      <c r="Q80" s="0" t="s">
         <v>390</v>
       </c>
       <c r="R80" s="0" t="s">
@@ -5100,25 +5096,25 @@
       <c r="C81" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H81" s="1" t="s">
+      <c r="H81" s="0" t="s">
         <v>514</v>
       </c>
-      <c r="K81" s="1" t="s">
+      <c r="K81" s="0" t="s">
         <v>515</v>
       </c>
-      <c r="M81" s="1" t="s">
+      <c r="M81" s="0" t="s">
         <v>516</v>
       </c>
       <c r="N81" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O81" s="1" t="n">
+      <c r="O81" s="0" t="n">
         <v>61602</v>
       </c>
       <c r="P81" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="Q81" s="1" t="s">
+      <c r="Q81" s="0" t="s">
         <v>434</v>
       </c>
       <c r="R81" s="0" t="s">
@@ -5135,19 +5131,19 @@
       <c r="C82" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="H82" s="0" t="s">
         <v>519</v>
       </c>
-      <c r="K82" s="1" t="s">
+      <c r="K82" s="0" t="s">
         <v>520</v>
       </c>
-      <c r="M82" s="1" t="s">
+      <c r="M82" s="0" t="s">
         <v>521</v>
       </c>
       <c r="N82" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O82" s="1" t="n">
+      <c r="O82" s="0" t="n">
         <v>62274</v>
       </c>
       <c r="P82" s="0" t="s">
@@ -5167,25 +5163,25 @@
       <c r="C83" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H83" s="1" t="s">
+      <c r="H83" s="0" t="s">
         <v>525</v>
       </c>
-      <c r="K83" s="1" t="s">
+      <c r="K83" s="0" t="s">
         <v>526</v>
       </c>
-      <c r="M83" s="1" t="s">
+      <c r="M83" s="0" t="s">
         <v>527</v>
       </c>
       <c r="N83" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O83" s="1" t="n">
+      <c r="O83" s="0" t="n">
         <v>61856</v>
       </c>
       <c r="P83" s="0" t="s">
         <v>528</v>
       </c>
-      <c r="Q83" s="1" t="s">
+      <c r="Q83" s="0" t="s">
         <v>187</v>
       </c>
       <c r="R83" s="0" t="s">
@@ -5202,25 +5198,25 @@
       <c r="C84" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H84" s="1" t="s">
+      <c r="H84" s="0" t="s">
         <v>531</v>
       </c>
-      <c r="K84" s="1" t="s">
+      <c r="K84" s="0" t="s">
         <v>532</v>
       </c>
-      <c r="M84" s="1" t="s">
+      <c r="M84" s="0" t="s">
         <v>533</v>
       </c>
       <c r="N84" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O84" s="1" t="n">
+      <c r="O84" s="0" t="n">
         <v>62363</v>
       </c>
       <c r="P84" s="0" t="s">
         <v>534</v>
       </c>
-      <c r="Q84" s="1" t="s">
+      <c r="Q84" s="0" t="s">
         <v>535</v>
       </c>
       <c r="R84" s="0" t="s">
@@ -5237,25 +5233,25 @@
       <c r="C85" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H85" s="1" t="s">
+      <c r="H85" s="0" t="s">
         <v>538</v>
       </c>
-      <c r="K85" s="1" t="s">
+      <c r="K85" s="0" t="s">
         <v>539</v>
       </c>
-      <c r="M85" s="1" t="s">
+      <c r="M85" s="0" t="s">
         <v>540</v>
       </c>
       <c r="N85" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O85" s="1" t="n">
+      <c r="O85" s="0" t="n">
         <v>62938</v>
       </c>
       <c r="P85" s="0" t="s">
         <v>541</v>
       </c>
-      <c r="Q85" s="1" t="s">
+      <c r="Q85" s="0" t="s">
         <v>35</v>
       </c>
       <c r="R85" s="0" t="s">
@@ -5272,25 +5268,25 @@
       <c r="C86" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H86" s="1" t="s">
+      <c r="H86" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="K86" s="1" t="s">
+      <c r="K86" s="0" t="s">
         <v>545</v>
       </c>
-      <c r="M86" s="1" t="s">
+      <c r="M86" s="0" t="s">
         <v>546</v>
       </c>
       <c r="N86" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O86" s="1" t="n">
+      <c r="O86" s="0" t="n">
         <v>62963</v>
       </c>
       <c r="P86" s="0" t="s">
         <v>547</v>
       </c>
-      <c r="Q86" s="1" t="s">
+      <c r="Q86" s="0" t="s">
         <v>35</v>
       </c>
       <c r="R86" s="0" t="s">
@@ -5307,25 +5303,25 @@
       <c r="C87" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H87" s="1" t="s">
+      <c r="H87" s="0" t="s">
         <v>550</v>
       </c>
-      <c r="K87" s="1" t="s">
+      <c r="K87" s="0" t="s">
         <v>551</v>
       </c>
-      <c r="M87" s="1" t="s">
+      <c r="M87" s="0" t="s">
         <v>552</v>
       </c>
       <c r="N87" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O87" s="1" t="n">
+      <c r="O87" s="0" t="n">
         <v>61327</v>
       </c>
       <c r="P87" s="0" t="s">
         <v>553</v>
       </c>
-      <c r="Q87" s="1" t="s">
+      <c r="Q87" s="0" t="s">
         <v>554</v>
       </c>
       <c r="R87" s="0" t="s">
@@ -5342,25 +5338,25 @@
       <c r="C88" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H88" s="1" t="s">
+      <c r="H88" s="0" t="s">
         <v>557</v>
       </c>
-      <c r="K88" s="1" t="s">
+      <c r="K88" s="0" t="s">
         <v>558</v>
       </c>
-      <c r="M88" s="1" t="s">
+      <c r="M88" s="0" t="s">
         <v>559</v>
       </c>
       <c r="N88" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O88" s="1" t="n">
+      <c r="O88" s="0" t="n">
         <v>62233</v>
       </c>
       <c r="P88" s="0" t="s">
         <v>560</v>
       </c>
-      <c r="Q88" s="1" t="s">
+      <c r="Q88" s="0" t="s">
         <v>561</v>
       </c>
       <c r="R88" s="0" t="s">
@@ -5377,25 +5373,25 @@
       <c r="C89" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H89" s="1" t="s">
+      <c r="H89" s="0" t="s">
         <v>564</v>
       </c>
-      <c r="K89" s="1" t="s">
+      <c r="K89" s="0" t="s">
         <v>565</v>
       </c>
-      <c r="M89" s="1" t="s">
+      <c r="M89" s="0" t="s">
         <v>566</v>
       </c>
       <c r="N89" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O89" s="1" t="n">
+      <c r="O89" s="0" t="n">
         <v>62450</v>
       </c>
       <c r="P89" s="0" t="s">
         <v>567</v>
       </c>
-      <c r="Q89" s="1" t="s">
+      <c r="Q89" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R89" s="0" t="s">
@@ -5412,25 +5408,25 @@
       <c r="C90" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H90" s="1" t="s">
+      <c r="H90" s="0" t="s">
         <v>570</v>
       </c>
-      <c r="K90" s="1" t="s">
+      <c r="K90" s="0" t="s">
         <v>571</v>
       </c>
-      <c r="M90" s="1" t="s">
+      <c r="M90" s="0" t="s">
         <v>572</v>
       </c>
       <c r="N90" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O90" s="1" t="n">
+      <c r="O90" s="0" t="n">
         <v>61201</v>
       </c>
       <c r="P90" s="0" t="s">
         <v>572</v>
       </c>
-      <c r="Q90" s="1" t="s">
+      <c r="Q90" s="0" t="s">
         <v>573</v>
       </c>
       <c r="R90" s="0" t="s">
@@ -5447,25 +5443,25 @@
       <c r="C91" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H91" s="1" t="s">
+      <c r="H91" s="0" t="s">
         <v>576</v>
       </c>
-      <c r="K91" s="1" t="s">
+      <c r="K91" s="0" t="s">
         <v>577</v>
       </c>
-      <c r="M91" s="1" t="s">
+      <c r="M91" s="0" t="s">
         <v>578</v>
       </c>
       <c r="N91" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O91" s="1" t="n">
+      <c r="O91" s="0" t="n">
         <v>62946</v>
       </c>
       <c r="P91" s="0" t="s">
         <v>579</v>
       </c>
-      <c r="Q91" s="1" t="s">
+      <c r="Q91" s="0" t="s">
         <v>35</v>
       </c>
       <c r="R91" s="0" t="s">
@@ -5482,25 +5478,25 @@
       <c r="C92" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H92" s="1" t="s">
+      <c r="H92" s="0" t="s">
         <v>582</v>
       </c>
-      <c r="K92" s="1" t="s">
+      <c r="K92" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="M92" s="1" t="s">
+      <c r="M92" s="0" t="s">
         <v>584</v>
       </c>
       <c r="N92" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O92" s="1" t="n">
+      <c r="O92" s="0" t="n">
         <v>62701</v>
       </c>
       <c r="P92" s="0" t="s">
         <v>585</v>
       </c>
-      <c r="Q92" s="1" t="s">
+      <c r="Q92" s="0" t="s">
         <v>586</v>
       </c>
       <c r="R92" s="0" t="s">
@@ -5517,25 +5513,25 @@
       <c r="C93" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H93" s="1" t="s">
+      <c r="H93" s="0" t="s">
         <v>589</v>
       </c>
-      <c r="K93" s="1" t="s">
+      <c r="K93" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="M93" s="1" t="s">
+      <c r="M93" s="0" t="s">
         <v>591</v>
       </c>
       <c r="N93" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O93" s="1" t="n">
+      <c r="O93" s="0" t="n">
         <v>62681</v>
       </c>
       <c r="P93" s="0" t="s">
         <v>592</v>
       </c>
-      <c r="Q93" s="1" t="s">
+      <c r="Q93" s="0" t="s">
         <v>56</v>
       </c>
       <c r="R93" s="0" t="s">
@@ -5552,25 +5548,25 @@
       <c r="C94" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H94" s="1" t="s">
+      <c r="H94" s="0" t="s">
         <v>595</v>
       </c>
-      <c r="K94" s="1" t="s">
+      <c r="K94" s="0" t="s">
         <v>596</v>
       </c>
-      <c r="M94" s="1" t="s">
+      <c r="M94" s="0" t="s">
         <v>597</v>
       </c>
       <c r="N94" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O94" s="1" t="n">
+      <c r="O94" s="0" t="n">
         <v>62694</v>
       </c>
       <c r="P94" s="0" t="s">
         <v>598</v>
       </c>
-      <c r="Q94" s="1" t="s">
+      <c r="Q94" s="0" t="s">
         <v>256</v>
       </c>
       <c r="R94" s="0" t="s">
@@ -5587,25 +5583,25 @@
       <c r="C95" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H95" s="1" t="s">
+      <c r="H95" s="0" t="s">
         <v>601</v>
       </c>
-      <c r="K95" s="1" t="s">
+      <c r="K95" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="M95" s="1" t="s">
+      <c r="M95" s="0" t="s">
         <v>603</v>
       </c>
       <c r="N95" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O95" s="1" t="n">
+      <c r="O95" s="0" t="n">
         <v>62565</v>
       </c>
       <c r="P95" s="0" t="s">
         <v>604</v>
       </c>
-      <c r="Q95" s="1" t="s">
+      <c r="Q95" s="0" t="s">
         <v>96</v>
       </c>
       <c r="R95" s="0" t="s">
@@ -5622,25 +5618,25 @@
       <c r="C96" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H96" s="1" t="s">
+      <c r="H96" s="0" t="s">
         <v>607</v>
       </c>
-      <c r="K96" s="1" t="s">
+      <c r="K96" s="0" t="s">
         <v>608</v>
       </c>
-      <c r="M96" s="1" t="s">
+      <c r="M96" s="0" t="s">
         <v>609</v>
       </c>
       <c r="N96" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O96" s="1" t="n">
+      <c r="O96" s="0" t="n">
         <v>62220</v>
       </c>
       <c r="P96" s="0" t="s">
         <v>610</v>
       </c>
-      <c r="Q96" s="1" t="s">
+      <c r="Q96" s="0" t="s">
         <v>611</v>
       </c>
       <c r="R96" s="0" t="s">
@@ -5657,25 +5653,25 @@
       <c r="C97" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H97" s="1" t="s">
+      <c r="H97" s="0" t="s">
         <v>614</v>
       </c>
-      <c r="K97" s="1" t="s">
+      <c r="K97" s="0" t="s">
         <v>615</v>
       </c>
-      <c r="M97" s="1" t="s">
+      <c r="M97" s="0" t="s">
         <v>616</v>
       </c>
       <c r="N97" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O97" s="1" t="n">
+      <c r="O97" s="0" t="n">
         <v>61483</v>
       </c>
       <c r="P97" s="0" t="s">
         <v>617</v>
       </c>
-      <c r="Q97" s="1" t="s">
+      <c r="Q97" s="0" t="s">
         <v>618</v>
       </c>
       <c r="R97" s="0" t="s">
@@ -5692,25 +5688,25 @@
       <c r="C98" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H98" s="1" t="s">
+      <c r="H98" s="0" t="s">
         <v>621</v>
       </c>
-      <c r="K98" s="1" t="s">
+      <c r="K98" s="0" t="s">
         <v>622</v>
       </c>
-      <c r="M98" s="1" t="s">
+      <c r="M98" s="0" t="s">
         <v>623</v>
       </c>
       <c r="N98" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O98" s="1" t="n">
+      <c r="O98" s="0" t="n">
         <v>61032</v>
       </c>
       <c r="P98" s="0" t="s">
         <v>624</v>
       </c>
-      <c r="Q98" s="1" t="s">
+      <c r="Q98" s="0" t="s">
         <v>390</v>
       </c>
       <c r="R98" s="0" t="s">
@@ -5727,25 +5723,25 @@
       <c r="C99" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H99" s="1" t="s">
+      <c r="H99" s="0" t="s">
         <v>627</v>
       </c>
-      <c r="K99" s="1" t="s">
+      <c r="K99" s="0" t="s">
         <v>628</v>
       </c>
-      <c r="M99" s="1" t="s">
+      <c r="M99" s="0" t="s">
         <v>629</v>
       </c>
       <c r="N99" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O99" s="1" t="n">
+      <c r="O99" s="0" t="n">
         <v>61554</v>
       </c>
       <c r="P99" s="0" t="s">
         <v>630</v>
       </c>
-      <c r="Q99" s="1" t="s">
+      <c r="Q99" s="0" t="s">
         <v>631</v>
       </c>
       <c r="R99" s="0" t="s">
@@ -5762,25 +5758,25 @@
       <c r="C100" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H100" s="1" t="s">
+      <c r="H100" s="0" t="s">
         <v>634</v>
       </c>
-      <c r="K100" s="1" t="s">
+      <c r="K100" s="0" t="s">
         <v>635</v>
       </c>
-      <c r="M100" s="1" t="s">
+      <c r="M100" s="0" t="s">
         <v>636</v>
       </c>
       <c r="N100" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O100" s="1" t="n">
+      <c r="O100" s="0" t="n">
         <v>62952</v>
       </c>
       <c r="P100" s="0" t="s">
         <v>637</v>
       </c>
-      <c r="Q100" s="1" t="s">
+      <c r="Q100" s="0" t="s">
         <v>638</v>
       </c>
       <c r="R100" s="0" t="s">
@@ -5797,25 +5793,25 @@
       <c r="C101" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H101" s="1" t="s">
+      <c r="H101" s="0" t="s">
         <v>641</v>
       </c>
-      <c r="K101" s="1" t="s">
+      <c r="K101" s="0" t="s">
         <v>642</v>
       </c>
-      <c r="M101" s="1" t="s">
+      <c r="M101" s="0" t="s">
         <v>643</v>
       </c>
       <c r="N101" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O101" s="1" t="n">
+      <c r="O101" s="0" t="n">
         <v>61832</v>
       </c>
       <c r="P101" s="0" t="s">
         <v>644</v>
       </c>
-      <c r="Q101" s="1" t="s">
+      <c r="Q101" s="0" t="s">
         <v>103</v>
       </c>
       <c r="R101" s="0" t="s">
@@ -5832,25 +5828,25 @@
       <c r="C102" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H102" s="1" t="s">
+      <c r="H102" s="0" t="s">
         <v>647</v>
       </c>
-      <c r="K102" s="1" t="s">
+      <c r="K102" s="0" t="s">
         <v>648</v>
       </c>
-      <c r="M102" s="1" t="s">
+      <c r="M102" s="0" t="s">
         <v>649</v>
       </c>
       <c r="N102" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O102" s="1" t="n">
+      <c r="O102" s="0" t="n">
         <v>62863</v>
       </c>
       <c r="P102" s="0" t="s">
         <v>650</v>
       </c>
-      <c r="Q102" s="1" t="s">
+      <c r="Q102" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R102" s="0" t="s">
@@ -5867,25 +5863,25 @@
       <c r="C103" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H103" s="1" t="s">
+      <c r="H103" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="K103" s="1" t="s">
+      <c r="K103" s="0" t="s">
         <v>653</v>
       </c>
-      <c r="M103" s="1" t="s">
+      <c r="M103" s="0" t="s">
         <v>654</v>
       </c>
       <c r="N103" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O103" s="1" t="n">
+      <c r="O103" s="0" t="n">
         <v>61462</v>
       </c>
       <c r="P103" s="0" t="s">
         <v>655</v>
       </c>
-      <c r="Q103" s="1" t="s">
+      <c r="Q103" s="0" t="s">
         <v>656</v>
       </c>
       <c r="R103" s="0" t="s">
@@ -5902,19 +5898,19 @@
       <c r="C104" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H104" s="1" t="s">
+      <c r="H104" s="0" t="s">
         <v>659</v>
       </c>
-      <c r="K104" s="1" t="s">
+      <c r="K104" s="0" t="s">
         <v>660</v>
       </c>
-      <c r="M104" s="1" t="s">
+      <c r="M104" s="0" t="s">
         <v>661</v>
       </c>
       <c r="N104" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O104" s="1" t="n">
+      <c r="O104" s="0" t="n">
         <v>62263</v>
       </c>
       <c r="P104" s="0" t="s">
@@ -5934,25 +5930,25 @@
       <c r="C105" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H105" s="1" t="s">
+      <c r="H105" s="0" t="s">
         <v>665</v>
       </c>
-      <c r="K105" s="1" t="s">
+      <c r="K105" s="0" t="s">
         <v>666</v>
       </c>
-      <c r="M105" s="1" t="s">
+      <c r="M105" s="0" t="s">
         <v>667</v>
       </c>
       <c r="N105" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O105" s="1" t="n">
+      <c r="O105" s="0" t="n">
         <v>62837</v>
       </c>
       <c r="P105" s="0" t="s">
         <v>668</v>
       </c>
-      <c r="Q105" s="1" t="s">
+      <c r="Q105" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R105" s="0" t="s">
@@ -5969,25 +5965,25 @@
       <c r="C106" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H106" s="1" t="s">
+      <c r="H106" s="0" t="s">
         <v>671</v>
       </c>
-      <c r="K106" s="1" t="s">
+      <c r="K106" s="0" t="s">
         <v>672</v>
       </c>
-      <c r="M106" s="1" t="s">
+      <c r="M106" s="0" t="s">
         <v>673</v>
       </c>
       <c r="N106" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O106" s="1" t="n">
+      <c r="O106" s="0" t="n">
         <v>62821</v>
       </c>
       <c r="P106" s="0" t="s">
         <v>674</v>
       </c>
-      <c r="Q106" s="1" t="s">
+      <c r="Q106" s="0" t="s">
         <v>168</v>
       </c>
       <c r="R106" s="0" t="s">
@@ -6004,25 +6000,25 @@
       <c r="C107" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H107" s="1" t="s">
+      <c r="H107" s="0" t="s">
         <v>677</v>
       </c>
-      <c r="K107" s="1" t="s">
+      <c r="K107" s="0" t="s">
         <v>678</v>
       </c>
-      <c r="M107" s="1" t="s">
+      <c r="M107" s="0" t="s">
         <v>679</v>
       </c>
       <c r="N107" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O107" s="1" t="n">
+      <c r="O107" s="0" t="n">
         <v>61270</v>
       </c>
       <c r="P107" s="0" t="s">
         <v>680</v>
       </c>
-      <c r="Q107" s="1" t="s">
+      <c r="Q107" s="0" t="s">
         <v>681</v>
       </c>
       <c r="R107" s="0" t="s">
@@ -6039,25 +6035,25 @@
       <c r="C108" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H108" s="1" t="s">
+      <c r="H108" s="0" t="s">
         <v>684</v>
       </c>
-      <c r="K108" s="1" t="s">
+      <c r="K108" s="0" t="s">
         <v>685</v>
       </c>
-      <c r="M108" s="1" t="s">
+      <c r="M108" s="0" t="s">
         <v>686</v>
       </c>
       <c r="N108" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O108" s="1" t="n">
+      <c r="O108" s="0" t="n">
         <v>60432</v>
       </c>
       <c r="P108" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="Q108" s="1" t="s">
+      <c r="Q108" s="0" t="s">
         <v>688</v>
       </c>
       <c r="R108" s="0" t="s">
@@ -6074,25 +6070,25 @@
       <c r="C109" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H109" s="1" t="s">
+      <c r="H109" s="0" t="s">
         <v>691</v>
       </c>
-      <c r="K109" s="1" t="s">
+      <c r="K109" s="0" t="s">
         <v>692</v>
       </c>
-      <c r="M109" s="1" t="s">
+      <c r="M109" s="0" t="s">
         <v>428</v>
       </c>
       <c r="N109" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O109" s="1" t="n">
+      <c r="O109" s="0" t="n">
         <v>62959</v>
       </c>
       <c r="P109" s="0" t="s">
         <v>693</v>
       </c>
-      <c r="Q109" s="1" t="s">
+      <c r="Q109" s="0" t="s">
         <v>35</v>
       </c>
       <c r="R109" s="0" t="s">
@@ -6109,25 +6105,25 @@
       <c r="C110" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H110" s="1" t="s">
+      <c r="H110" s="0" t="s">
         <v>696</v>
       </c>
-      <c r="K110" s="1" t="s">
+      <c r="K110" s="0" t="s">
         <v>697</v>
       </c>
-      <c r="M110" s="1" t="s">
+      <c r="M110" s="0" t="s">
         <v>698</v>
       </c>
       <c r="N110" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O110" s="1" t="n">
+      <c r="O110" s="0" t="n">
         <v>61101</v>
       </c>
       <c r="P110" s="0" t="s">
         <v>699</v>
       </c>
-      <c r="Q110" s="1" t="s">
+      <c r="Q110" s="0" t="s">
         <v>49</v>
       </c>
       <c r="R110" s="0" t="s">
@@ -6144,25 +6140,25 @@
       <c r="C111" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H111" s="1" t="s">
+      <c r="H111" s="0" t="s">
         <v>702</v>
       </c>
-      <c r="K111" s="1" t="s">
+      <c r="K111" s="0" t="s">
         <v>703</v>
       </c>
-      <c r="M111" s="1" t="s">
+      <c r="M111" s="0" t="s">
         <v>704</v>
       </c>
       <c r="N111" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O111" s="1" t="n">
+      <c r="O111" s="0" t="n">
         <v>61530</v>
       </c>
       <c r="P111" s="0" t="s">
         <v>705</v>
       </c>
-      <c r="Q111" s="1" t="s">
+      <c r="Q111" s="0" t="s">
         <v>706</v>
       </c>
       <c r="R111" s="0" t="s">

</xml_diff>

<commit_message>
Lake and LaSalle were swapped
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/il_courts.xlsx
+++ b/docassemble/ILAO/data/sources/il_courts.xlsx
@@ -1132,31 +1132,31 @@
     <t xml:space="preserve">Waukegan</t>
   </si>
   <si>
+    <t xml:space="preserve">Lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.19thcircuitcourt.state.il.us/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LaSalle County Courthouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(815) 434-8671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119 West Madison Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ottawa</t>
+  </si>
+  <si>
     <t xml:space="preserve">LaSalle</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.19thcircuitcourt.state.il.us/</t>
-  </si>
-  <si>
     <t xml:space="preserve">lasalle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LaSalle County Courthouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(815) 434-8671</t>
-  </si>
-  <si>
-    <t xml:space="preserve">119 West Madison Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ottawa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lake</t>
   </si>
   <si>
     <t xml:space="preserve">Lawrence County Courthouse</t>
@@ -2244,27 +2244,27 @@
   <dimension ref="A1:U111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="R97" activeCellId="0" sqref="R97"/>
+      <selection pane="bottomLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="2.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="3.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="65.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18"/>

</xml_diff>

<commit_message>
More Tyler codes bugs
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/il_courts.xlsx
+++ b/docassemble/ILAO/data/sources/il_courts.xlsx
@@ -604,7 +604,7 @@
     <t xml:space="preserve">Douglas</t>
   </si>
   <si>
-    <t xml:space="preserve">douglass</t>
+    <t xml:space="preserve">douglas</t>
   </si>
   <si>
     <t xml:space="preserve">DuPage County Courthouse</t>
@@ -853,7 +853,7 @@
     <t xml:space="preserve">http://www.9thjudicial.org/Hancock/hancock.html</t>
   </si>
   <si>
-    <t xml:space="preserve">hankcock</t>
+    <t xml:space="preserve">hancock</t>
   </si>
   <si>
     <t xml:space="preserve">Hardin County Courthouse</t>
@@ -2244,12 +2244,12 @@
   <dimension ref="A1:U111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
+      <selection pane="bottomLeft" activeCell="E119" activeCellId="0" sqref="E119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.86"/>

</xml_diff>

<commit_message>
update interview list to handle exclusions, update courthouse address, update ilao easy form list
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/il_courts.xlsx
+++ b/docassemble/ILAO/data/sources/il_courts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80F4B1E-CE9E-402B-B770-824CADCDEA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1F8E4E-7545-4E92-A7BF-BD1FCD272D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="2985" windowWidth="32445" windowHeight="16515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5295" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,9 +639,6 @@
     <t>401 Court Street</t>
   </si>
   <si>
-    <t>540 S. Randall Rd.</t>
-  </si>
-  <si>
     <t>450 East Court Street</t>
   </si>
   <si>
@@ -894,9 +891,6 @@
     <t>Vienna</t>
   </si>
   <si>
-    <t>St. Charles</t>
-  </si>
-  <si>
     <t>Yorkville</t>
   </si>
   <si>
@@ -1843,6 +1837,12 @@
   </si>
   <si>
     <t>district</t>
+  </si>
+  <si>
+    <t>100 S. 3rd Street</t>
+  </si>
+  <si>
+    <t>Geneva</t>
   </si>
 </sst>
 </file>
@@ -1878,9 +1878,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2163,10 +2162,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,16 +2174,16 @@
     <col min="2" max="2" width="39.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="110.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="110.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
@@ -2201,7 +2200,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2212,7 +2211,7 @@
       <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
       <c r="I1" t="s">
@@ -2221,25 +2220,25 @@
       <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
       <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
       <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>122</v>
       </c>
       <c r="R1" t="s">
@@ -2257,30 +2256,30 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C2" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>151</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>138</v>
       </c>
       <c r="N2" t="s">
         <v>121</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2">
         <v>62301</v>
       </c>
       <c r="P2" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2289,30 +2288,30 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C3" t="s">
         <v>120</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>152</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>124</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" t="s">
         <v>139</v>
       </c>
       <c r="N3" t="s">
         <v>121</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3">
         <v>62914</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2321,30 +2320,30 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C4" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>153</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>125</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" t="s">
         <v>140</v>
       </c>
       <c r="N4" t="s">
         <v>121</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4">
         <v>62246</v>
       </c>
       <c r="P4" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2353,30 +2352,30 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C5" t="s">
         <v>120</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>154</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" t="s">
         <v>126</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" t="s">
         <v>141</v>
       </c>
       <c r="N5" t="s">
         <v>121</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5">
         <v>61008</v>
       </c>
       <c r="P5" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2385,30 +2384,30 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C6" t="s">
         <v>120</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>155</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" t="s">
         <v>142</v>
       </c>
       <c r="N6" t="s">
         <v>121</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6">
         <v>62353</v>
       </c>
       <c r="P6" t="s">
         <v>23</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2417,30 +2416,30 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C7" t="s">
         <v>120</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>156</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" t="s">
         <v>128</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" t="s">
         <v>143</v>
       </c>
       <c r="N7" t="s">
         <v>121</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7">
         <v>61356</v>
       </c>
       <c r="P7" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2449,30 +2448,30 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C8" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>157</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" t="s">
         <v>129</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" t="s">
         <v>53</v>
       </c>
       <c r="N8" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8">
         <v>62047</v>
       </c>
       <c r="P8" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2481,30 +2480,30 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C9" t="s">
         <v>120</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>158</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" t="s">
         <v>130</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" t="s">
         <v>144</v>
       </c>
       <c r="N9" t="s">
         <v>121</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9">
         <v>61053</v>
       </c>
       <c r="P9" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2513,30 +2512,30 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C10" t="s">
         <v>120</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>159</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" t="s">
         <v>131</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" t="s">
         <v>145</v>
       </c>
       <c r="N10" t="s">
         <v>121</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10">
         <v>62691</v>
       </c>
       <c r="P10" t="s">
         <v>27</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2545,30 +2544,30 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C11" t="s">
         <v>120</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>160</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" t="s">
         <v>132</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" t="s">
         <v>146</v>
       </c>
       <c r="N11" t="s">
         <v>121</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11">
         <v>61801</v>
       </c>
       <c r="P11" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2577,30 +2576,30 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C12" t="s">
         <v>120</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
         <v>161</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" t="s">
         <v>133</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" t="s">
         <v>147</v>
       </c>
       <c r="N12" t="s">
         <v>121</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12">
         <v>62568</v>
       </c>
       <c r="P12" t="s">
         <v>29</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2609,30 +2608,30 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C13" t="s">
         <v>120</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" t="s">
         <v>162</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" t="s">
         <v>134</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M13" t="s">
         <v>77</v>
       </c>
       <c r="N13" t="s">
         <v>121</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13">
         <v>62441</v>
       </c>
       <c r="P13" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2641,30 +2640,30 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C14" t="s">
         <v>120</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" t="s">
         <v>163</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" t="s">
         <v>135</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M14" t="s">
         <v>148</v>
       </c>
       <c r="N14" t="s">
         <v>121</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14">
         <v>62858</v>
       </c>
       <c r="P14" t="s">
         <v>31</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2673,30 +2672,30 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C15" t="s">
         <v>120</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" t="s">
         <v>164</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" t="s">
         <v>136</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="M15" t="s">
         <v>149</v>
       </c>
       <c r="N15" t="s">
         <v>121</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15">
         <v>62231</v>
       </c>
       <c r="P15" t="s">
         <v>32</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="Q15" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2705,30 +2704,30 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C16" t="s">
         <v>120</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" t="s">
         <v>165</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" t="s">
         <v>137</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="M16" t="s">
         <v>150</v>
       </c>
       <c r="N16" t="s">
         <v>121</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16">
         <v>61920</v>
       </c>
       <c r="P16" t="s">
         <v>33</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2737,7 +2736,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C17" t="s">
         <v>120</v>
@@ -2745,26 +2744,26 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>593</v>
+      <c r="H17" t="s">
+        <v>573</v>
+      </c>
+      <c r="K17" t="s">
+        <v>588</v>
+      </c>
+      <c r="M17" t="s">
+        <v>591</v>
       </c>
       <c r="N17" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17">
         <v>60602</v>
       </c>
       <c r="P17" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="1" t="s">
-        <v>604</v>
+      <c r="Q17" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2772,7 +2771,7 @@
         <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C18" t="s">
         <v>120</v>
@@ -2780,26 +2779,26 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>594</v>
+      <c r="H18" t="s">
+        <v>574</v>
+      </c>
+      <c r="K18" t="s">
+        <v>582</v>
+      </c>
+      <c r="M18" t="s">
+        <v>592</v>
       </c>
       <c r="N18" t="s">
         <v>121</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18">
         <v>60077</v>
       </c>
       <c r="P18" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" s="1" t="s">
-        <v>599</v>
+      <c r="Q18" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2807,7 +2806,7 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C19" t="s">
         <v>120</v>
@@ -2815,26 +2814,26 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>595</v>
+      <c r="H19" t="s">
+        <v>575</v>
+      </c>
+      <c r="K19" t="s">
+        <v>583</v>
+      </c>
+      <c r="M19" t="s">
+        <v>593</v>
       </c>
       <c r="N19" t="s">
         <v>121</v>
       </c>
-      <c r="O19" s="1">
+      <c r="O19">
         <v>60008</v>
       </c>
       <c r="P19" t="s">
         <v>34</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>600</v>
+      <c r="Q19" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2842,7 +2841,7 @@
         <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C20" t="s">
         <v>120</v>
@@ -2850,26 +2849,26 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>596</v>
+      <c r="H20" t="s">
+        <v>576</v>
+      </c>
+      <c r="K20" t="s">
+        <v>584</v>
+      </c>
+      <c r="M20" t="s">
+        <v>594</v>
       </c>
       <c r="N20" t="s">
         <v>121</v>
       </c>
-      <c r="O20" s="1">
+      <c r="O20">
         <v>60153</v>
       </c>
       <c r="P20" t="s">
         <v>34</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>601</v>
+      <c r="Q20" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2877,7 +2876,7 @@
         <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C21" t="s">
         <v>120</v>
@@ -2885,26 +2884,26 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>597</v>
+      <c r="H21" t="s">
+        <v>577</v>
+      </c>
+      <c r="K21" t="s">
+        <v>585</v>
+      </c>
+      <c r="M21" t="s">
+        <v>595</v>
       </c>
       <c r="N21" t="s">
         <v>121</v>
       </c>
-      <c r="O21" s="1">
+      <c r="O21">
         <v>60455</v>
       </c>
       <c r="P21" t="s">
         <v>34</v>
       </c>
-      <c r="Q21" s="1" t="s">
-        <v>602</v>
+      <c r="Q21" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2912,7 +2911,7 @@
         <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C22" t="s">
         <v>120</v>
@@ -2920,26 +2919,26 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>598</v>
+      <c r="H22" t="s">
+        <v>578</v>
+      </c>
+      <c r="K22" t="s">
+        <v>586</v>
+      </c>
+      <c r="M22" t="s">
+        <v>596</v>
       </c>
       <c r="N22" t="s">
         <v>121</v>
       </c>
-      <c r="O22" s="1">
+      <c r="O22">
         <v>60428</v>
       </c>
       <c r="P22" t="s">
         <v>34</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>603</v>
+      <c r="Q22" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -2947,31 +2946,31 @@
         <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C23" t="s">
         <v>120</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="K23" s="1" t="s">
+      <c r="H23" t="s">
+        <v>579</v>
+      </c>
+      <c r="K23" t="s">
+        <v>589</v>
+      </c>
+      <c r="M23" t="s">
         <v>591</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>593</v>
-      </c>
       <c r="N23" t="s">
         <v>121</v>
       </c>
-      <c r="O23" s="1">
+      <c r="O23">
         <v>60607</v>
       </c>
       <c r="P23" t="s">
         <v>34</v>
       </c>
-      <c r="Q23" s="1" t="s">
-        <v>604</v>
+      <c r="Q23" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -2979,31 +2978,31 @@
         <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C24" t="s">
         <v>120</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>593</v>
+      <c r="H24" t="s">
+        <v>580</v>
+      </c>
+      <c r="K24" t="s">
+        <v>587</v>
+      </c>
+      <c r="M24" t="s">
+        <v>591</v>
       </c>
       <c r="N24" t="s">
         <v>121</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O24">
         <v>60608</v>
       </c>
       <c r="P24" t="s">
         <v>34</v>
       </c>
-      <c r="Q24" s="1" t="s">
-        <v>604</v>
+      <c r="Q24" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -3011,31 +3010,31 @@
         <v>110</v>
       </c>
       <c r="B25" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C25" t="s">
         <v>120</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>593</v>
+      <c r="H25" t="s">
+        <v>581</v>
+      </c>
+      <c r="K25" t="s">
+        <v>590</v>
+      </c>
+      <c r="M25" t="s">
+        <v>591</v>
       </c>
       <c r="N25" t="s">
         <v>121</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O25">
         <v>60612</v>
       </c>
       <c r="P25" t="s">
         <v>34</v>
       </c>
-      <c r="Q25" s="1" t="s">
-        <v>604</v>
+      <c r="Q25" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -3043,31 +3042,31 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C26" t="s">
         <v>120</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="K26" s="1" t="s">
+      <c r="H26" t="s">
+        <v>489</v>
+      </c>
+      <c r="K26" t="s">
         <v>176</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>263</v>
+      <c r="M26" t="s">
+        <v>262</v>
       </c>
       <c r="N26" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O26">
         <v>62454</v>
       </c>
       <c r="P26" t="s">
         <v>35</v>
       </c>
-      <c r="Q26" s="1" t="s">
-        <v>344</v>
+      <c r="Q26" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -3075,30 +3074,30 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C27" t="s">
         <v>120</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="K27" s="1" t="s">
+      <c r="H27" t="s">
+        <v>490</v>
+      </c>
+      <c r="K27" t="s">
         <v>177</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>264</v>
+      <c r="M27" t="s">
+        <v>263</v>
       </c>
       <c r="N27" t="s">
         <v>121</v>
       </c>
-      <c r="O27" s="1">
+      <c r="O27">
         <v>62468</v>
       </c>
       <c r="P27" t="s">
         <v>36</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3107,31 +3106,31 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C28" t="s">
         <v>120</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="K28" s="1" t="s">
+      <c r="H28" t="s">
+        <v>491</v>
+      </c>
+      <c r="K28" t="s">
         <v>178</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>265</v>
+      <c r="M28" t="s">
+        <v>264</v>
       </c>
       <c r="N28" t="s">
         <v>121</v>
       </c>
-      <c r="O28" s="1">
+      <c r="O28">
         <v>60178</v>
       </c>
       <c r="P28" t="s">
         <v>37</v>
       </c>
-      <c r="Q28" s="1" t="s">
-        <v>345</v>
+      <c r="Q28" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -3139,31 +3138,31 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C29" t="s">
         <v>120</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="K29" s="1" t="s">
+      <c r="H29" t="s">
+        <v>492</v>
+      </c>
+      <c r="K29" t="s">
         <v>179</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="M29" t="s">
         <v>32</v>
       </c>
       <c r="N29" t="s">
         <v>121</v>
       </c>
-      <c r="O29" s="1">
+      <c r="O29">
         <v>61727</v>
       </c>
       <c r="P29" t="s">
         <v>38</v>
       </c>
-      <c r="Q29" s="1" t="s">
-        <v>346</v>
+      <c r="Q29" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -3171,31 +3170,31 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C30" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="K30" s="1" t="s">
+      <c r="H30" t="s">
+        <v>493</v>
+      </c>
+      <c r="K30" t="s">
         <v>180</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>266</v>
+      <c r="M30" t="s">
+        <v>265</v>
       </c>
       <c r="N30" t="s">
         <v>121</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O30">
         <v>61953</v>
       </c>
       <c r="P30" t="s">
         <v>39</v>
       </c>
-      <c r="Q30" s="1" t="s">
-        <v>346</v>
+      <c r="Q30" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -3203,31 +3202,31 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C31" t="s">
         <v>120</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="K31" s="1" t="s">
+      <c r="H31" t="s">
+        <v>494</v>
+      </c>
+      <c r="K31" t="s">
         <v>181</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>267</v>
+      <c r="M31" t="s">
+        <v>266</v>
       </c>
       <c r="N31" t="s">
         <v>121</v>
       </c>
-      <c r="O31" s="1">
+      <c r="O31">
         <v>60187</v>
       </c>
       <c r="P31" t="s">
         <v>40</v>
       </c>
-      <c r="Q31" s="1" t="s">
-        <v>347</v>
+      <c r="Q31" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -3235,30 +3234,30 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C32" t="s">
         <v>120</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="K32" s="1" t="s">
+      <c r="H32" t="s">
+        <v>495</v>
+      </c>
+      <c r="K32" t="s">
         <v>182</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>268</v>
+      <c r="M32" t="s">
+        <v>267</v>
       </c>
       <c r="N32" t="s">
         <v>121</v>
       </c>
-      <c r="O32" s="1">
+      <c r="O32">
         <v>61944</v>
       </c>
       <c r="P32" t="s">
         <v>41</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q32" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3267,31 +3266,31 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C33" t="s">
         <v>120</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="K33" s="1" t="s">
+      <c r="H33" t="s">
+        <v>496</v>
+      </c>
+      <c r="K33" t="s">
         <v>183</v>
       </c>
-      <c r="M33" s="1" t="s">
-        <v>269</v>
+      <c r="M33" t="s">
+        <v>268</v>
       </c>
       <c r="N33" t="s">
         <v>121</v>
       </c>
-      <c r="O33" s="1">
+      <c r="O33">
         <v>62806</v>
       </c>
       <c r="P33" t="s">
         <v>42</v>
       </c>
-      <c r="Q33" s="1" t="s">
-        <v>344</v>
+      <c r="Q33" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -3299,30 +3298,30 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C34" t="s">
         <v>120</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="K34" s="1" t="s">
+      <c r="H34" t="s">
+        <v>497</v>
+      </c>
+      <c r="K34" t="s">
         <v>184</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="M34" t="s">
         <v>43</v>
       </c>
       <c r="N34" t="s">
         <v>121</v>
       </c>
-      <c r="O34" s="1">
+      <c r="O34">
         <v>62401</v>
       </c>
       <c r="P34" t="s">
         <v>43</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="Q34" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3331,30 +3330,30 @@
         <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C35" t="s">
         <v>120</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="K35" s="1" t="s">
+      <c r="H35" t="s">
+        <v>498</v>
+      </c>
+      <c r="K35" t="s">
         <v>185</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>270</v>
+      <c r="M35" t="s">
+        <v>269</v>
       </c>
       <c r="N35" t="s">
         <v>121</v>
       </c>
-      <c r="O35" s="1">
+      <c r="O35">
         <v>62471</v>
       </c>
       <c r="P35" t="s">
         <v>44</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="Q35" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3363,31 +3362,31 @@
         <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C36" t="s">
         <v>120</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="K36" s="1" t="s">
+      <c r="H36" t="s">
+        <v>499</v>
+      </c>
+      <c r="K36" t="s">
         <v>186</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>271</v>
+      <c r="M36" t="s">
+        <v>270</v>
       </c>
       <c r="N36" t="s">
         <v>121</v>
       </c>
-      <c r="O36" s="1">
+      <c r="O36">
         <v>60957</v>
       </c>
       <c r="P36" t="s">
         <v>45</v>
       </c>
-      <c r="Q36" s="1" t="s">
-        <v>348</v>
+      <c r="Q36" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -3395,31 +3394,31 @@
         <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C37" t="s">
         <v>120</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="K37" s="1" t="s">
+      <c r="H37" t="s">
+        <v>500</v>
+      </c>
+      <c r="K37" t="s">
         <v>187</v>
       </c>
-      <c r="M37" s="1" t="s">
-        <v>272</v>
+      <c r="M37" t="s">
+        <v>271</v>
       </c>
       <c r="N37" t="s">
         <v>121</v>
       </c>
-      <c r="O37" s="1">
+      <c r="O37">
         <v>62812</v>
       </c>
       <c r="P37" t="s">
         <v>46</v>
       </c>
-      <c r="Q37" s="1" t="s">
-        <v>344</v>
+      <c r="Q37" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -3427,31 +3426,31 @@
         <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C38" t="s">
         <v>120</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="K38" s="1" t="s">
+      <c r="H38" t="s">
+        <v>501</v>
+      </c>
+      <c r="K38" t="s">
         <v>188</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>273</v>
+      <c r="M38" t="s">
+        <v>272</v>
       </c>
       <c r="N38" t="s">
         <v>121</v>
       </c>
-      <c r="O38" s="1">
+      <c r="O38">
         <v>61542</v>
       </c>
       <c r="P38" t="s">
         <v>47</v>
       </c>
-      <c r="Q38" s="1" t="s">
-        <v>349</v>
+      <c r="Q38" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3459,31 +3458,31 @@
         <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C39" t="s">
         <v>120</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="K39" s="1" t="s">
+      <c r="H39" t="s">
+        <v>502</v>
+      </c>
+      <c r="K39" t="s">
         <v>189</v>
       </c>
-      <c r="M39" s="1" t="s">
-        <v>274</v>
+      <c r="M39" t="s">
+        <v>273</v>
       </c>
       <c r="N39" t="s">
         <v>121</v>
       </c>
-      <c r="O39" s="1">
+      <c r="O39">
         <v>62984</v>
       </c>
       <c r="P39" t="s">
         <v>48</v>
       </c>
-      <c r="Q39" s="1" t="s">
-        <v>344</v>
+      <c r="Q39" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -3491,31 +3490,31 @@
         <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C40" t="s">
         <v>120</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="K40" s="1" t="s">
+      <c r="H40" t="s">
+        <v>503</v>
+      </c>
+      <c r="K40" t="s">
         <v>190</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>275</v>
+      <c r="M40" t="s">
+        <v>274</v>
       </c>
       <c r="N40" t="s">
         <v>121</v>
       </c>
-      <c r="O40" s="1">
+      <c r="O40">
         <v>62016</v>
       </c>
       <c r="P40" t="s">
         <v>49</v>
       </c>
-      <c r="Q40" s="1" t="s">
-        <v>350</v>
+      <c r="Q40" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -3523,31 +3522,31 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C41" t="s">
         <v>120</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="K41" s="1" t="s">
+      <c r="H41" t="s">
+        <v>504</v>
+      </c>
+      <c r="K41" t="s">
         <v>191</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>276</v>
+      <c r="M41" t="s">
+        <v>275</v>
       </c>
       <c r="N41" t="s">
         <v>121</v>
       </c>
-      <c r="O41" s="1">
+      <c r="O41">
         <v>60450</v>
       </c>
       <c r="P41" t="s">
         <v>50</v>
       </c>
-      <c r="Q41" s="1" t="s">
-        <v>351</v>
+      <c r="Q41" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -3555,31 +3554,31 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C42" t="s">
         <v>120</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="K42" s="1" t="s">
+      <c r="H42" t="s">
+        <v>505</v>
+      </c>
+      <c r="K42" t="s">
         <v>192</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>277</v>
+      <c r="M42" t="s">
+        <v>276</v>
       </c>
       <c r="N42" t="s">
         <v>121</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O42">
         <v>62859</v>
       </c>
       <c r="P42" t="s">
         <v>51</v>
       </c>
-      <c r="Q42" s="1" t="s">
-        <v>344</v>
+      <c r="Q42" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -3587,31 +3586,31 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C43" t="s">
         <v>120</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="K43" s="1" t="s">
+      <c r="H43" t="s">
+        <v>506</v>
+      </c>
+      <c r="K43" t="s">
         <v>193</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>278</v>
+      <c r="M43" t="s">
+        <v>277</v>
       </c>
       <c r="N43" t="s">
         <v>121</v>
       </c>
-      <c r="O43" s="1">
+      <c r="O43">
         <v>62321</v>
       </c>
       <c r="P43" t="s">
         <v>52</v>
       </c>
-      <c r="Q43" s="1" t="s">
-        <v>352</v>
+      <c r="Q43" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -3619,31 +3618,31 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C44" t="s">
         <v>120</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="K44" s="1" t="s">
+      <c r="H44" t="s">
+        <v>507</v>
+      </c>
+      <c r="K44" t="s">
         <v>194</v>
       </c>
-      <c r="M44" s="1" t="s">
-        <v>279</v>
+      <c r="M44" t="s">
+        <v>278</v>
       </c>
       <c r="N44" t="s">
         <v>121</v>
       </c>
-      <c r="O44" s="1">
+      <c r="O44">
         <v>62931</v>
       </c>
       <c r="P44" t="s">
         <v>53</v>
       </c>
-      <c r="Q44" s="1" t="s">
-        <v>344</v>
+      <c r="Q44" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -3651,31 +3650,31 @@
         <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C45" t="s">
         <v>120</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="K45" s="1" t="s">
+      <c r="H45" t="s">
+        <v>508</v>
+      </c>
+      <c r="K45" t="s">
         <v>195</v>
       </c>
-      <c r="M45" s="1" t="s">
-        <v>280</v>
+      <c r="M45" t="s">
+        <v>279</v>
       </c>
       <c r="N45" t="s">
         <v>121</v>
       </c>
-      <c r="O45" s="1">
+      <c r="O45">
         <v>61469</v>
       </c>
       <c r="P45" t="s">
         <v>54</v>
       </c>
-      <c r="Q45" s="1" t="s">
-        <v>353</v>
+      <c r="Q45" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -3683,31 +3682,31 @@
         <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C46" t="s">
         <v>120</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="K46" s="1" t="s">
+      <c r="H46" t="s">
+        <v>509</v>
+      </c>
+      <c r="K46" t="s">
         <v>196</v>
       </c>
-      <c r="M46" s="1" t="s">
-        <v>281</v>
+      <c r="M46" t="s">
+        <v>280</v>
       </c>
       <c r="N46" t="s">
         <v>121</v>
       </c>
-      <c r="O46" s="1">
+      <c r="O46">
         <v>61238</v>
       </c>
       <c r="P46" t="s">
         <v>55</v>
       </c>
-      <c r="Q46" s="1" t="s">
-        <v>354</v>
+      <c r="Q46" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -3715,31 +3714,31 @@
         <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C47" t="s">
         <v>120</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="K47" s="1" t="s">
+      <c r="H47" t="s">
+        <v>510</v>
+      </c>
+      <c r="K47" t="s">
         <v>197</v>
       </c>
-      <c r="M47" s="1" t="s">
-        <v>282</v>
+      <c r="M47" t="s">
+        <v>281</v>
       </c>
       <c r="N47" t="s">
         <v>121</v>
       </c>
-      <c r="O47" s="1">
+      <c r="O47">
         <v>60970</v>
       </c>
       <c r="P47" t="s">
         <v>56</v>
       </c>
-      <c r="Q47" s="1" t="s">
-        <v>355</v>
+      <c r="Q47" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -3747,30 +3746,30 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C48" t="s">
         <v>120</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="K48" s="1" t="s">
+      <c r="H48" t="s">
+        <v>511</v>
+      </c>
+      <c r="K48" t="s">
         <v>198</v>
       </c>
-      <c r="M48" s="1" t="s">
-        <v>283</v>
+      <c r="M48" t="s">
+        <v>282</v>
       </c>
       <c r="N48" t="s">
         <v>121</v>
       </c>
-      <c r="O48" s="1">
+      <c r="O48">
         <v>62966</v>
       </c>
       <c r="P48" t="s">
         <v>57</v>
       </c>
-      <c r="Q48" s="1" t="s">
+      <c r="Q48" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3779,30 +3778,30 @@
         <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C49" t="s">
         <v>120</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="K49" s="1" t="s">
+      <c r="H49" t="s">
+        <v>512</v>
+      </c>
+      <c r="K49" t="s">
         <v>199</v>
       </c>
-      <c r="M49" s="1" t="s">
-        <v>284</v>
+      <c r="M49" t="s">
+        <v>283</v>
       </c>
       <c r="N49" t="s">
         <v>121</v>
       </c>
-      <c r="O49" s="1">
+      <c r="O49">
         <v>62448</v>
       </c>
       <c r="P49" t="s">
         <v>58</v>
       </c>
-      <c r="Q49" s="1" t="s">
+      <c r="Q49" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3811,31 +3810,31 @@
         <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C50" t="s">
         <v>120</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="K50" s="1" t="s">
+      <c r="H50" t="s">
+        <v>513</v>
+      </c>
+      <c r="K50" t="s">
         <v>200</v>
       </c>
-      <c r="M50" s="1" t="s">
-        <v>285</v>
+      <c r="M50" t="s">
+        <v>284</v>
       </c>
       <c r="N50" t="s">
         <v>121</v>
       </c>
-      <c r="O50" s="1">
+      <c r="O50">
         <v>62864</v>
       </c>
       <c r="P50" t="s">
         <v>59</v>
       </c>
-      <c r="Q50" s="1" t="s">
-        <v>344</v>
+      <c r="Q50" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -3843,31 +3842,31 @@
         <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C51" t="s">
         <v>120</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="K51" s="1" t="s">
+      <c r="H51" t="s">
+        <v>514</v>
+      </c>
+      <c r="K51" t="s">
         <v>201</v>
       </c>
-      <c r="M51" s="1" t="s">
-        <v>286</v>
+      <c r="M51" t="s">
+        <v>285</v>
       </c>
       <c r="N51" t="s">
         <v>121</v>
       </c>
-      <c r="O51" s="1">
+      <c r="O51">
         <v>62052</v>
       </c>
       <c r="P51" t="s">
         <v>60</v>
       </c>
-      <c r="Q51" s="1" t="s">
-        <v>350</v>
+      <c r="Q51" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -3875,30 +3874,30 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C52" t="s">
         <v>120</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="K52" s="1" t="s">
+      <c r="H52" t="s">
+        <v>515</v>
+      </c>
+      <c r="K52" t="s">
         <v>202</v>
       </c>
-      <c r="M52" s="1" t="s">
-        <v>287</v>
+      <c r="M52" t="s">
+        <v>286</v>
       </c>
       <c r="N52" t="s">
         <v>121</v>
       </c>
-      <c r="O52" s="1">
+      <c r="O52">
         <v>61036</v>
       </c>
       <c r="P52" t="s">
         <v>61</v>
       </c>
-      <c r="Q52" s="1" t="s">
+      <c r="Q52" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3907,30 +3906,30 @@
         <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C53" t="s">
         <v>120</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="K53" s="1" t="s">
+      <c r="H53" t="s">
+        <v>516</v>
+      </c>
+      <c r="K53" t="s">
         <v>203</v>
       </c>
-      <c r="M53" s="1" t="s">
-        <v>288</v>
+      <c r="M53" t="s">
+        <v>287</v>
       </c>
       <c r="N53" t="s">
         <v>121</v>
       </c>
-      <c r="O53" s="1">
+      <c r="O53">
         <v>62995</v>
       </c>
       <c r="P53" t="s">
         <v>62</v>
       </c>
-      <c r="Q53" s="1" t="s">
+      <c r="Q53" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3939,31 +3938,31 @@
         <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C54" t="s">
         <v>120</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>289</v>
+      <c r="H54" t="s">
+        <v>517</v>
+      </c>
+      <c r="K54" t="s">
+        <v>604</v>
+      </c>
+      <c r="M54" t="s">
+        <v>605</v>
       </c>
       <c r="N54" t="s">
         <v>121</v>
       </c>
-      <c r="O54" s="1">
-        <v>60174</v>
+      <c r="O54">
+        <v>60134</v>
       </c>
       <c r="P54" t="s">
         <v>63</v>
       </c>
-      <c r="Q54" s="1" t="s">
-        <v>356</v>
+      <c r="Q54" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -3971,31 +3970,31 @@
         <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C55" t="s">
         <v>120</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="M55" s="1" t="s">
+      <c r="H55" t="s">
+        <v>518</v>
+      </c>
+      <c r="K55" t="s">
+        <v>204</v>
+      </c>
+      <c r="M55" t="s">
         <v>64</v>
       </c>
       <c r="N55" t="s">
         <v>121</v>
       </c>
-      <c r="O55" s="1">
+      <c r="O55">
         <v>60901</v>
       </c>
       <c r="P55" t="s">
         <v>64</v>
       </c>
-      <c r="Q55" s="1" t="s">
-        <v>355</v>
+      <c r="Q55" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -4003,31 +4002,31 @@
         <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C56" t="s">
         <v>120</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>290</v>
+      <c r="H56" t="s">
+        <v>519</v>
+      </c>
+      <c r="K56" t="s">
+        <v>205</v>
+      </c>
+      <c r="M56" t="s">
+        <v>288</v>
       </c>
       <c r="N56" t="s">
         <v>121</v>
       </c>
-      <c r="O56" s="1">
+      <c r="O56">
         <v>60543</v>
       </c>
       <c r="P56" t="s">
         <v>65</v>
       </c>
-      <c r="Q56" s="1" t="s">
-        <v>357</v>
+      <c r="Q56" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -4035,31 +4034,31 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C57" t="s">
         <v>120</v>
       </c>
-      <c r="H57" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>291</v>
+      <c r="H57" t="s">
+        <v>520</v>
+      </c>
+      <c r="K57" t="s">
+        <v>206</v>
+      </c>
+      <c r="M57" t="s">
+        <v>289</v>
       </c>
       <c r="N57" t="s">
         <v>121</v>
       </c>
-      <c r="O57" s="1">
+      <c r="O57">
         <v>61401</v>
       </c>
       <c r="P57" t="s">
         <v>66</v>
       </c>
-      <c r="Q57" s="1" t="s">
-        <v>358</v>
+      <c r="Q57" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -4067,31 +4066,31 @@
         <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C58" t="s">
         <v>120</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>292</v>
+      <c r="H58" t="s">
+        <v>521</v>
+      </c>
+      <c r="K58" t="s">
+        <v>207</v>
+      </c>
+      <c r="M58" t="s">
+        <v>290</v>
       </c>
       <c r="N58" t="s">
         <v>121</v>
       </c>
-      <c r="O58" s="1">
+      <c r="O58">
         <v>60085</v>
       </c>
       <c r="P58" t="s">
         <v>67</v>
       </c>
-      <c r="Q58" s="1" t="s">
-        <v>359</v>
+      <c r="Q58" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -4099,24 +4098,24 @@
         <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C59" t="s">
         <v>120</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="M59" s="1" t="s">
-        <v>293</v>
+      <c r="H59" t="s">
+        <v>522</v>
+      </c>
+      <c r="K59" t="s">
+        <v>208</v>
+      </c>
+      <c r="M59" t="s">
+        <v>291</v>
       </c>
       <c r="N59" t="s">
         <v>121</v>
       </c>
-      <c r="O59" s="1">
+      <c r="O59">
         <v>61350</v>
       </c>
       <c r="P59" t="s">
@@ -4128,31 +4127,31 @@
         <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C60" t="s">
         <v>120</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>294</v>
+      <c r="H60" t="s">
+        <v>523</v>
+      </c>
+      <c r="K60" t="s">
+        <v>209</v>
+      </c>
+      <c r="M60" t="s">
+        <v>292</v>
       </c>
       <c r="N60" t="s">
         <v>121</v>
       </c>
-      <c r="O60" s="1">
+      <c r="O60">
         <v>62439</v>
       </c>
       <c r="P60" t="s">
         <v>69</v>
       </c>
-      <c r="Q60" s="1" t="s">
-        <v>344</v>
+      <c r="Q60" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -4160,31 +4159,31 @@
         <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C61" t="s">
         <v>120</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>295</v>
+      <c r="H61" t="s">
+        <v>524</v>
+      </c>
+      <c r="K61" t="s">
+        <v>210</v>
+      </c>
+      <c r="M61" t="s">
+        <v>293</v>
       </c>
       <c r="N61" t="s">
         <v>121</v>
       </c>
-      <c r="O61" s="1">
+      <c r="O61">
         <v>61021</v>
       </c>
       <c r="P61" t="s">
         <v>70</v>
       </c>
-      <c r="Q61" s="1" t="s">
-        <v>360</v>
+      <c r="Q61" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -4192,31 +4191,31 @@
         <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C62" t="s">
         <v>120</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>296</v>
+      <c r="H62" t="s">
+        <v>525</v>
+      </c>
+      <c r="K62" t="s">
+        <v>211</v>
+      </c>
+      <c r="M62" t="s">
+        <v>294</v>
       </c>
       <c r="N62" t="s">
         <v>121</v>
       </c>
-      <c r="O62" s="1">
+      <c r="O62">
         <v>61764</v>
       </c>
       <c r="P62" t="s">
         <v>71</v>
       </c>
-      <c r="Q62" s="1" t="s">
-        <v>361</v>
+      <c r="Q62" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -4224,31 +4223,31 @@
         <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C63" t="s">
         <v>120</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M63" s="1" t="s">
-        <v>297</v>
+      <c r="H63" t="s">
+        <v>526</v>
+      </c>
+      <c r="K63" t="s">
+        <v>212</v>
+      </c>
+      <c r="M63" t="s">
+        <v>295</v>
       </c>
       <c r="N63" t="s">
         <v>121</v>
       </c>
-      <c r="O63" s="1">
+      <c r="O63">
         <v>62656</v>
       </c>
       <c r="P63" t="s">
         <v>72</v>
       </c>
-      <c r="Q63" s="1" t="s">
-        <v>348</v>
+      <c r="Q63" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -4256,31 +4255,31 @@
         <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C64" t="s">
         <v>120</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M64" s="1" t="s">
-        <v>298</v>
+      <c r="H64" t="s">
+        <v>527</v>
+      </c>
+      <c r="K64" t="s">
+        <v>213</v>
+      </c>
+      <c r="M64" t="s">
+        <v>296</v>
       </c>
       <c r="N64" t="s">
         <v>121</v>
       </c>
-      <c r="O64" s="1">
+      <c r="O64">
         <v>62523</v>
       </c>
       <c r="P64" t="s">
         <v>73</v>
       </c>
-      <c r="Q64" s="1" t="s">
-        <v>346</v>
+      <c r="Q64" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -4288,31 +4287,31 @@
         <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C65" t="s">
         <v>120</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="K65" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="M65" s="1" t="s">
-        <v>299</v>
+      <c r="H65" t="s">
+        <v>528</v>
+      </c>
+      <c r="K65" t="s">
+        <v>214</v>
+      </c>
+      <c r="M65" t="s">
+        <v>297</v>
       </c>
       <c r="N65" t="s">
         <v>121</v>
       </c>
-      <c r="O65" s="1">
+      <c r="O65">
         <v>62626</v>
       </c>
       <c r="P65" t="s">
         <v>74</v>
       </c>
-      <c r="Q65" s="1" t="s">
-        <v>350</v>
+      <c r="Q65" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -4320,31 +4319,31 @@
         <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C66" t="s">
         <v>120</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="M66" s="1" t="s">
-        <v>300</v>
+      <c r="H66" t="s">
+        <v>529</v>
+      </c>
+      <c r="K66" t="s">
+        <v>215</v>
+      </c>
+      <c r="M66" t="s">
+        <v>298</v>
       </c>
       <c r="N66" t="s">
         <v>121</v>
       </c>
-      <c r="O66" s="1">
+      <c r="O66">
         <v>62025</v>
       </c>
       <c r="P66" t="s">
         <v>75</v>
       </c>
-      <c r="Q66" s="1" t="s">
-        <v>362</v>
+      <c r="Q66" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -4352,30 +4351,30 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C67" t="s">
         <v>120</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="K67" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="M67" s="1" t="s">
-        <v>301</v>
+      <c r="H67" t="s">
+        <v>530</v>
+      </c>
+      <c r="K67" t="s">
+        <v>216</v>
+      </c>
+      <c r="M67" t="s">
+        <v>299</v>
       </c>
       <c r="N67" t="s">
         <v>121</v>
       </c>
-      <c r="O67" s="1">
+      <c r="O67">
         <v>62881</v>
       </c>
       <c r="P67" t="s">
         <v>76</v>
       </c>
-      <c r="Q67" s="1" t="s">
+      <c r="Q67" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4384,31 +4383,31 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C68" t="s">
         <v>120</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="K68" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>302</v>
+      <c r="H68" t="s">
+        <v>531</v>
+      </c>
+      <c r="K68" t="s">
+        <v>217</v>
+      </c>
+      <c r="M68" t="s">
+        <v>300</v>
       </c>
       <c r="N68" t="s">
         <v>121</v>
       </c>
-      <c r="O68" s="1">
+      <c r="O68">
         <v>61540</v>
       </c>
       <c r="P68" t="s">
         <v>77</v>
       </c>
-      <c r="Q68" s="1" t="s">
-        <v>363</v>
+      <c r="Q68" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -4416,30 +4415,30 @@
         <v>60</v>
       </c>
       <c r="B69" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C69" t="s">
         <v>120</v>
       </c>
-      <c r="H69" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="K69" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="M69" s="1" t="s">
-        <v>303</v>
+      <c r="H69" t="s">
+        <v>532</v>
+      </c>
+      <c r="K69" t="s">
+        <v>218</v>
+      </c>
+      <c r="M69" t="s">
+        <v>301</v>
       </c>
       <c r="N69" t="s">
         <v>121</v>
       </c>
-      <c r="O69" s="1">
+      <c r="O69">
         <v>62644</v>
       </c>
       <c r="P69" t="s">
         <v>78</v>
       </c>
-      <c r="Q69" s="1" t="s">
+      <c r="Q69" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4448,30 +4447,30 @@
         <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C70" t="s">
         <v>120</v>
       </c>
-      <c r="H70" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="K70" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="M70" s="1" t="s">
-        <v>304</v>
+      <c r="H70" t="s">
+        <v>533</v>
+      </c>
+      <c r="K70" t="s">
+        <v>219</v>
+      </c>
+      <c r="M70" t="s">
+        <v>302</v>
       </c>
       <c r="N70" t="s">
         <v>121</v>
       </c>
-      <c r="O70" s="1">
+      <c r="O70">
         <v>62960</v>
       </c>
       <c r="P70" t="s">
         <v>79</v>
       </c>
-      <c r="Q70" s="1" t="s">
+      <c r="Q70" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4480,31 +4479,31 @@
         <v>62</v>
       </c>
       <c r="B71" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C71" t="s">
         <v>120</v>
       </c>
-      <c r="H71" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="K71" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M71" s="1" t="s">
-        <v>305</v>
+      <c r="H71" t="s">
+        <v>534</v>
+      </c>
+      <c r="K71" t="s">
+        <v>220</v>
+      </c>
+      <c r="M71" t="s">
+        <v>303</v>
       </c>
       <c r="N71" t="s">
         <v>121</v>
       </c>
-      <c r="O71" s="1">
+      <c r="O71">
         <v>61455</v>
       </c>
       <c r="P71" t="s">
         <v>80</v>
       </c>
-      <c r="Q71" s="1" t="s">
-        <v>364</v>
+      <c r="Q71" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -4512,31 +4511,31 @@
         <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C72" t="s">
         <v>120</v>
       </c>
-      <c r="H72" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="K72" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="M72" s="1" t="s">
-        <v>306</v>
+      <c r="H72" t="s">
+        <v>535</v>
+      </c>
+      <c r="K72" t="s">
+        <v>221</v>
+      </c>
+      <c r="M72" t="s">
+        <v>304</v>
       </c>
       <c r="N72" t="s">
         <v>121</v>
       </c>
-      <c r="O72" s="1">
+      <c r="O72">
         <v>60098</v>
       </c>
       <c r="P72" t="s">
         <v>81</v>
       </c>
-      <c r="Q72" s="1" t="s">
-        <v>365</v>
+      <c r="Q72" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -4544,31 +4543,31 @@
         <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C73" t="s">
         <v>120</v>
       </c>
-      <c r="H73" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="K73" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="M73" s="1" t="s">
-        <v>307</v>
+      <c r="H73" t="s">
+        <v>536</v>
+      </c>
+      <c r="K73" t="s">
+        <v>222</v>
+      </c>
+      <c r="M73" t="s">
+        <v>305</v>
       </c>
       <c r="N73" t="s">
         <v>121</v>
       </c>
-      <c r="O73" s="1">
+      <c r="O73">
         <v>61701</v>
       </c>
       <c r="P73" t="s">
         <v>82</v>
       </c>
-      <c r="Q73" s="1" t="s">
-        <v>366</v>
+      <c r="Q73" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -4576,31 +4575,31 @@
         <v>65</v>
       </c>
       <c r="B74" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C74" t="s">
         <v>120</v>
       </c>
-      <c r="H74" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="M74" s="1" t="s">
-        <v>308</v>
+      <c r="H74" t="s">
+        <v>537</v>
+      </c>
+      <c r="K74" t="s">
+        <v>223</v>
+      </c>
+      <c r="M74" t="s">
+        <v>306</v>
       </c>
       <c r="N74" t="s">
         <v>121</v>
       </c>
-      <c r="O74" s="1">
+      <c r="O74">
         <v>62675</v>
       </c>
       <c r="P74" t="s">
         <v>83</v>
       </c>
-      <c r="Q74" s="1" t="s">
-        <v>367</v>
+      <c r="Q74" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
@@ -4608,31 +4607,31 @@
         <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C75" t="s">
         <v>120</v>
       </c>
-      <c r="H75" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="K75" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="M75" s="1" t="s">
-        <v>309</v>
+      <c r="H75" t="s">
+        <v>538</v>
+      </c>
+      <c r="K75" t="s">
+        <v>224</v>
+      </c>
+      <c r="M75" t="s">
+        <v>307</v>
       </c>
       <c r="N75" t="s">
         <v>121</v>
       </c>
-      <c r="O75" s="1">
+      <c r="O75">
         <v>61231</v>
       </c>
       <c r="P75" t="s">
         <v>84</v>
       </c>
-      <c r="Q75" s="1" t="s">
-        <v>368</v>
+      <c r="Q75" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
@@ -4640,24 +4639,24 @@
         <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C76" t="s">
         <v>120</v>
       </c>
-      <c r="H76" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="M76" s="1" t="s">
-        <v>310</v>
+      <c r="H76" t="s">
+        <v>539</v>
+      </c>
+      <c r="K76" t="s">
+        <v>225</v>
+      </c>
+      <c r="M76" t="s">
+        <v>308</v>
       </c>
       <c r="N76" t="s">
         <v>121</v>
       </c>
-      <c r="O76" s="1">
+      <c r="O76">
         <v>62298</v>
       </c>
       <c r="P76" t="s">
@@ -4669,30 +4668,30 @@
         <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C77" t="s">
         <v>120</v>
       </c>
-      <c r="H77" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="M77" s="1" t="s">
-        <v>311</v>
+      <c r="H77" t="s">
+        <v>540</v>
+      </c>
+      <c r="K77" t="s">
+        <v>226</v>
+      </c>
+      <c r="M77" t="s">
+        <v>309</v>
       </c>
       <c r="N77" t="s">
         <v>121</v>
       </c>
-      <c r="O77" s="1">
+      <c r="O77">
         <v>62049</v>
       </c>
       <c r="P77" t="s">
         <v>86</v>
       </c>
-      <c r="Q77" s="1" t="s">
+      <c r="Q77" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4701,31 +4700,31 @@
         <v>69</v>
       </c>
       <c r="B78" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C78" t="s">
         <v>120</v>
       </c>
-      <c r="H78" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="K78" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="M78" s="1" t="s">
-        <v>312</v>
+      <c r="H78" t="s">
+        <v>541</v>
+      </c>
+      <c r="K78" t="s">
+        <v>227</v>
+      </c>
+      <c r="M78" t="s">
+        <v>310</v>
       </c>
       <c r="N78" t="s">
         <v>121</v>
       </c>
-      <c r="O78" s="1">
+      <c r="O78">
         <v>62650</v>
       </c>
       <c r="P78" t="s">
         <v>87</v>
       </c>
-      <c r="Q78" s="1" t="s">
-        <v>350</v>
+      <c r="Q78" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -4733,31 +4732,31 @@
         <v>70</v>
       </c>
       <c r="B79" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C79" t="s">
         <v>120</v>
       </c>
-      <c r="H79" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="K79" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M79" s="1" t="s">
-        <v>313</v>
+      <c r="H79" t="s">
+        <v>542</v>
+      </c>
+      <c r="K79" t="s">
+        <v>228</v>
+      </c>
+      <c r="M79" t="s">
+        <v>311</v>
       </c>
       <c r="N79" t="s">
         <v>121</v>
       </c>
-      <c r="O79" s="1">
+      <c r="O79">
         <v>61951</v>
       </c>
       <c r="P79" t="s">
         <v>88</v>
       </c>
-      <c r="Q79" s="1" t="s">
-        <v>346</v>
+      <c r="Q79" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -4765,31 +4764,31 @@
         <v>71</v>
       </c>
       <c r="B80" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C80" t="s">
         <v>120</v>
       </c>
-      <c r="H80" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="M80" s="1" t="s">
-        <v>314</v>
+      <c r="H80" t="s">
+        <v>543</v>
+      </c>
+      <c r="K80" t="s">
+        <v>229</v>
+      </c>
+      <c r="M80" t="s">
+        <v>312</v>
       </c>
       <c r="N80" t="s">
         <v>121</v>
       </c>
-      <c r="O80" s="1">
+      <c r="O80">
         <v>61061</v>
       </c>
       <c r="P80" t="s">
         <v>89</v>
       </c>
-      <c r="Q80" s="1" t="s">
-        <v>360</v>
+      <c r="Q80" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
@@ -4797,31 +4796,31 @@
         <v>72</v>
       </c>
       <c r="B81" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C81" t="s">
         <v>120</v>
       </c>
-      <c r="H81" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="M81" s="1" t="s">
+      <c r="H81" t="s">
+        <v>544</v>
+      </c>
+      <c r="K81" t="s">
+        <v>230</v>
+      </c>
+      <c r="M81" t="s">
         <v>90</v>
       </c>
       <c r="N81" t="s">
         <v>121</v>
       </c>
-      <c r="O81" s="1">
+      <c r="O81">
         <v>61602</v>
       </c>
       <c r="P81" t="s">
         <v>90</v>
       </c>
-      <c r="Q81" s="1" t="s">
-        <v>363</v>
+      <c r="Q81" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
@@ -4829,24 +4828,24 @@
         <v>73</v>
       </c>
       <c r="B82" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C82" t="s">
         <v>120</v>
       </c>
-      <c r="H82" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="K82" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="M82" s="1" t="s">
-        <v>315</v>
+      <c r="H82" t="s">
+        <v>545</v>
+      </c>
+      <c r="K82" t="s">
+        <v>231</v>
+      </c>
+      <c r="M82" t="s">
+        <v>313</v>
       </c>
       <c r="N82" t="s">
         <v>121</v>
       </c>
-      <c r="O82" s="1">
+      <c r="O82">
         <v>62274</v>
       </c>
       <c r="P82" t="s">
@@ -4858,31 +4857,31 @@
         <v>74</v>
       </c>
       <c r="B83" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C83" t="s">
         <v>120</v>
       </c>
-      <c r="H83" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="K83" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="M83" s="1" t="s">
-        <v>316</v>
+      <c r="H83" t="s">
+        <v>546</v>
+      </c>
+      <c r="K83" t="s">
+        <v>232</v>
+      </c>
+      <c r="M83" t="s">
+        <v>314</v>
       </c>
       <c r="N83" t="s">
         <v>121</v>
       </c>
-      <c r="O83" s="1">
+      <c r="O83">
         <v>61856</v>
       </c>
       <c r="P83" t="s">
         <v>92</v>
       </c>
-      <c r="Q83" s="1" t="s">
-        <v>346</v>
+      <c r="Q83" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
@@ -4890,31 +4889,31 @@
         <v>75</v>
       </c>
       <c r="B84" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C84" t="s">
         <v>120</v>
       </c>
-      <c r="H84" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="K84" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M84" s="1" t="s">
-        <v>317</v>
+      <c r="H84" t="s">
+        <v>547</v>
+      </c>
+      <c r="K84" t="s">
+        <v>233</v>
+      </c>
+      <c r="M84" t="s">
+        <v>315</v>
       </c>
       <c r="N84" t="s">
         <v>121</v>
       </c>
-      <c r="O84" s="1">
+      <c r="O84">
         <v>62363</v>
       </c>
       <c r="P84" t="s">
         <v>93</v>
       </c>
-      <c r="Q84" s="1" t="s">
-        <v>369</v>
+      <c r="Q84" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
@@ -4922,30 +4921,30 @@
         <v>76</v>
       </c>
       <c r="B85" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C85" t="s">
         <v>120</v>
       </c>
-      <c r="H85" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="K85" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="M85" s="1" t="s">
-        <v>318</v>
+      <c r="H85" t="s">
+        <v>548</v>
+      </c>
+      <c r="K85" t="s">
+        <v>234</v>
+      </c>
+      <c r="M85" t="s">
+        <v>316</v>
       </c>
       <c r="N85" t="s">
         <v>121</v>
       </c>
-      <c r="O85" s="1">
+      <c r="O85">
         <v>62938</v>
       </c>
       <c r="P85" t="s">
         <v>94</v>
       </c>
-      <c r="Q85" s="1" t="s">
+      <c r="Q85" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4954,30 +4953,30 @@
         <v>77</v>
       </c>
       <c r="B86" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C86" t="s">
         <v>120</v>
       </c>
-      <c r="H86" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="K86" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="M86" s="1" t="s">
-        <v>319</v>
+      <c r="H86" t="s">
+        <v>549</v>
+      </c>
+      <c r="K86" t="s">
+        <v>235</v>
+      </c>
+      <c r="M86" t="s">
+        <v>317</v>
       </c>
       <c r="N86" t="s">
         <v>121</v>
       </c>
-      <c r="O86" s="1">
+      <c r="O86">
         <v>62963</v>
       </c>
       <c r="P86" t="s">
         <v>95</v>
       </c>
-      <c r="Q86" s="1" t="s">
+      <c r="Q86" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4986,31 +4985,31 @@
         <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C87" t="s">
         <v>120</v>
       </c>
-      <c r="H87" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="K87" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>320</v>
+      <c r="H87" t="s">
+        <v>550</v>
+      </c>
+      <c r="K87" t="s">
+        <v>236</v>
+      </c>
+      <c r="M87" t="s">
+        <v>318</v>
       </c>
       <c r="N87" t="s">
         <v>121</v>
       </c>
-      <c r="O87" s="1">
+      <c r="O87">
         <v>61327</v>
       </c>
       <c r="P87" t="s">
         <v>96</v>
       </c>
-      <c r="Q87" s="1" t="s">
-        <v>370</v>
+      <c r="Q87" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
@@ -5018,31 +5017,31 @@
         <v>79</v>
       </c>
       <c r="B88" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C88" t="s">
         <v>120</v>
       </c>
-      <c r="H88" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="K88" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="M88" s="1" t="s">
-        <v>321</v>
+      <c r="H88" t="s">
+        <v>551</v>
+      </c>
+      <c r="K88" t="s">
+        <v>237</v>
+      </c>
+      <c r="M88" t="s">
+        <v>319</v>
       </c>
       <c r="N88" t="s">
         <v>121</v>
       </c>
-      <c r="O88" s="1">
+      <c r="O88">
         <v>62233</v>
       </c>
       <c r="P88" t="s">
         <v>97</v>
       </c>
-      <c r="Q88" s="1" t="s">
-        <v>371</v>
+      <c r="Q88" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
@@ -5050,31 +5049,31 @@
         <v>80</v>
       </c>
       <c r="B89" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C89" t="s">
         <v>120</v>
       </c>
-      <c r="H89" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="K89" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="M89" s="1" t="s">
-        <v>322</v>
+      <c r="H89" t="s">
+        <v>552</v>
+      </c>
+      <c r="K89" t="s">
+        <v>238</v>
+      </c>
+      <c r="M89" t="s">
+        <v>320</v>
       </c>
       <c r="N89" t="s">
         <v>121</v>
       </c>
-      <c r="O89" s="1">
+      <c r="O89">
         <v>62450</v>
       </c>
       <c r="P89" t="s">
         <v>98</v>
       </c>
-      <c r="Q89" s="1" t="s">
-        <v>344</v>
+      <c r="Q89" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
@@ -5082,31 +5081,31 @@
         <v>81</v>
       </c>
       <c r="B90" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C90" t="s">
         <v>120</v>
       </c>
-      <c r="H90" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="K90" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M90" s="1" t="s">
+      <c r="H90" t="s">
+        <v>553</v>
+      </c>
+      <c r="K90" t="s">
+        <v>239</v>
+      </c>
+      <c r="M90" t="s">
         <v>99</v>
       </c>
       <c r="N90" t="s">
         <v>121</v>
       </c>
-      <c r="O90" s="1">
+      <c r="O90">
         <v>61201</v>
       </c>
       <c r="P90" t="s">
         <v>99</v>
       </c>
-      <c r="Q90" s="1" t="s">
-        <v>372</v>
+      <c r="Q90" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
@@ -5114,30 +5113,30 @@
         <v>82</v>
       </c>
       <c r="B91" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C91" t="s">
         <v>120</v>
       </c>
-      <c r="H91" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="K91" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="M91" s="1" t="s">
-        <v>323</v>
+      <c r="H91" t="s">
+        <v>554</v>
+      </c>
+      <c r="K91" t="s">
+        <v>240</v>
+      </c>
+      <c r="M91" t="s">
+        <v>321</v>
       </c>
       <c r="N91" t="s">
         <v>121</v>
       </c>
-      <c r="O91" s="1">
+      <c r="O91">
         <v>62946</v>
       </c>
       <c r="P91" t="s">
         <v>100</v>
       </c>
-      <c r="Q91" s="1" t="s">
+      <c r="Q91" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5146,31 +5145,31 @@
         <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C92" t="s">
         <v>120</v>
       </c>
-      <c r="H92" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="K92" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M92" s="1" t="s">
-        <v>324</v>
+      <c r="H92" t="s">
+        <v>555</v>
+      </c>
+      <c r="K92" t="s">
+        <v>241</v>
+      </c>
+      <c r="M92" t="s">
+        <v>322</v>
       </c>
       <c r="N92" t="s">
         <v>121</v>
       </c>
-      <c r="O92" s="1">
+      <c r="O92">
         <v>62701</v>
       </c>
       <c r="P92" t="s">
         <v>101</v>
       </c>
-      <c r="Q92" s="1" t="s">
-        <v>373</v>
+      <c r="Q92" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
@@ -5178,30 +5177,30 @@
         <v>84</v>
       </c>
       <c r="B93" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C93" t="s">
         <v>120</v>
       </c>
-      <c r="H93" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="K93" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M93" s="1" t="s">
-        <v>325</v>
+      <c r="H93" t="s">
+        <v>556</v>
+      </c>
+      <c r="K93" t="s">
+        <v>242</v>
+      </c>
+      <c r="M93" t="s">
+        <v>323</v>
       </c>
       <c r="N93" t="s">
         <v>121</v>
       </c>
-      <c r="O93" s="1">
+      <c r="O93">
         <v>62681</v>
       </c>
       <c r="P93" t="s">
         <v>102</v>
       </c>
-      <c r="Q93" s="1" t="s">
+      <c r="Q93" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5210,31 +5209,31 @@
         <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C94" t="s">
         <v>120</v>
       </c>
-      <c r="H94" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="K94" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M94" s="1" t="s">
-        <v>326</v>
+      <c r="H94" t="s">
+        <v>557</v>
+      </c>
+      <c r="K94" t="s">
+        <v>243</v>
+      </c>
+      <c r="M94" t="s">
+        <v>324</v>
       </c>
       <c r="N94" t="s">
         <v>121</v>
       </c>
-      <c r="O94" s="1">
+      <c r="O94">
         <v>62694</v>
       </c>
       <c r="P94" t="s">
         <v>103</v>
       </c>
-      <c r="Q94" s="1" t="s">
-        <v>350</v>
+      <c r="Q94" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
@@ -5242,30 +5241,30 @@
         <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C95" t="s">
         <v>120</v>
       </c>
-      <c r="H95" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="K95" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="M95" s="1" t="s">
-        <v>327</v>
+      <c r="H95" t="s">
+        <v>558</v>
+      </c>
+      <c r="K95" t="s">
+        <v>244</v>
+      </c>
+      <c r="M95" t="s">
+        <v>325</v>
       </c>
       <c r="N95" t="s">
         <v>121</v>
       </c>
-      <c r="O95" s="1">
+      <c r="O95">
         <v>62565</v>
       </c>
       <c r="P95" t="s">
         <v>104</v>
       </c>
-      <c r="Q95" s="1" t="s">
+      <c r="Q95" t="s">
         <v>173</v>
       </c>
     </row>
@@ -5274,31 +5273,31 @@
         <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C96" t="s">
         <v>120</v>
       </c>
-      <c r="H96" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="K96" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="M96" s="1" t="s">
-        <v>328</v>
+      <c r="H96" t="s">
+        <v>559</v>
+      </c>
+      <c r="K96" t="s">
+        <v>245</v>
+      </c>
+      <c r="M96" t="s">
+        <v>326</v>
       </c>
       <c r="N96" t="s">
         <v>121</v>
       </c>
-      <c r="O96" s="1">
+      <c r="O96">
         <v>62220</v>
       </c>
       <c r="P96" t="s">
         <v>105</v>
       </c>
-      <c r="Q96" s="1" t="s">
-        <v>374</v>
+      <c r="Q96" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
@@ -5306,31 +5305,31 @@
         <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C97" t="s">
         <v>120</v>
       </c>
-      <c r="H97" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="K97" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="M97" s="1" t="s">
-        <v>329</v>
+      <c r="H97" t="s">
+        <v>560</v>
+      </c>
+      <c r="K97" t="s">
+        <v>246</v>
+      </c>
+      <c r="M97" t="s">
+        <v>327</v>
       </c>
       <c r="N97" t="s">
         <v>121</v>
       </c>
-      <c r="O97" s="1">
+      <c r="O97">
         <v>61483</v>
       </c>
       <c r="P97" t="s">
         <v>106</v>
       </c>
-      <c r="Q97" s="1" t="s">
-        <v>375</v>
+      <c r="Q97" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
@@ -5338,31 +5337,31 @@
         <v>89</v>
       </c>
       <c r="B98" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C98" t="s">
         <v>120</v>
       </c>
-      <c r="H98" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="K98" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="M98" s="1" t="s">
-        <v>330</v>
+      <c r="H98" t="s">
+        <v>561</v>
+      </c>
+      <c r="K98" t="s">
+        <v>247</v>
+      </c>
+      <c r="M98" t="s">
+        <v>328</v>
       </c>
       <c r="N98" t="s">
         <v>121</v>
       </c>
-      <c r="O98" s="1">
+      <c r="O98">
         <v>61032</v>
       </c>
       <c r="P98" t="s">
         <v>107</v>
       </c>
-      <c r="Q98" s="1" t="s">
-        <v>360</v>
+      <c r="Q98" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
@@ -5370,31 +5369,31 @@
         <v>90</v>
       </c>
       <c r="B99" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C99" t="s">
         <v>120</v>
       </c>
-      <c r="H99" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="K99" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="M99" s="1" t="s">
-        <v>331</v>
+      <c r="H99" t="s">
+        <v>562</v>
+      </c>
+      <c r="K99" t="s">
+        <v>248</v>
+      </c>
+      <c r="M99" t="s">
+        <v>329</v>
       </c>
       <c r="N99" t="s">
         <v>121</v>
       </c>
-      <c r="O99" s="1">
+      <c r="O99">
         <v>61554</v>
       </c>
       <c r="P99" t="s">
         <v>108</v>
       </c>
-      <c r="Q99" s="1" t="s">
-        <v>376</v>
+      <c r="Q99" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
@@ -5402,31 +5401,31 @@
         <v>91</v>
       </c>
       <c r="B100" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C100" t="s">
         <v>120</v>
       </c>
-      <c r="H100" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="K100" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="M100" s="1" t="s">
-        <v>332</v>
+      <c r="H100" t="s">
+        <v>563</v>
+      </c>
+      <c r="K100" t="s">
+        <v>249</v>
+      </c>
+      <c r="M100" t="s">
+        <v>330</v>
       </c>
       <c r="N100" t="s">
         <v>121</v>
       </c>
-      <c r="O100" s="1">
+      <c r="O100">
         <v>62952</v>
       </c>
       <c r="P100" t="s">
         <v>109</v>
       </c>
-      <c r="Q100" s="1" t="s">
-        <v>377</v>
+      <c r="Q100" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
@@ -5434,30 +5433,30 @@
         <v>92</v>
       </c>
       <c r="B101" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C101" t="s">
         <v>120</v>
       </c>
-      <c r="H101" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="K101" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="M101" s="1" t="s">
-        <v>333</v>
+      <c r="H101" t="s">
+        <v>564</v>
+      </c>
+      <c r="K101" t="s">
+        <v>250</v>
+      </c>
+      <c r="M101" t="s">
+        <v>331</v>
       </c>
       <c r="N101" t="s">
         <v>121</v>
       </c>
-      <c r="O101" s="1">
+      <c r="O101">
         <v>61832</v>
       </c>
       <c r="P101" t="s">
         <v>110</v>
       </c>
-      <c r="Q101" s="1" t="s">
+      <c r="Q101" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5466,31 +5465,31 @@
         <v>93</v>
       </c>
       <c r="B102" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C102" t="s">
         <v>120</v>
       </c>
-      <c r="H102" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="K102" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="M102" s="1" t="s">
-        <v>334</v>
+      <c r="H102" t="s">
+        <v>565</v>
+      </c>
+      <c r="K102" t="s">
+        <v>251</v>
+      </c>
+      <c r="M102" t="s">
+        <v>332</v>
       </c>
       <c r="N102" t="s">
         <v>121</v>
       </c>
-      <c r="O102" s="1">
+      <c r="O102">
         <v>62863</v>
       </c>
       <c r="P102" t="s">
         <v>111</v>
       </c>
-      <c r="Q102" s="1" t="s">
-        <v>344</v>
+      <c r="Q102" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
@@ -5498,31 +5497,31 @@
         <v>94</v>
       </c>
       <c r="B103" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C103" t="s">
         <v>120</v>
       </c>
-      <c r="H103" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="K103" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="M103" s="1" t="s">
-        <v>335</v>
+      <c r="H103" t="s">
+        <v>506</v>
+      </c>
+      <c r="K103" t="s">
+        <v>252</v>
+      </c>
+      <c r="M103" t="s">
+        <v>333</v>
       </c>
       <c r="N103" t="s">
         <v>121</v>
       </c>
-      <c r="O103" s="1">
+      <c r="O103">
         <v>61462</v>
       </c>
       <c r="P103" t="s">
         <v>112</v>
       </c>
-      <c r="Q103" s="1" t="s">
-        <v>378</v>
+      <c r="Q103" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
@@ -5530,24 +5529,24 @@
         <v>95</v>
       </c>
       <c r="B104" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C104" t="s">
         <v>120</v>
       </c>
-      <c r="H104" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="K104" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="M104" s="1" t="s">
-        <v>336</v>
+      <c r="H104" t="s">
+        <v>566</v>
+      </c>
+      <c r="K104" t="s">
+        <v>253</v>
+      </c>
+      <c r="M104" t="s">
+        <v>334</v>
       </c>
       <c r="N104" t="s">
         <v>121</v>
       </c>
-      <c r="O104" s="1">
+      <c r="O104">
         <v>62263</v>
       </c>
       <c r="P104" t="s">
@@ -5559,31 +5558,31 @@
         <v>96</v>
       </c>
       <c r="B105" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C105" t="s">
         <v>120</v>
       </c>
-      <c r="H105" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="K105" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="M105" s="1" t="s">
-        <v>337</v>
+      <c r="H105" t="s">
+        <v>567</v>
+      </c>
+      <c r="K105" t="s">
+        <v>254</v>
+      </c>
+      <c r="M105" t="s">
+        <v>335</v>
       </c>
       <c r="N105" t="s">
         <v>121</v>
       </c>
-      <c r="O105" s="1">
+      <c r="O105">
         <v>62837</v>
       </c>
       <c r="P105" t="s">
         <v>113</v>
       </c>
-      <c r="Q105" s="1" t="s">
-        <v>344</v>
+      <c r="Q105" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
@@ -5591,31 +5590,31 @@
         <v>97</v>
       </c>
       <c r="B106" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C106" t="s">
         <v>120</v>
       </c>
-      <c r="H106" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="K106" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="M106" s="1" t="s">
-        <v>338</v>
+      <c r="H106" t="s">
+        <v>568</v>
+      </c>
+      <c r="K106" t="s">
+        <v>255</v>
+      </c>
+      <c r="M106" t="s">
+        <v>336</v>
       </c>
       <c r="N106" t="s">
         <v>121</v>
       </c>
-      <c r="O106" s="1">
+      <c r="O106">
         <v>62821</v>
       </c>
       <c r="P106" t="s">
         <v>114</v>
       </c>
-      <c r="Q106" s="1" t="s">
-        <v>344</v>
+      <c r="Q106" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
@@ -5623,31 +5622,31 @@
         <v>98</v>
       </c>
       <c r="B107" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C107" t="s">
         <v>120</v>
       </c>
-      <c r="H107" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="K107" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="M107" s="1" t="s">
-        <v>339</v>
+      <c r="H107" t="s">
+        <v>569</v>
+      </c>
+      <c r="K107" t="s">
+        <v>256</v>
+      </c>
+      <c r="M107" t="s">
+        <v>337</v>
       </c>
       <c r="N107" t="s">
         <v>121</v>
       </c>
-      <c r="O107" s="1">
+      <c r="O107">
         <v>61270</v>
       </c>
       <c r="P107" t="s">
         <v>115</v>
       </c>
-      <c r="Q107" s="1" t="s">
-        <v>379</v>
+      <c r="Q107" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
@@ -5655,31 +5654,31 @@
         <v>99</v>
       </c>
       <c r="B108" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C108" t="s">
         <v>120</v>
       </c>
-      <c r="H108" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="K108" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="M108" s="1" t="s">
-        <v>340</v>
+      <c r="H108" t="s">
+        <v>570</v>
+      </c>
+      <c r="K108" t="s">
+        <v>257</v>
+      </c>
+      <c r="M108" t="s">
+        <v>338</v>
       </c>
       <c r="N108" t="s">
         <v>121</v>
       </c>
-      <c r="O108" s="1">
+      <c r="O108">
         <v>60432</v>
       </c>
       <c r="P108" t="s">
         <v>116</v>
       </c>
-      <c r="Q108" s="1" t="s">
-        <v>380</v>
+      <c r="Q108" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
@@ -5687,30 +5686,30 @@
         <v>100</v>
       </c>
       <c r="B109" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C109" t="s">
         <v>120</v>
       </c>
-      <c r="H109" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="K109" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M109" s="1" t="s">
+      <c r="H109" t="s">
+        <v>571</v>
+      </c>
+      <c r="K109" t="s">
+        <v>258</v>
+      </c>
+      <c r="M109" t="s">
         <v>76</v>
       </c>
       <c r="N109" t="s">
         <v>121</v>
       </c>
-      <c r="O109" s="1">
+      <c r="O109">
         <v>62959</v>
       </c>
       <c r="P109" t="s">
         <v>117</v>
       </c>
-      <c r="Q109" s="1" t="s">
+      <c r="Q109" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5719,30 +5718,30 @@
         <v>101</v>
       </c>
       <c r="B110" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C110" t="s">
         <v>120</v>
       </c>
-      <c r="H110" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="K110" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="M110" s="1" t="s">
-        <v>341</v>
+      <c r="H110" t="s">
+        <v>572</v>
+      </c>
+      <c r="K110" t="s">
+        <v>259</v>
+      </c>
+      <c r="M110" t="s">
+        <v>339</v>
       </c>
       <c r="N110" t="s">
         <v>121</v>
       </c>
-      <c r="O110" s="1">
+      <c r="O110">
         <v>61101</v>
       </c>
       <c r="P110" t="s">
         <v>118</v>
       </c>
-      <c r="Q110" s="1" t="s">
+      <c r="Q110" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5751,31 +5750,31 @@
         <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C111" t="s">
         <v>120</v>
       </c>
-      <c r="H111" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="K111" s="1" t="s">
+      <c r="H111" t="s">
+        <v>340</v>
+      </c>
+      <c r="K111" t="s">
+        <v>260</v>
+      </c>
+      <c r="M111" t="s">
         <v>261</v>
       </c>
-      <c r="M111" s="1" t="s">
-        <v>262</v>
-      </c>
       <c r="N111" t="s">
         <v>121</v>
       </c>
-      <c r="O111" s="1">
+      <c r="O111">
         <v>61530</v>
       </c>
       <c r="P111" t="s">
         <v>119</v>
       </c>
-      <c r="Q111" s="1" t="s">
-        <v>343</v>
+      <c r="Q111" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated il courts list
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/il_courts.xlsx
+++ b/docassemble/ILAO/data/sources/il_courts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Downloads\update courthouse list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1F8E4E-7545-4E92-A7BF-BD1FCD272D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE28CCEC-93BC-4514-BA13-7FD1779D810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5295" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="570" windowWidth="28800" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="636">
   <si>
     <t>name</t>
   </si>
@@ -525,36 +525,15 @@
     <t>(217) 348-0538</t>
   </si>
   <si>
-    <t>https://www.co.adams.il.us</t>
-  </si>
-  <si>
     <t>http://www.firstcircuitil.org/</t>
   </si>
   <si>
-    <t>https://bondcountyil.com/bond-county-courthouse/</t>
-  </si>
-  <si>
-    <t>http://www.17thcircuit.illinoiscourts.gov</t>
-  </si>
-  <si>
     <t>https://www.co.adams.il.us/government/departments/judicial</t>
   </si>
   <si>
     <t>http://www.15thjudicialcircuit.com/</t>
   </si>
   <si>
-    <t>http://www.co.champaign.il.us/circuitcourt/circuitcourt.php</t>
-  </si>
-  <si>
-    <t>https://fourthcircuitil.com/</t>
-  </si>
-  <si>
-    <t>http://fifthcircuitil.com/</t>
-  </si>
-  <si>
-    <t>https://circuitclerk.bureaucounty-il.gov</t>
-  </si>
-  <si>
     <t>1 Court St.</t>
   </si>
   <si>
@@ -579,18 +558,12 @@
     <t>50 E. Main</t>
   </si>
   <si>
-    <t>120 W Jefferson, Suite 101</t>
-  </si>
-  <si>
     <t>221 S 7th Street</t>
   </si>
   <si>
     <t>200 West State</t>
   </si>
   <si>
-    <t>901 Public Square</t>
-  </si>
-  <si>
     <t>100 N. Main St.</t>
   </si>
   <si>
@@ -675,9 +648,6 @@
     <t>155 N. Main Street</t>
   </si>
   <si>
-    <t>100 East Main Street</t>
-  </si>
-  <si>
     <t>122 N. Prairie St.</t>
   </si>
   <si>
@@ -711,15 +681,9 @@
     <t>300 W. State Street</t>
   </si>
   <si>
-    <t>10 South Main Street Suite 12</t>
-  </si>
-  <si>
     <t>106 S. 5th St.</t>
   </si>
   <si>
-    <t>324 Main St., Ste. 215</t>
-  </si>
-  <si>
     <t>1 Public Square Floor 2</t>
   </si>
   <si>
@@ -999,9 +963,6 @@
     <t>Rushville</t>
   </si>
   <si>
-    <t xml:space="preserve"> Winchester</t>
-  </si>
-  <si>
     <t>Shelbyville</t>
   </si>
   <si>
@@ -1050,78 +1011,21 @@
     <t>(309) 467-3312</t>
   </si>
   <si>
-    <t>http://www.woodford-county.org/</t>
-  </si>
-  <si>
     <t>http://www.illinoissecondcircuit.info/</t>
   </si>
   <si>
-    <t>https://dekalbcounty.org/</t>
-  </si>
-  <si>
-    <t>http://www.sixthcircuitcourt.com/</t>
-  </si>
-  <si>
     <t>https://www.dupageco.org/courts/</t>
   </si>
   <si>
-    <t>https://www.mcleancountyil.gov/581/Circuit-Court-Rules-11th-Judicial-Circui</t>
-  </si>
-  <si>
-    <t>http://www.9thjudicial.org/Fulton/fulton.html</t>
-  </si>
-  <si>
-    <t>https://co.sangamon.il.us/departments/s-z/seventh-judicial-circuit-court</t>
-  </si>
-  <si>
-    <t>https://www.grundyco.org/grundy-county-courthouse/</t>
-  </si>
-  <si>
     <t>http://www.9thjudicial.org/Hancock/hancock.html</t>
   </si>
   <si>
-    <t>http://www.9thjudicial.org/Henderson/henderson.html</t>
-  </si>
-  <si>
     <t>https://www.rockislandcounty.org/CourtAdmin/Home/</t>
   </si>
   <si>
-    <t>https://www.k3county.net/21stJudicial/index.html</t>
-  </si>
-  <si>
-    <t>https://www.illinois16thjudicialcircuit.org/</t>
-  </si>
-  <si>
-    <t>https://www.co.kendall.il.us/offices/judiciary</t>
-  </si>
-  <si>
-    <t>http://www.9thjudicial.org/Knox/knox.html</t>
-  </si>
-  <si>
-    <t>https://www.19thcircuitcourt.state.il.us/</t>
-  </si>
-  <si>
     <t>http://www.15thjudicialcircuit.com</t>
   </si>
   <si>
-    <t>https://www.livingstoncounty-il.org/wordpress/county-services/circuit-court/</t>
-  </si>
-  <si>
-    <t>https://www.co.madison.il.us/departments/circuit_court/index.php</t>
-  </si>
-  <si>
-    <t>http://www.10thcircuitcourtil.org</t>
-  </si>
-  <si>
-    <t>http://www.9thjudicial.org/Mcdonough/mcdonough.html</t>
-  </si>
-  <si>
-    <t>https://www.mchenrycountyil.gov/county-government/courts/22nd-judicial-circuit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mcleancountyil.gov/81/Circuit-Court </t>
-  </si>
-  <si>
     <t>https://www.menardcountyil.com/elected-officials/circuit-court-clerk/</t>
   </si>
   <si>
@@ -1131,39 +1035,12 @@
     <t>https://www.pikecountyil.org/circuit-court/</t>
   </si>
   <si>
-    <t>https://10thcircuitcourtil.org/</t>
-  </si>
-  <si>
-    <t>https://am.randolphco.org/index.php/gov-menu/judicial-circuit/circuitjudge-menu</t>
-  </si>
-  <si>
-    <t>https://www.rockislandcounty.org/CourtServices/Home/</t>
-  </si>
-  <si>
     <t>https://co.sangamon.il.us/courts</t>
   </si>
   <si>
-    <t>https://www.co.st-clair.il.us</t>
-  </si>
-  <si>
-    <t>http://www.starkcountyillinois.com/</t>
-  </si>
-  <si>
-    <t>https://www.10thcircuitcourtil.org/</t>
-  </si>
-  <si>
     <t>https://www.unioncountyil.gov/union-county-courthouse/</t>
   </si>
   <si>
-    <t>http://www.9thjudicial.org/Warren/warren.html</t>
-  </si>
-  <si>
-    <t>https://www.whiteside.org/</t>
-  </si>
-  <si>
-    <t>http://www.willcountycourts.com</t>
-  </si>
-  <si>
     <t>Richard J. Daley Center</t>
   </si>
   <si>
@@ -1512,9 +1389,6 @@
     <t>(630) 407-8904</t>
   </si>
   <si>
-    <t>(217) 466-7447</t>
-  </si>
-  <si>
     <t>(618) 445-2016</t>
   </si>
   <si>
@@ -1686,9 +1560,6 @@
     <t>(618) 392-2151</t>
   </si>
   <si>
-    <t>309-558-3312</t>
-  </si>
-  <si>
     <t>(618) 253-5096</t>
   </si>
   <si>
@@ -1734,9 +1605,6 @@
     <t>(618) 382-7211</t>
   </si>
   <si>
-    <t>815-772-5170</t>
-  </si>
-  <si>
     <t>(815) 727-8540</t>
   </si>
   <si>
@@ -1833,9 +1701,6 @@
     <t>http://www.cookcountycourt.org/ABOUT-THE-COURT/Municipal-Department/Sixth-Municipal-District-Markham</t>
   </si>
   <si>
-    <t>https://www.cookcountyclerkofcourt.org</t>
-  </si>
-  <si>
     <t>district</t>
   </si>
   <si>
@@ -1843,16 +1708,249 @@
   </si>
   <si>
     <t>Geneva</t>
+  </si>
+  <si>
+    <t>https://www.co.adams.il.us/government/departments/circuit-clerk</t>
+  </si>
+  <si>
+    <t>https://boonecircuitclerk.us/</t>
+  </si>
+  <si>
+    <t>https://www.bccircuitclerk.com/</t>
+  </si>
+  <si>
+    <t>https://circuitclerk.bureaucounty-il.gov/</t>
+  </si>
+  <si>
+    <t>https://co.cass.il.us/elected-officials/circuit-court-clerk</t>
+  </si>
+  <si>
+    <t>https://www.champaigncircuitclerk.org/</t>
+  </si>
+  <si>
+    <t>https://christiancountyil.com/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://www.clarkcountyil.org/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://claycountyillinois.org/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://clintoncountycircuitclerk.com/</t>
+  </si>
+  <si>
+    <t>https://cumberlandcoil.gov/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://dekalbcounty.org/departments/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://www.dewittcountyill.com/clerk.htm</t>
+  </si>
+  <si>
+    <t>http://www.douglascountyil.gov/circuit-clerk</t>
+  </si>
+  <si>
+    <t>https://edgarcountyillinois.com/offices/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>(217) 466-7473</t>
+  </si>
+  <si>
+    <t>120 W Jefferson</t>
+  </si>
+  <si>
+    <t>http://www.co.effingham.il.us/circuit-clerk</t>
+  </si>
+  <si>
+    <t>http://fayettecountyillinois.org/2159/Circuit-Clerk</t>
+  </si>
+  <si>
+    <t>https://fordcounty.illinois.gov/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>1 Public Square</t>
+  </si>
+  <si>
+    <t>https://franklincountyil.gov/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>http://www.9thjudicial.org/Fulton/fulton-circuit-clerk.html</t>
+  </si>
+  <si>
+    <t>www.grundycountyil.gov/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>http://www.9thjudicial.org/Henderson/henderson-circuit-clerk.html</t>
+  </si>
+  <si>
+    <t>https://iroquoiscountyil.gov/offices/circuit-clerk</t>
+  </si>
+  <si>
+    <t>http://www.jeffersoncountyillinois.com/contact-circuit-clerk</t>
+  </si>
+  <si>
+    <t>https://jerseycounty-il.gov/</t>
+  </si>
+  <si>
+    <t>https://cic.countyofkane.org/</t>
+  </si>
+  <si>
+    <t>https://kankakeecountycircuitclerk.com/ </t>
+  </si>
+  <si>
+    <t>https://www.co.kendall.il.us/offices/circuit-clerk</t>
+  </si>
+  <si>
+    <t>https://co.knox.il.us/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://www.lakecountycircuitclerk.org/</t>
+  </si>
+  <si>
+    <t>https://www.lasallecounty.com/ </t>
+  </si>
+  <si>
+    <t>https://www.livingstoncounty-il.org/wordpress/county-services/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://logancountyil.gov/index.php?option=com_content&amp;view=article&amp;id=168&amp;Itemid=530&amp;lang=en</t>
+  </si>
+  <si>
+    <t>https://www.cclerk.co.macon.il.us/</t>
+  </si>
+  <si>
+    <t>https://www.macoupincountyil.gov/circuit_clerk.htm</t>
+  </si>
+  <si>
+    <t>https://www.co.madison.il.us/departments/circuit_clerk/index.php</t>
+  </si>
+  <si>
+    <t>100 East Main Street, Room 204</t>
+  </si>
+  <si>
+    <t>https://marioncountycircuitclerk.org/</t>
+  </si>
+  <si>
+    <t>http://marshallcountyillinois.com/elected-officials/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://www.masoncountyil.gov/circuit.htm</t>
+  </si>
+  <si>
+    <t>http://mcg.mcdonough.il.us/circuitclerk.html</t>
+  </si>
+  <si>
+    <t>https://www.mchenrycountyil.gov/county-government/departments-a-i/circuit-clerk</t>
+  </si>
+  <si>
+    <t>https://www.mcleancountyil.gov/80/Circuit-Clerk</t>
+  </si>
+  <si>
+    <t>https://monroecountyil.gov/departments/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://montgomeryco.com/index.php/circuit-court-clerk</t>
+  </si>
+  <si>
+    <t>http://morgancounty-il.com/departments/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>10 South Main Street</t>
+  </si>
+  <si>
+    <t>https://www.moultriecountyil.com/departments/circuit_clerk/index.php</t>
+  </si>
+  <si>
+    <t>324 Main St.</t>
+  </si>
+  <si>
+    <t>https://www.peoriacounty.gov/1215/Circuit-Clerk</t>
+  </si>
+  <si>
+    <t>https://piatt.gov/circuit_clerk/ </t>
+  </si>
+  <si>
+    <t>https://www.co.putnam.il.us/county-offices/circuit-court-clerk-office</t>
+  </si>
+  <si>
+    <t>https://am.randolphco.org/index.php/gov-menu/electedofficials/circuitclerk-menu</t>
+  </si>
+  <si>
+    <t>https://richlandcountycourt.org/</t>
+  </si>
+  <si>
+    <t>(309) 558-3289</t>
+  </si>
+  <si>
+    <t>http://www.rockislandcounty.org/CircuitClerk/Home/</t>
+  </si>
+  <si>
+    <t>https://www.sangamoncountycircuitclerk.org/</t>
+  </si>
+  <si>
+    <t>Winchester</t>
+  </si>
+  <si>
+    <t>https://www.co.st-clair.il.us/departments/circuit-clerk</t>
+  </si>
+  <si>
+    <t>http://www.starkcountyillinois.com/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>https://tazewellcountyil.com/</t>
+  </si>
+  <si>
+    <t>https://www.vercounty.org/</t>
+  </si>
+  <si>
+    <t>http://www.warrencountyil.com/offices/circuit-clerk</t>
+  </si>
+  <si>
+    <t>https://washingtoncountycircuitclerk.com/index.htm</t>
+  </si>
+  <si>
+    <t>https://wayneclerk.com/</t>
+  </si>
+  <si>
+    <t>(815) 772-5170</t>
+  </si>
+  <si>
+    <t>https://www.whiteside.org/county-information/general-information/whiteside-county-courts/2008061750.html</t>
+  </si>
+  <si>
+    <t>https://www.circuitclerkofwillcounty.com/</t>
+  </si>
+  <si>
+    <t>https://www.cc.co.winnebago.il.us/</t>
+  </si>
+  <si>
+    <t>https://www.woodford-county.org/154/Clerk-of-the-Circuit-Court</t>
+  </si>
+  <si>
+    <t>https://www.cookcountycourt.org/</t>
+  </si>
+  <si>
+    <t>https://bondcountyil.gov/circuit-clerk/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1875,13 +1973,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2162,10 +2263,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <selection pane="bottomLeft" activeCell="Q102" sqref="Q102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,7 +2284,7 @@
     <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.140625" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="110.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="81.28515625" customWidth="1"/>
     <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
@@ -2200,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>603</v>
+        <v>558</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2256,7 +2357,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>347</v>
       </c>
       <c r="C2" t="s">
         <v>120</v>
@@ -2280,7 +2381,7 @@
         <v>19</v>
       </c>
       <c r="Q2" t="s">
-        <v>166</v>
+        <v>561</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2288,7 +2389,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>348</v>
       </c>
       <c r="C3" t="s">
         <v>120</v>
@@ -2312,7 +2413,7 @@
         <v>20</v>
       </c>
       <c r="Q3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -2320,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>390</v>
+        <v>349</v>
       </c>
       <c r="C4" t="s">
         <v>120</v>
@@ -2344,7 +2445,7 @@
         <v>21</v>
       </c>
       <c r="Q4" t="s">
-        <v>168</v>
+        <v>635</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -2352,7 +2453,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>391</v>
+        <v>350</v>
       </c>
       <c r="C5" t="s">
         <v>120</v>
@@ -2376,7 +2477,7 @@
         <v>22</v>
       </c>
       <c r="Q5" t="s">
-        <v>169</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -2384,7 +2485,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>392</v>
+        <v>351</v>
       </c>
       <c r="C6" t="s">
         <v>120</v>
@@ -2408,7 +2509,7 @@
         <v>23</v>
       </c>
       <c r="Q6" t="s">
-        <v>170</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -2416,7 +2517,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>393</v>
+        <v>352</v>
       </c>
       <c r="C7" t="s">
         <v>120</v>
@@ -2440,7 +2541,7 @@
         <v>24</v>
       </c>
       <c r="Q7" t="s">
-        <v>175</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2448,7 +2549,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>394</v>
+        <v>353</v>
       </c>
       <c r="C8" t="s">
         <v>120</v>
@@ -2471,8 +2572,8 @@
       <c r="P8" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" t="s">
-        <v>170</v>
+      <c r="Q8" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2480,7 +2581,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>395</v>
+        <v>354</v>
       </c>
       <c r="C9" t="s">
         <v>120</v>
@@ -2504,7 +2605,7 @@
         <v>26</v>
       </c>
       <c r="Q9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2512,7 +2613,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>396</v>
+        <v>355</v>
       </c>
       <c r="C10" t="s">
         <v>120</v>
@@ -2536,7 +2637,7 @@
         <v>27</v>
       </c>
       <c r="Q10" t="s">
-        <v>170</v>
+        <v>565</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2544,7 +2645,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>397</v>
+        <v>356</v>
       </c>
       <c r="C11" t="s">
         <v>120</v>
@@ -2568,7 +2669,7 @@
         <v>28</v>
       </c>
       <c r="Q11" t="s">
-        <v>172</v>
+        <v>566</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -2576,7 +2677,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>398</v>
+        <v>357</v>
       </c>
       <c r="C12" t="s">
         <v>120</v>
@@ -2600,7 +2701,7 @@
         <v>29</v>
       </c>
       <c r="Q12" t="s">
-        <v>173</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -2608,7 +2709,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>399</v>
+        <v>358</v>
       </c>
       <c r="C13" t="s">
         <v>120</v>
@@ -2632,7 +2733,7 @@
         <v>30</v>
       </c>
       <c r="Q13" t="s">
-        <v>174</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -2640,7 +2741,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>400</v>
+        <v>359</v>
       </c>
       <c r="C14" t="s">
         <v>120</v>
@@ -2664,7 +2765,7 @@
         <v>31</v>
       </c>
       <c r="Q14" t="s">
-        <v>173</v>
+        <v>569</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -2672,7 +2773,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>401</v>
+        <v>360</v>
       </c>
       <c r="C15" t="s">
         <v>120</v>
@@ -2696,7 +2797,7 @@
         <v>32</v>
       </c>
       <c r="Q15" t="s">
-        <v>173</v>
+        <v>570</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2704,7 +2805,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>402</v>
+        <v>361</v>
       </c>
       <c r="C16" t="s">
         <v>120</v>
@@ -2727,16 +2828,14 @@
       <c r="P16" t="s">
         <v>33</v>
       </c>
-      <c r="Q16" t="s">
-        <v>174</v>
-      </c>
+      <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>379</v>
+        <v>338</v>
       </c>
       <c r="C17" t="s">
         <v>120</v>
@@ -2745,13 +2844,13 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>573</v>
+        <v>529</v>
       </c>
       <c r="K17" t="s">
-        <v>588</v>
+        <v>544</v>
       </c>
       <c r="M17" t="s">
-        <v>591</v>
+        <v>547</v>
       </c>
       <c r="N17" t="s">
         <v>121</v>
@@ -2763,7 +2862,7 @@
         <v>34</v>
       </c>
       <c r="Q17" t="s">
-        <v>602</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2771,7 +2870,7 @@
         <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>380</v>
+        <v>339</v>
       </c>
       <c r="C18" t="s">
         <v>120</v>
@@ -2780,13 +2879,13 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>574</v>
+        <v>530</v>
       </c>
       <c r="K18" t="s">
-        <v>582</v>
+        <v>538</v>
       </c>
       <c r="M18" t="s">
-        <v>592</v>
+        <v>548</v>
       </c>
       <c r="N18" t="s">
         <v>121</v>
@@ -2798,7 +2897,7 @@
         <v>34</v>
       </c>
       <c r="Q18" t="s">
-        <v>597</v>
+        <v>553</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2806,7 +2905,7 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>381</v>
+        <v>340</v>
       </c>
       <c r="C19" t="s">
         <v>120</v>
@@ -2815,13 +2914,13 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
       <c r="K19" t="s">
-        <v>583</v>
+        <v>539</v>
       </c>
       <c r="M19" t="s">
-        <v>593</v>
+        <v>549</v>
       </c>
       <c r="N19" t="s">
         <v>121</v>
@@ -2833,7 +2932,7 @@
         <v>34</v>
       </c>
       <c r="Q19" t="s">
-        <v>598</v>
+        <v>554</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2841,7 +2940,7 @@
         <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>382</v>
+        <v>341</v>
       </c>
       <c r="C20" t="s">
         <v>120</v>
@@ -2850,13 +2949,13 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>576</v>
+        <v>532</v>
       </c>
       <c r="K20" t="s">
-        <v>584</v>
+        <v>540</v>
       </c>
       <c r="M20" t="s">
-        <v>594</v>
+        <v>550</v>
       </c>
       <c r="N20" t="s">
         <v>121</v>
@@ -2868,7 +2967,7 @@
         <v>34</v>
       </c>
       <c r="Q20" t="s">
-        <v>599</v>
+        <v>555</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2876,7 +2975,7 @@
         <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>383</v>
+        <v>342</v>
       </c>
       <c r="C21" t="s">
         <v>120</v>
@@ -2885,13 +2984,13 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>577</v>
+        <v>533</v>
       </c>
       <c r="K21" t="s">
-        <v>585</v>
+        <v>541</v>
       </c>
       <c r="M21" t="s">
-        <v>595</v>
+        <v>551</v>
       </c>
       <c r="N21" t="s">
         <v>121</v>
@@ -2903,7 +3002,7 @@
         <v>34</v>
       </c>
       <c r="Q21" t="s">
-        <v>600</v>
+        <v>556</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2911,7 +3010,7 @@
         <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>384</v>
+        <v>343</v>
       </c>
       <c r="C22" t="s">
         <v>120</v>
@@ -2920,13 +3019,13 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>578</v>
+        <v>534</v>
       </c>
       <c r="K22" t="s">
-        <v>586</v>
+        <v>542</v>
       </c>
       <c r="M22" t="s">
-        <v>596</v>
+        <v>552</v>
       </c>
       <c r="N22" t="s">
         <v>121</v>
@@ -2938,7 +3037,7 @@
         <v>34</v>
       </c>
       <c r="Q22" t="s">
-        <v>601</v>
+        <v>557</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -2946,19 +3045,19 @@
         <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>385</v>
+        <v>344</v>
       </c>
       <c r="C23" t="s">
         <v>120</v>
       </c>
       <c r="H23" t="s">
-        <v>579</v>
+        <v>535</v>
       </c>
       <c r="K23" t="s">
-        <v>589</v>
+        <v>545</v>
       </c>
       <c r="M23" t="s">
-        <v>591</v>
+        <v>547</v>
       </c>
       <c r="N23" t="s">
         <v>121</v>
@@ -2970,7 +3069,7 @@
         <v>34</v>
       </c>
       <c r="Q23" t="s">
-        <v>602</v>
+        <v>634</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -2978,19 +3077,19 @@
         <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>386</v>
+        <v>345</v>
       </c>
       <c r="C24" t="s">
         <v>120</v>
       </c>
       <c r="H24" t="s">
-        <v>580</v>
+        <v>536</v>
       </c>
       <c r="K24" t="s">
-        <v>587</v>
+        <v>543</v>
       </c>
       <c r="M24" t="s">
-        <v>591</v>
+        <v>547</v>
       </c>
       <c r="N24" t="s">
         <v>121</v>
@@ -3002,7 +3101,7 @@
         <v>34</v>
       </c>
       <c r="Q24" t="s">
-        <v>602</v>
+        <v>634</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -3010,19 +3109,19 @@
         <v>110</v>
       </c>
       <c r="B25" t="s">
-        <v>387</v>
+        <v>346</v>
       </c>
       <c r="C25" t="s">
         <v>120</v>
       </c>
       <c r="H25" t="s">
-        <v>581</v>
+        <v>537</v>
       </c>
       <c r="K25" t="s">
-        <v>590</v>
+        <v>546</v>
       </c>
       <c r="M25" t="s">
-        <v>591</v>
+        <v>547</v>
       </c>
       <c r="N25" t="s">
         <v>121</v>
@@ -3034,7 +3133,7 @@
         <v>34</v>
       </c>
       <c r="Q25" t="s">
-        <v>602</v>
+        <v>634</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -3042,19 +3141,19 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>403</v>
+        <v>362</v>
       </c>
       <c r="C26" t="s">
         <v>120</v>
       </c>
       <c r="H26" t="s">
-        <v>489</v>
+        <v>448</v>
       </c>
       <c r="K26" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="M26" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="N26" t="s">
         <v>121</v>
@@ -3066,7 +3165,7 @@
         <v>35</v>
       </c>
       <c r="Q26" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -3074,19 +3173,19 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>404</v>
+        <v>363</v>
       </c>
       <c r="C27" t="s">
         <v>120</v>
       </c>
       <c r="H27" t="s">
-        <v>490</v>
+        <v>449</v>
       </c>
       <c r="K27" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="M27" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="N27" t="s">
         <v>121</v>
@@ -3098,7 +3197,7 @@
         <v>36</v>
       </c>
       <c r="Q27" t="s">
-        <v>174</v>
+        <v>571</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -3106,19 +3205,19 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>405</v>
+        <v>364</v>
       </c>
       <c r="C28" t="s">
         <v>120</v>
       </c>
       <c r="H28" t="s">
-        <v>491</v>
+        <v>450</v>
       </c>
       <c r="K28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="M28" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="N28" t="s">
         <v>121</v>
@@ -3130,7 +3229,7 @@
         <v>37</v>
       </c>
       <c r="Q28" t="s">
-        <v>343</v>
+        <v>572</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -3138,16 +3237,16 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>406</v>
+        <v>365</v>
       </c>
       <c r="C29" t="s">
         <v>120</v>
       </c>
       <c r="H29" t="s">
-        <v>492</v>
+        <v>451</v>
       </c>
       <c r="K29" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="M29" t="s">
         <v>32</v>
@@ -3162,7 +3261,7 @@
         <v>38</v>
       </c>
       <c r="Q29" t="s">
-        <v>344</v>
+        <v>573</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -3170,19 +3269,19 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>407</v>
+        <v>366</v>
       </c>
       <c r="C30" t="s">
         <v>120</v>
       </c>
       <c r="H30" t="s">
-        <v>493</v>
+        <v>452</v>
       </c>
       <c r="K30" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="M30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="N30" t="s">
         <v>121</v>
@@ -3194,7 +3293,7 @@
         <v>39</v>
       </c>
       <c r="Q30" t="s">
-        <v>344</v>
+        <v>574</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -3202,19 +3301,19 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>408</v>
+        <v>367</v>
       </c>
       <c r="C31" t="s">
         <v>120</v>
       </c>
       <c r="H31" t="s">
-        <v>494</v>
+        <v>453</v>
       </c>
       <c r="K31" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="M31" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="N31" t="s">
         <v>121</v>
@@ -3226,7 +3325,7 @@
         <v>40</v>
       </c>
       <c r="Q31" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -3234,19 +3333,19 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>409</v>
+        <v>368</v>
       </c>
       <c r="C32" t="s">
         <v>120</v>
       </c>
       <c r="H32" t="s">
-        <v>495</v>
+        <v>576</v>
       </c>
       <c r="K32" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="M32" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="N32" t="s">
         <v>121</v>
@@ -3258,7 +3357,7 @@
         <v>41</v>
       </c>
       <c r="Q32" t="s">
-        <v>174</v>
+        <v>575</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -3266,19 +3365,19 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>410</v>
+        <v>369</v>
       </c>
       <c r="C33" t="s">
         <v>120</v>
       </c>
       <c r="H33" t="s">
-        <v>496</v>
+        <v>454</v>
       </c>
       <c r="K33" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="M33" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="N33" t="s">
         <v>121</v>
@@ -3290,7 +3389,7 @@
         <v>42</v>
       </c>
       <c r="Q33" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -3298,16 +3397,16 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>411</v>
+        <v>370</v>
       </c>
       <c r="C34" t="s">
         <v>120</v>
       </c>
       <c r="H34" t="s">
-        <v>497</v>
+        <v>455</v>
       </c>
       <c r="K34" t="s">
-        <v>184</v>
+        <v>577</v>
       </c>
       <c r="M34" t="s">
         <v>43</v>
@@ -3322,7 +3421,7 @@
         <v>43</v>
       </c>
       <c r="Q34" t="s">
-        <v>173</v>
+        <v>578</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -3330,19 +3429,19 @@
         <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>412</v>
+        <v>371</v>
       </c>
       <c r="C35" t="s">
         <v>120</v>
       </c>
       <c r="H35" t="s">
-        <v>498</v>
+        <v>456</v>
       </c>
       <c r="K35" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="M35" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="N35" t="s">
         <v>121</v>
@@ -3354,7 +3453,7 @@
         <v>44</v>
       </c>
       <c r="Q35" t="s">
-        <v>173</v>
+        <v>579</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -3362,19 +3461,19 @@
         <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>413</v>
+        <v>372</v>
       </c>
       <c r="C36" t="s">
         <v>120</v>
       </c>
       <c r="H36" t="s">
-        <v>499</v>
+        <v>457</v>
       </c>
       <c r="K36" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="M36" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="N36" t="s">
         <v>121</v>
@@ -3386,7 +3485,7 @@
         <v>45</v>
       </c>
       <c r="Q36" t="s">
-        <v>346</v>
+        <v>580</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -3394,19 +3493,19 @@
         <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>414</v>
+        <v>373</v>
       </c>
       <c r="C37" t="s">
         <v>120</v>
       </c>
       <c r="H37" t="s">
-        <v>500</v>
+        <v>458</v>
       </c>
       <c r="K37" t="s">
-        <v>187</v>
+        <v>581</v>
       </c>
       <c r="M37" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="N37" t="s">
         <v>121</v>
@@ -3418,7 +3517,7 @@
         <v>46</v>
       </c>
       <c r="Q37" t="s">
-        <v>342</v>
+        <v>582</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -3426,19 +3525,19 @@
         <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>415</v>
+        <v>374</v>
       </c>
       <c r="C38" t="s">
         <v>120</v>
       </c>
       <c r="H38" t="s">
-        <v>501</v>
+        <v>459</v>
       </c>
       <c r="K38" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="M38" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="N38" t="s">
         <v>121</v>
@@ -3450,7 +3549,7 @@
         <v>47</v>
       </c>
       <c r="Q38" t="s">
-        <v>347</v>
+        <v>583</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3458,19 +3557,19 @@
         <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>416</v>
+        <v>375</v>
       </c>
       <c r="C39" t="s">
         <v>120</v>
       </c>
       <c r="H39" t="s">
-        <v>502</v>
+        <v>460</v>
       </c>
       <c r="K39" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="M39" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="N39" t="s">
         <v>121</v>
@@ -3482,7 +3581,7 @@
         <v>48</v>
       </c>
       <c r="Q39" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -3490,19 +3589,19 @@
         <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>417</v>
+        <v>376</v>
       </c>
       <c r="C40" t="s">
         <v>120</v>
       </c>
       <c r="H40" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="K40" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="M40" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="N40" t="s">
         <v>121</v>
@@ -3512,9 +3611,6 @@
       </c>
       <c r="P40" t="s">
         <v>49</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -3522,19 +3618,19 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>418</v>
+        <v>377</v>
       </c>
       <c r="C41" t="s">
         <v>120</v>
       </c>
       <c r="H41" t="s">
-        <v>504</v>
+        <v>462</v>
       </c>
       <c r="K41" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="M41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="N41" t="s">
         <v>121</v>
@@ -3546,7 +3642,7 @@
         <v>50</v>
       </c>
       <c r="Q41" t="s">
-        <v>349</v>
+        <v>584</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -3554,19 +3650,19 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>419</v>
+        <v>378</v>
       </c>
       <c r="C42" t="s">
         <v>120</v>
       </c>
       <c r="H42" t="s">
-        <v>505</v>
+        <v>463</v>
       </c>
       <c r="K42" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="M42" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="N42" t="s">
         <v>121</v>
@@ -3578,7 +3674,7 @@
         <v>51</v>
       </c>
       <c r="Q42" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -3586,19 +3682,19 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>420</v>
+        <v>379</v>
       </c>
       <c r="C43" t="s">
         <v>120</v>
       </c>
       <c r="H43" t="s">
-        <v>506</v>
+        <v>464</v>
       </c>
       <c r="K43" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="M43" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="N43" t="s">
         <v>121</v>
@@ -3610,7 +3706,7 @@
         <v>52</v>
       </c>
       <c r="Q43" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -3618,19 +3714,19 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>421</v>
+        <v>380</v>
       </c>
       <c r="C44" t="s">
         <v>120</v>
       </c>
       <c r="H44" t="s">
-        <v>507</v>
+        <v>465</v>
       </c>
       <c r="K44" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="M44" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="N44" t="s">
         <v>121</v>
@@ -3640,9 +3736,6 @@
       </c>
       <c r="P44" t="s">
         <v>53</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -3650,19 +3743,19 @@
         <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>422</v>
+        <v>381</v>
       </c>
       <c r="C45" t="s">
         <v>120</v>
       </c>
       <c r="H45" t="s">
-        <v>508</v>
+        <v>466</v>
       </c>
       <c r="K45" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="M45" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="N45" t="s">
         <v>121</v>
@@ -3674,7 +3767,7 @@
         <v>54</v>
       </c>
       <c r="Q45" t="s">
-        <v>351</v>
+        <v>585</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -3682,19 +3775,19 @@
         <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>423</v>
+        <v>382</v>
       </c>
       <c r="C46" t="s">
         <v>120</v>
       </c>
       <c r="H46" t="s">
-        <v>509</v>
+        <v>467</v>
       </c>
       <c r="K46" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="M46" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="N46" t="s">
         <v>121</v>
@@ -3706,7 +3799,7 @@
         <v>55</v>
       </c>
       <c r="Q46" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -3714,19 +3807,19 @@
         <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>424</v>
+        <v>383</v>
       </c>
       <c r="C47" t="s">
         <v>120</v>
       </c>
       <c r="H47" t="s">
-        <v>510</v>
+        <v>468</v>
       </c>
       <c r="K47" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="M47" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="N47" t="s">
         <v>121</v>
@@ -3738,7 +3831,7 @@
         <v>56</v>
       </c>
       <c r="Q47" t="s">
-        <v>353</v>
+        <v>586</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -3746,19 +3839,19 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>425</v>
+        <v>384</v>
       </c>
       <c r="C48" t="s">
         <v>120</v>
       </c>
       <c r="H48" t="s">
-        <v>511</v>
+        <v>469</v>
       </c>
       <c r="K48" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="M48" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="N48" t="s">
         <v>121</v>
@@ -3770,7 +3863,7 @@
         <v>57</v>
       </c>
       <c r="Q48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -3778,19 +3871,19 @@
         <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>426</v>
+        <v>385</v>
       </c>
       <c r="C49" t="s">
         <v>120</v>
       </c>
       <c r="H49" t="s">
-        <v>512</v>
+        <v>470</v>
       </c>
       <c r="K49" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="M49" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="N49" t="s">
         <v>121</v>
@@ -3800,9 +3893,6 @@
       </c>
       <c r="P49" t="s">
         <v>58</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -3810,19 +3900,19 @@
         <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>427</v>
+        <v>386</v>
       </c>
       <c r="C50" t="s">
         <v>120</v>
       </c>
       <c r="H50" t="s">
-        <v>513</v>
+        <v>471</v>
       </c>
       <c r="K50" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="M50" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="N50" t="s">
         <v>121</v>
@@ -3834,7 +3924,7 @@
         <v>59</v>
       </c>
       <c r="Q50" t="s">
-        <v>342</v>
+        <v>587</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -3842,19 +3932,19 @@
         <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>428</v>
+        <v>387</v>
       </c>
       <c r="C51" t="s">
         <v>120</v>
       </c>
       <c r="H51" t="s">
-        <v>514</v>
+        <v>472</v>
       </c>
       <c r="K51" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="M51" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="N51" t="s">
         <v>121</v>
@@ -3866,7 +3956,7 @@
         <v>60</v>
       </c>
       <c r="Q51" t="s">
-        <v>348</v>
+        <v>588</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -3874,19 +3964,19 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>429</v>
+        <v>388</v>
       </c>
       <c r="C52" t="s">
         <v>120</v>
       </c>
       <c r="H52" t="s">
-        <v>515</v>
+        <v>473</v>
       </c>
       <c r="K52" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="M52" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="N52" t="s">
         <v>121</v>
@@ -3898,7 +3988,7 @@
         <v>61</v>
       </c>
       <c r="Q52" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -3906,19 +3996,19 @@
         <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>430</v>
+        <v>389</v>
       </c>
       <c r="C53" t="s">
         <v>120</v>
       </c>
       <c r="H53" t="s">
-        <v>516</v>
+        <v>474</v>
       </c>
       <c r="K53" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="M53" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="N53" t="s">
         <v>121</v>
@@ -3930,7 +4020,7 @@
         <v>62</v>
       </c>
       <c r="Q53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
@@ -3938,19 +4028,19 @@
         <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>431</v>
+        <v>390</v>
       </c>
       <c r="C54" t="s">
         <v>120</v>
       </c>
       <c r="H54" t="s">
-        <v>517</v>
+        <v>475</v>
       </c>
       <c r="K54" t="s">
-        <v>604</v>
+        <v>559</v>
       </c>
       <c r="M54" t="s">
-        <v>605</v>
+        <v>560</v>
       </c>
       <c r="N54" t="s">
         <v>121</v>
@@ -3962,7 +4052,7 @@
         <v>63</v>
       </c>
       <c r="Q54" t="s">
-        <v>354</v>
+        <v>589</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -3970,16 +4060,16 @@
         <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>432</v>
+        <v>391</v>
       </c>
       <c r="C55" t="s">
         <v>120</v>
       </c>
       <c r="H55" t="s">
-        <v>518</v>
+        <v>476</v>
       </c>
       <c r="K55" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="M55" t="s">
         <v>64</v>
@@ -3994,7 +4084,7 @@
         <v>64</v>
       </c>
       <c r="Q55" t="s">
-        <v>353</v>
+        <v>590</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -4002,31 +4092,31 @@
         <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>433</v>
+        <v>392</v>
       </c>
       <c r="C56" t="s">
         <v>120</v>
       </c>
       <c r="H56" t="s">
-        <v>519</v>
+        <v>477</v>
       </c>
       <c r="K56" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="M56" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="N56" t="s">
         <v>121</v>
       </c>
       <c r="O56">
-        <v>60543</v>
+        <v>60560</v>
       </c>
       <c r="P56" t="s">
         <v>65</v>
       </c>
       <c r="Q56" t="s">
-        <v>355</v>
+        <v>591</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -4034,19 +4124,19 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>434</v>
+        <v>393</v>
       </c>
       <c r="C57" t="s">
         <v>120</v>
       </c>
       <c r="H57" t="s">
-        <v>520</v>
+        <v>478</v>
       </c>
       <c r="K57" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="M57" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="N57" t="s">
         <v>121</v>
@@ -4058,7 +4148,7 @@
         <v>66</v>
       </c>
       <c r="Q57" t="s">
-        <v>356</v>
+        <v>592</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -4066,19 +4156,19 @@
         <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>435</v>
+        <v>394</v>
       </c>
       <c r="C58" t="s">
         <v>120</v>
       </c>
       <c r="H58" t="s">
-        <v>521</v>
+        <v>479</v>
       </c>
       <c r="K58" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="M58" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="N58" t="s">
         <v>121</v>
@@ -4087,10 +4177,10 @@
         <v>60085</v>
       </c>
       <c r="P58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q58" t="s">
-        <v>357</v>
+        <v>593</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -4098,19 +4188,19 @@
         <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>436</v>
+        <v>395</v>
       </c>
       <c r="C59" t="s">
         <v>120</v>
       </c>
       <c r="H59" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="K59" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="M59" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="N59" t="s">
         <v>121</v>
@@ -4119,7 +4209,10 @@
         <v>61350</v>
       </c>
       <c r="P59" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -4127,19 +4220,19 @@
         <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>437</v>
+        <v>396</v>
       </c>
       <c r="C60" t="s">
         <v>120</v>
       </c>
       <c r="H60" t="s">
-        <v>523</v>
+        <v>481</v>
       </c>
       <c r="K60" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="M60" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="N60" t="s">
         <v>121</v>
@@ -4149,9 +4242,6 @@
       </c>
       <c r="P60" t="s">
         <v>69</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -4159,19 +4249,19 @@
         <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>438</v>
+        <v>397</v>
       </c>
       <c r="C61" t="s">
         <v>120</v>
       </c>
       <c r="H61" t="s">
-        <v>524</v>
+        <v>482</v>
       </c>
       <c r="K61" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="M61" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="N61" t="s">
         <v>121</v>
@@ -4183,7 +4273,7 @@
         <v>70</v>
       </c>
       <c r="Q61" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -4191,19 +4281,19 @@
         <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>439</v>
+        <v>398</v>
       </c>
       <c r="C62" t="s">
         <v>120</v>
       </c>
       <c r="H62" t="s">
-        <v>525</v>
+        <v>483</v>
       </c>
       <c r="K62" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="M62" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="N62" t="s">
         <v>121</v>
@@ -4215,7 +4305,7 @@
         <v>71</v>
       </c>
       <c r="Q62" t="s">
-        <v>359</v>
+        <v>595</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -4223,19 +4313,19 @@
         <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>440</v>
+        <v>399</v>
       </c>
       <c r="C63" t="s">
         <v>120</v>
       </c>
       <c r="H63" t="s">
-        <v>526</v>
+        <v>484</v>
       </c>
       <c r="K63" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="M63" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="N63" t="s">
         <v>121</v>
@@ -4247,7 +4337,7 @@
         <v>72</v>
       </c>
       <c r="Q63" t="s">
-        <v>346</v>
+        <v>596</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -4255,19 +4345,19 @@
         <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>441</v>
+        <v>400</v>
       </c>
       <c r="C64" t="s">
         <v>120</v>
       </c>
       <c r="H64" t="s">
-        <v>527</v>
+        <v>485</v>
       </c>
       <c r="K64" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="M64" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="N64" t="s">
         <v>121</v>
@@ -4279,7 +4369,7 @@
         <v>73</v>
       </c>
       <c r="Q64" t="s">
-        <v>344</v>
+        <v>597</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -4287,19 +4377,19 @@
         <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>442</v>
+        <v>401</v>
       </c>
       <c r="C65" t="s">
         <v>120</v>
       </c>
       <c r="H65" t="s">
-        <v>528</v>
+        <v>486</v>
       </c>
       <c r="K65" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="M65" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="N65" t="s">
         <v>121</v>
@@ -4311,7 +4401,7 @@
         <v>74</v>
       </c>
       <c r="Q65" t="s">
-        <v>348</v>
+        <v>598</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -4319,19 +4409,19 @@
         <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>443</v>
+        <v>402</v>
       </c>
       <c r="C66" t="s">
         <v>120</v>
       </c>
       <c r="H66" t="s">
-        <v>529</v>
+        <v>487</v>
       </c>
       <c r="K66" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="M66" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="N66" t="s">
         <v>121</v>
@@ -4343,7 +4433,7 @@
         <v>75</v>
       </c>
       <c r="Q66" t="s">
-        <v>360</v>
+        <v>599</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -4351,19 +4441,19 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>444</v>
+        <v>403</v>
       </c>
       <c r="C67" t="s">
         <v>120</v>
       </c>
       <c r="H67" t="s">
-        <v>530</v>
+        <v>488</v>
       </c>
       <c r="K67" t="s">
-        <v>216</v>
+        <v>600</v>
       </c>
       <c r="M67" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="N67" t="s">
         <v>121</v>
@@ -4375,7 +4465,7 @@
         <v>76</v>
       </c>
       <c r="Q67" t="s">
-        <v>173</v>
+        <v>601</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -4383,19 +4473,19 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>445</v>
+        <v>404</v>
       </c>
       <c r="C68" t="s">
         <v>120</v>
       </c>
       <c r="H68" t="s">
-        <v>531</v>
+        <v>489</v>
       </c>
       <c r="K68" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="M68" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="N68" t="s">
         <v>121</v>
@@ -4407,7 +4497,7 @@
         <v>77</v>
       </c>
       <c r="Q68" t="s">
-        <v>361</v>
+        <v>602</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -4415,19 +4505,19 @@
         <v>60</v>
       </c>
       <c r="B69" t="s">
-        <v>446</v>
+        <v>405</v>
       </c>
       <c r="C69" t="s">
         <v>120</v>
       </c>
       <c r="H69" t="s">
-        <v>532</v>
+        <v>490</v>
       </c>
       <c r="K69" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="M69" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="N69" t="s">
         <v>121</v>
@@ -4439,7 +4529,7 @@
         <v>78</v>
       </c>
       <c r="Q69" t="s">
-        <v>170</v>
+        <v>603</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -4447,19 +4537,19 @@
         <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>447</v>
+        <v>406</v>
       </c>
       <c r="C70" t="s">
         <v>120</v>
       </c>
       <c r="H70" t="s">
-        <v>533</v>
+        <v>491</v>
       </c>
       <c r="K70" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="M70" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="N70" t="s">
         <v>121</v>
@@ -4471,7 +4561,7 @@
         <v>79</v>
       </c>
       <c r="Q70" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -4479,19 +4569,19 @@
         <v>62</v>
       </c>
       <c r="B71" t="s">
-        <v>448</v>
+        <v>407</v>
       </c>
       <c r="C71" t="s">
         <v>120</v>
       </c>
       <c r="H71" t="s">
-        <v>534</v>
+        <v>492</v>
       </c>
       <c r="K71" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M71" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="N71" t="s">
         <v>121</v>
@@ -4503,7 +4593,7 @@
         <v>80</v>
       </c>
       <c r="Q71" t="s">
-        <v>362</v>
+        <v>604</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -4511,19 +4601,19 @@
         <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>449</v>
+        <v>408</v>
       </c>
       <c r="C72" t="s">
         <v>120</v>
       </c>
       <c r="H72" t="s">
-        <v>535</v>
+        <v>493</v>
       </c>
       <c r="K72" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M72" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="N72" t="s">
         <v>121</v>
@@ -4535,7 +4625,7 @@
         <v>81</v>
       </c>
       <c r="Q72" t="s">
-        <v>363</v>
+        <v>605</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -4543,19 +4633,19 @@
         <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>450</v>
+        <v>409</v>
       </c>
       <c r="C73" t="s">
         <v>120</v>
       </c>
       <c r="H73" t="s">
-        <v>536</v>
+        <v>494</v>
       </c>
       <c r="K73" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="M73" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="N73" t="s">
         <v>121</v>
@@ -4567,7 +4657,7 @@
         <v>82</v>
       </c>
       <c r="Q73" t="s">
-        <v>364</v>
+        <v>606</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -4575,19 +4665,19 @@
         <v>65</v>
       </c>
       <c r="B74" t="s">
-        <v>451</v>
+        <v>410</v>
       </c>
       <c r="C74" t="s">
         <v>120</v>
       </c>
       <c r="H74" t="s">
-        <v>537</v>
+        <v>495</v>
       </c>
       <c r="K74" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="M74" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="N74" t="s">
         <v>121</v>
@@ -4599,7 +4689,7 @@
         <v>83</v>
       </c>
       <c r="Q74" t="s">
-        <v>365</v>
+        <v>333</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
@@ -4607,19 +4697,19 @@
         <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>452</v>
+        <v>411</v>
       </c>
       <c r="C75" t="s">
         <v>120</v>
       </c>
       <c r="H75" t="s">
-        <v>538</v>
+        <v>496</v>
       </c>
       <c r="K75" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="M75" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="N75" t="s">
         <v>121</v>
@@ -4631,7 +4721,7 @@
         <v>84</v>
       </c>
       <c r="Q75" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
@@ -4639,19 +4729,19 @@
         <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>453</v>
+        <v>412</v>
       </c>
       <c r="C76" t="s">
         <v>120</v>
       </c>
       <c r="H76" t="s">
-        <v>539</v>
+        <v>497</v>
       </c>
       <c r="K76" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="M76" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="N76" t="s">
         <v>121</v>
@@ -4661,6 +4751,9 @@
       </c>
       <c r="P76" t="s">
         <v>85</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
@@ -4668,19 +4761,19 @@
         <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>454</v>
+        <v>413</v>
       </c>
       <c r="C77" t="s">
         <v>120</v>
       </c>
       <c r="H77" t="s">
-        <v>540</v>
+        <v>498</v>
       </c>
       <c r="K77" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="M77" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="N77" t="s">
         <v>121</v>
@@ -4692,7 +4785,7 @@
         <v>86</v>
       </c>
       <c r="Q77" t="s">
-        <v>173</v>
+        <v>608</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
@@ -4700,19 +4793,19 @@
         <v>69</v>
       </c>
       <c r="B78" t="s">
-        <v>455</v>
+        <v>414</v>
       </c>
       <c r="C78" t="s">
         <v>120</v>
       </c>
       <c r="H78" t="s">
-        <v>541</v>
+        <v>499</v>
       </c>
       <c r="K78" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="M78" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="N78" t="s">
         <v>121</v>
@@ -4724,7 +4817,7 @@
         <v>87</v>
       </c>
       <c r="Q78" t="s">
-        <v>348</v>
+        <v>609</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -4732,19 +4825,19 @@
         <v>70</v>
       </c>
       <c r="B79" t="s">
-        <v>456</v>
+        <v>415</v>
       </c>
       <c r="C79" t="s">
         <v>120</v>
       </c>
       <c r="H79" t="s">
-        <v>542</v>
+        <v>500</v>
       </c>
       <c r="K79" t="s">
-        <v>228</v>
+        <v>610</v>
       </c>
       <c r="M79" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="N79" t="s">
         <v>121</v>
@@ -4756,7 +4849,7 @@
         <v>88</v>
       </c>
       <c r="Q79" t="s">
-        <v>344</v>
+        <v>611</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -4764,19 +4857,19 @@
         <v>71</v>
       </c>
       <c r="B80" t="s">
-        <v>457</v>
+        <v>416</v>
       </c>
       <c r="C80" t="s">
         <v>120</v>
       </c>
       <c r="H80" t="s">
-        <v>543</v>
+        <v>501</v>
       </c>
       <c r="K80" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="M80" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="N80" t="s">
         <v>121</v>
@@ -4788,7 +4881,7 @@
         <v>89</v>
       </c>
       <c r="Q80" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
@@ -4796,16 +4889,16 @@
         <v>72</v>
       </c>
       <c r="B81" t="s">
-        <v>458</v>
+        <v>417</v>
       </c>
       <c r="C81" t="s">
         <v>120</v>
       </c>
       <c r="H81" t="s">
-        <v>544</v>
+        <v>502</v>
       </c>
       <c r="K81" t="s">
-        <v>230</v>
+        <v>612</v>
       </c>
       <c r="M81" t="s">
         <v>90</v>
@@ -4820,7 +4913,7 @@
         <v>90</v>
       </c>
       <c r="Q81" t="s">
-        <v>361</v>
+        <v>613</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
@@ -4828,19 +4921,19 @@
         <v>73</v>
       </c>
       <c r="B82" t="s">
-        <v>459</v>
+        <v>418</v>
       </c>
       <c r="C82" t="s">
         <v>120</v>
       </c>
       <c r="H82" t="s">
-        <v>545</v>
+        <v>503</v>
       </c>
       <c r="K82" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="M82" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="N82" t="s">
         <v>121</v>
@@ -4857,19 +4950,19 @@
         <v>74</v>
       </c>
       <c r="B83" t="s">
-        <v>460</v>
+        <v>419</v>
       </c>
       <c r="C83" t="s">
         <v>120</v>
       </c>
       <c r="H83" t="s">
-        <v>546</v>
+        <v>504</v>
       </c>
       <c r="K83" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="M83" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="N83" t="s">
         <v>121</v>
@@ -4881,7 +4974,7 @@
         <v>92</v>
       </c>
       <c r="Q83" t="s">
-        <v>344</v>
+        <v>614</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
@@ -4889,19 +4982,19 @@
         <v>75</v>
       </c>
       <c r="B84" t="s">
-        <v>461</v>
+        <v>420</v>
       </c>
       <c r="C84" t="s">
         <v>120</v>
       </c>
       <c r="H84" t="s">
-        <v>547</v>
+        <v>505</v>
       </c>
       <c r="K84" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="M84" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="N84" t="s">
         <v>121</v>
@@ -4913,7 +5006,7 @@
         <v>93</v>
       </c>
       <c r="Q84" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
@@ -4921,19 +5014,19 @@
         <v>76</v>
       </c>
       <c r="B85" t="s">
-        <v>462</v>
+        <v>421</v>
       </c>
       <c r="C85" t="s">
         <v>120</v>
       </c>
       <c r="H85" t="s">
-        <v>548</v>
+        <v>506</v>
       </c>
       <c r="K85" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="M85" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="N85" t="s">
         <v>121</v>
@@ -4945,7 +5038,7 @@
         <v>94</v>
       </c>
       <c r="Q85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
@@ -4953,19 +5046,19 @@
         <v>77</v>
       </c>
       <c r="B86" t="s">
-        <v>463</v>
+        <v>422</v>
       </c>
       <c r="C86" t="s">
         <v>120</v>
       </c>
       <c r="H86" t="s">
-        <v>549</v>
+        <v>507</v>
       </c>
       <c r="K86" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="M86" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="N86" t="s">
         <v>121</v>
@@ -4977,7 +5070,7 @@
         <v>95</v>
       </c>
       <c r="Q86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
@@ -4985,19 +5078,19 @@
         <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>464</v>
+        <v>423</v>
       </c>
       <c r="C87" t="s">
         <v>120</v>
       </c>
       <c r="H87" t="s">
-        <v>550</v>
+        <v>508</v>
       </c>
       <c r="K87" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="M87" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="N87" t="s">
         <v>121</v>
@@ -5009,7 +5102,7 @@
         <v>96</v>
       </c>
       <c r="Q87" t="s">
-        <v>368</v>
+        <v>615</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
@@ -5017,19 +5110,19 @@
         <v>79</v>
       </c>
       <c r="B88" t="s">
-        <v>465</v>
+        <v>424</v>
       </c>
       <c r="C88" t="s">
         <v>120</v>
       </c>
       <c r="H88" t="s">
-        <v>551</v>
+        <v>509</v>
       </c>
       <c r="K88" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="M88" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="N88" t="s">
         <v>121</v>
@@ -5041,7 +5134,7 @@
         <v>97</v>
       </c>
       <c r="Q88" t="s">
-        <v>369</v>
+        <v>616</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
@@ -5049,19 +5142,19 @@
         <v>80</v>
       </c>
       <c r="B89" t="s">
-        <v>466</v>
+        <v>425</v>
       </c>
       <c r="C89" t="s">
         <v>120</v>
       </c>
       <c r="H89" t="s">
-        <v>552</v>
+        <v>510</v>
       </c>
       <c r="K89" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="M89" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="N89" t="s">
         <v>121</v>
@@ -5073,7 +5166,7 @@
         <v>98</v>
       </c>
       <c r="Q89" t="s">
-        <v>342</v>
+        <v>617</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
@@ -5081,16 +5174,16 @@
         <v>81</v>
       </c>
       <c r="B90" t="s">
-        <v>467</v>
+        <v>426</v>
       </c>
       <c r="C90" t="s">
         <v>120</v>
       </c>
       <c r="H90" t="s">
-        <v>553</v>
+        <v>618</v>
       </c>
       <c r="K90" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="M90" t="s">
         <v>99</v>
@@ -5105,7 +5198,7 @@
         <v>99</v>
       </c>
       <c r="Q90" t="s">
-        <v>370</v>
+        <v>619</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
@@ -5113,19 +5206,19 @@
         <v>82</v>
       </c>
       <c r="B91" t="s">
-        <v>468</v>
+        <v>427</v>
       </c>
       <c r="C91" t="s">
         <v>120</v>
       </c>
       <c r="H91" t="s">
-        <v>554</v>
+        <v>511</v>
       </c>
       <c r="K91" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="M91" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="N91" t="s">
         <v>121</v>
@@ -5134,10 +5227,10 @@
         <v>62946</v>
       </c>
       <c r="P91" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q91" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
@@ -5145,19 +5238,19 @@
         <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>469</v>
+        <v>428</v>
       </c>
       <c r="C92" t="s">
         <v>120</v>
       </c>
       <c r="H92" t="s">
-        <v>555</v>
+        <v>512</v>
       </c>
       <c r="K92" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="M92" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="N92" t="s">
         <v>121</v>
@@ -5166,10 +5259,10 @@
         <v>62701</v>
       </c>
       <c r="P92" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q92" t="s">
-        <v>371</v>
+        <v>336</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
@@ -5177,19 +5270,19 @@
         <v>84</v>
       </c>
       <c r="B93" t="s">
-        <v>470</v>
+        <v>429</v>
       </c>
       <c r="C93" t="s">
         <v>120</v>
       </c>
       <c r="H93" t="s">
-        <v>556</v>
+        <v>513</v>
       </c>
       <c r="K93" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="M93" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="N93" t="s">
         <v>121</v>
@@ -5198,10 +5291,10 @@
         <v>62681</v>
       </c>
       <c r="P93" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q93" t="s">
-        <v>170</v>
+        <v>620</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
@@ -5209,19 +5302,19 @@
         <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>471</v>
+        <v>430</v>
       </c>
       <c r="C94" t="s">
         <v>120</v>
       </c>
       <c r="H94" t="s">
-        <v>557</v>
+        <v>514</v>
       </c>
       <c r="K94" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="M94" t="s">
-        <v>324</v>
+        <v>621</v>
       </c>
       <c r="N94" t="s">
         <v>121</v>
@@ -5230,10 +5323,7 @@
         <v>62694</v>
       </c>
       <c r="P94" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>348</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
@@ -5241,19 +5331,19 @@
         <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>472</v>
+        <v>431</v>
       </c>
       <c r="C95" t="s">
         <v>120</v>
       </c>
       <c r="H95" t="s">
-        <v>558</v>
+        <v>515</v>
       </c>
       <c r="K95" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="M95" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="N95" t="s">
         <v>121</v>
@@ -5262,10 +5352,7 @@
         <v>62565</v>
       </c>
       <c r="P95" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>173</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
@@ -5273,19 +5360,19 @@
         <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>473</v>
+        <v>432</v>
       </c>
       <c r="C96" t="s">
         <v>120</v>
       </c>
       <c r="H96" t="s">
-        <v>559</v>
+        <v>516</v>
       </c>
       <c r="K96" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="M96" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="N96" t="s">
         <v>121</v>
@@ -5294,10 +5381,10 @@
         <v>62220</v>
       </c>
       <c r="P96" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="Q96" t="s">
-        <v>372</v>
+        <v>622</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
@@ -5305,19 +5392,19 @@
         <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>474</v>
+        <v>433</v>
       </c>
       <c r="C97" t="s">
         <v>120</v>
       </c>
       <c r="H97" t="s">
-        <v>560</v>
+        <v>517</v>
       </c>
       <c r="K97" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="M97" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="N97" t="s">
         <v>121</v>
@@ -5329,7 +5416,7 @@
         <v>106</v>
       </c>
       <c r="Q97" t="s">
-        <v>373</v>
+        <v>623</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
@@ -5337,19 +5424,19 @@
         <v>89</v>
       </c>
       <c r="B98" t="s">
-        <v>475</v>
+        <v>434</v>
       </c>
       <c r="C98" t="s">
         <v>120</v>
       </c>
       <c r="H98" t="s">
-        <v>561</v>
+        <v>518</v>
       </c>
       <c r="K98" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="M98" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="N98" t="s">
         <v>121</v>
@@ -5361,7 +5448,7 @@
         <v>107</v>
       </c>
       <c r="Q98" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
@@ -5369,19 +5456,19 @@
         <v>90</v>
       </c>
       <c r="B99" t="s">
-        <v>476</v>
+        <v>435</v>
       </c>
       <c r="C99" t="s">
         <v>120</v>
       </c>
       <c r="H99" t="s">
-        <v>562</v>
+        <v>519</v>
       </c>
       <c r="K99" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="M99" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="N99" t="s">
         <v>121</v>
@@ -5393,7 +5480,7 @@
         <v>108</v>
       </c>
       <c r="Q99" t="s">
-        <v>374</v>
+        <v>624</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
@@ -5401,19 +5488,19 @@
         <v>91</v>
       </c>
       <c r="B100" t="s">
-        <v>477</v>
+        <v>436</v>
       </c>
       <c r="C100" t="s">
         <v>120</v>
       </c>
       <c r="H100" t="s">
-        <v>563</v>
+        <v>520</v>
       </c>
       <c r="K100" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="M100" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="N100" t="s">
         <v>121</v>
@@ -5425,7 +5512,7 @@
         <v>109</v>
       </c>
       <c r="Q100" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
@@ -5433,19 +5520,19 @@
         <v>92</v>
       </c>
       <c r="B101" t="s">
-        <v>478</v>
+        <v>437</v>
       </c>
       <c r="C101" t="s">
         <v>120</v>
       </c>
       <c r="H101" t="s">
-        <v>564</v>
+        <v>521</v>
       </c>
       <c r="K101" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="M101" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="N101" t="s">
         <v>121</v>
@@ -5457,7 +5544,7 @@
         <v>110</v>
       </c>
       <c r="Q101" t="s">
-        <v>174</v>
+        <v>625</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
@@ -5465,19 +5552,19 @@
         <v>93</v>
       </c>
       <c r="B102" t="s">
-        <v>479</v>
+        <v>438</v>
       </c>
       <c r="C102" t="s">
         <v>120</v>
       </c>
       <c r="H102" t="s">
-        <v>565</v>
+        <v>522</v>
       </c>
       <c r="K102" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="M102" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="N102" t="s">
         <v>121</v>
@@ -5489,7 +5576,7 @@
         <v>111</v>
       </c>
       <c r="Q102" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
@@ -5497,19 +5584,19 @@
         <v>94</v>
       </c>
       <c r="B103" t="s">
-        <v>480</v>
+        <v>439</v>
       </c>
       <c r="C103" t="s">
         <v>120</v>
       </c>
       <c r="H103" t="s">
-        <v>506</v>
+        <v>464</v>
       </c>
       <c r="K103" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="M103" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="N103" t="s">
         <v>121</v>
@@ -5521,7 +5608,7 @@
         <v>112</v>
       </c>
       <c r="Q103" t="s">
-        <v>376</v>
+        <v>626</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
@@ -5529,19 +5616,19 @@
         <v>95</v>
       </c>
       <c r="B104" t="s">
-        <v>481</v>
+        <v>440</v>
       </c>
       <c r="C104" t="s">
         <v>120</v>
       </c>
       <c r="H104" t="s">
-        <v>566</v>
+        <v>523</v>
       </c>
       <c r="K104" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="M104" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="N104" t="s">
         <v>121</v>
@@ -5551,6 +5638,9 @@
       </c>
       <c r="P104" t="s">
         <v>15</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
@@ -5558,19 +5648,19 @@
         <v>96</v>
       </c>
       <c r="B105" t="s">
-        <v>482</v>
+        <v>441</v>
       </c>
       <c r="C105" t="s">
         <v>120</v>
       </c>
       <c r="H105" t="s">
-        <v>567</v>
+        <v>524</v>
       </c>
       <c r="K105" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="M105" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="N105" t="s">
         <v>121</v>
@@ -5582,7 +5672,7 @@
         <v>113</v>
       </c>
       <c r="Q105" t="s">
-        <v>342</v>
+        <v>628</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
@@ -5590,19 +5680,19 @@
         <v>97</v>
       </c>
       <c r="B106" t="s">
-        <v>483</v>
+        <v>442</v>
       </c>
       <c r="C106" t="s">
         <v>120</v>
       </c>
       <c r="H106" t="s">
-        <v>568</v>
+        <v>525</v>
       </c>
       <c r="K106" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="M106" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="N106" t="s">
         <v>121</v>
@@ -5614,7 +5704,7 @@
         <v>114</v>
       </c>
       <c r="Q106" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
@@ -5622,19 +5712,19 @@
         <v>98</v>
       </c>
       <c r="B107" t="s">
-        <v>484</v>
+        <v>443</v>
       </c>
       <c r="C107" t="s">
         <v>120</v>
       </c>
       <c r="H107" t="s">
-        <v>569</v>
+        <v>629</v>
       </c>
       <c r="K107" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="M107" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="N107" t="s">
         <v>121</v>
@@ -5646,7 +5736,7 @@
         <v>115</v>
       </c>
       <c r="Q107" t="s">
-        <v>377</v>
+        <v>630</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
@@ -5654,19 +5744,19 @@
         <v>99</v>
       </c>
       <c r="B108" t="s">
-        <v>485</v>
+        <v>444</v>
       </c>
       <c r="C108" t="s">
         <v>120</v>
       </c>
       <c r="H108" t="s">
-        <v>570</v>
+        <v>526</v>
       </c>
       <c r="K108" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="M108" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="N108" t="s">
         <v>121</v>
@@ -5678,7 +5768,7 @@
         <v>116</v>
       </c>
       <c r="Q108" t="s">
-        <v>378</v>
+        <v>631</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
@@ -5686,16 +5776,16 @@
         <v>100</v>
       </c>
       <c r="B109" t="s">
-        <v>486</v>
+        <v>445</v>
       </c>
       <c r="C109" t="s">
         <v>120</v>
       </c>
       <c r="H109" t="s">
-        <v>571</v>
+        <v>527</v>
       </c>
       <c r="K109" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="M109" t="s">
         <v>76</v>
@@ -5710,7 +5800,7 @@
         <v>117</v>
       </c>
       <c r="Q109" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
@@ -5718,19 +5808,19 @@
         <v>101</v>
       </c>
       <c r="B110" t="s">
-        <v>487</v>
+        <v>446</v>
       </c>
       <c r="C110" t="s">
         <v>120</v>
       </c>
       <c r="H110" t="s">
-        <v>572</v>
+        <v>528</v>
       </c>
       <c r="K110" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="M110" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="N110" t="s">
         <v>121</v>
@@ -5742,7 +5832,7 @@
         <v>118</v>
       </c>
       <c r="Q110" t="s">
-        <v>169</v>
+        <v>632</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
@@ -5750,19 +5840,19 @@
         <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>488</v>
+        <v>447</v>
       </c>
       <c r="C111" t="s">
         <v>120</v>
       </c>
       <c r="H111" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="K111" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="M111" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="N111" t="s">
         <v>121</v>
@@ -5774,11 +5864,14 @@
         <v>119</v>
       </c>
       <c r="Q111" t="s">
-        <v>341</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q8" r:id="rId1" xr:uid="{6F173FB4-FEBF-46C6-8125-972BF506A691}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed lightmode.js, updated cook courthouses
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/il_courts.xlsx
+++ b/docassemble/ILAO/data/sources/il_courts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Downloads\update courthouse list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE28CCEC-93BC-4514-BA13-7FD1779D810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DF0A30-9755-40E7-9C36-0370FC0955C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="570" windowWidth="28800" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1977,9 +1977,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2263,10 +2264,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="Q102" sqref="Q102"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,7 +2573,7 @@
       <c r="P8" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="2" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3050,6 +3051,9 @@
       <c r="C23" t="s">
         <v>120</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="H23" t="s">
         <v>535</v>
       </c>
@@ -3082,6 +3086,9 @@
       <c r="C24" t="s">
         <v>120</v>
       </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
       <c r="H24" t="s">
         <v>536</v>
       </c>
@@ -3114,6 +3121,9 @@
       <c r="C25" t="s">
         <v>120</v>
       </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
       <c r="H25" t="s">
         <v>537</v>
       </c>
@@ -5868,10 +5878,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="Q8" r:id="rId1" xr:uid="{6F173FB4-FEBF-46C6-8125-972BF506A691}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added circuit court numbers to the courts spreadsheet
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/il_courts.xlsx
+++ b/docassemble/ILAO/data/sources/il_courts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Downloads\update courthouse list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DF0A30-9755-40E7-9C36-0370FC0955C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB19EA58-AE97-426A-AEE0-B11446BC642B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="663">
   <si>
     <t>name</t>
   </si>
@@ -1933,6 +1933,87 @@
   </si>
   <si>
     <t>https://bondcountyil.gov/circuit-clerk/</t>
+  </si>
+  <si>
+    <t>circuit</t>
+  </si>
+  <si>
+    <t>Eighth</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Seventeenth</t>
+  </si>
+  <si>
+    <t>Thirteenth</t>
+  </si>
+  <si>
+    <t>Fifthteenth</t>
+  </si>
+  <si>
+    <t>Sixth</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>Fifth</t>
+  </si>
+  <si>
+    <t>Fifith</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Twenty-third</t>
+  </si>
+  <si>
+    <t>Eighteenth</t>
+  </si>
+  <si>
+    <t>Eleventh</t>
+  </si>
+  <si>
+    <t>Ninth</t>
+  </si>
+  <si>
+    <t>Seventh</t>
+  </si>
+  <si>
+    <t>Fourteenth</t>
+  </si>
+  <si>
+    <t>Twenty-first</t>
+  </si>
+  <si>
+    <t>Sixteenth</t>
+  </si>
+  <si>
+    <t>Nineteenth</t>
+  </si>
+  <si>
+    <t>Fifteenth</t>
+  </si>
+  <si>
+    <t>Tenth</t>
+  </si>
+  <si>
+    <t>Twenty-second</t>
+  </si>
+  <si>
+    <t>Twenty-fourth</t>
+  </si>
+  <si>
+    <t>Twentieth</t>
+  </si>
+  <si>
+    <t>Twelfth</t>
   </si>
 </sst>
 </file>
@@ -1977,10 +2058,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2262,36 +2342,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T111"/>
+  <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="U112" sqref="U112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="81.28515625" customWidth="1"/>
-    <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="81.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.109375" customWidth="1"/>
+    <col min="20" max="20" width="9" customWidth="1"/>
+    <col min="21" max="21" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2352,8 +2433,11 @@
       <c r="T1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2384,8 +2468,11 @@
       <c r="Q2" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2416,8 +2503,11 @@
       <c r="Q3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2448,8 +2538,11 @@
       <c r="Q4" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2480,8 +2573,11 @@
       <c r="Q5" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2512,8 +2608,11 @@
       <c r="Q6" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2544,8 +2643,11 @@
       <c r="Q7" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2573,11 +2675,14 @@
       <c r="P8" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2608,8 +2713,11 @@
       <c r="Q9" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2640,8 +2748,11 @@
       <c r="Q10" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2672,8 +2783,11 @@
       <c r="Q11" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2704,8 +2818,11 @@
       <c r="Q12" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2736,8 +2853,11 @@
       <c r="Q13" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2768,8 +2888,11 @@
       <c r="Q14" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2800,8 +2923,11 @@
       <c r="Q15" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2830,8 +2956,11 @@
         <v>33</v>
       </c>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U16" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2865,8 +2994,11 @@
       <c r="Q17" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>103</v>
       </c>
@@ -2900,8 +3032,11 @@
       <c r="Q18" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>104</v>
       </c>
@@ -2935,8 +3070,11 @@
       <c r="Q19" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>105</v>
       </c>
@@ -2970,8 +3108,11 @@
       <c r="Q20" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>106</v>
       </c>
@@ -3005,8 +3146,11 @@
       <c r="Q21" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>107</v>
       </c>
@@ -3040,8 +3184,11 @@
       <c r="Q22" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>108</v>
       </c>
@@ -3075,8 +3222,11 @@
       <c r="Q23" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>109</v>
       </c>
@@ -3110,8 +3260,11 @@
       <c r="Q24" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>110</v>
       </c>
@@ -3145,8 +3298,11 @@
       <c r="Q25" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>17</v>
       </c>
@@ -3177,8 +3333,11 @@
       <c r="Q26" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U26" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>18</v>
       </c>
@@ -3209,8 +3368,11 @@
       <c r="Q27" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U27" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>19</v>
       </c>
@@ -3241,8 +3403,11 @@
       <c r="Q28" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U28" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20</v>
       </c>
@@ -3273,8 +3438,11 @@
       <c r="Q29" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U29" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>21</v>
       </c>
@@ -3305,8 +3473,11 @@
       <c r="Q30" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U30" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>22</v>
       </c>
@@ -3337,8 +3508,11 @@
       <c r="Q31" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U31" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>23</v>
       </c>
@@ -3369,8 +3543,11 @@
       <c r="Q32" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U32" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>24</v>
       </c>
@@ -3401,8 +3578,11 @@
       <c r="Q33" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U33" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>25</v>
       </c>
@@ -3433,8 +3613,11 @@
       <c r="Q34" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U34" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>26</v>
       </c>
@@ -3465,8 +3648,11 @@
       <c r="Q35" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U35" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>27</v>
       </c>
@@ -3497,8 +3683,11 @@
       <c r="Q36" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U36" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>28</v>
       </c>
@@ -3529,8 +3718,11 @@
       <c r="Q37" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U37" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>29</v>
       </c>
@@ -3561,8 +3753,11 @@
       <c r="Q38" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U38" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>30</v>
       </c>
@@ -3593,8 +3788,11 @@
       <c r="Q39" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U39" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>31</v>
       </c>
@@ -3622,8 +3820,11 @@
       <c r="P40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U40" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>32</v>
       </c>
@@ -3654,8 +3855,11 @@
       <c r="Q41" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U41" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>33</v>
       </c>
@@ -3686,8 +3890,11 @@
       <c r="Q42" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U42" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>34</v>
       </c>
@@ -3718,8 +3925,11 @@
       <c r="Q43" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U43" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>35</v>
       </c>
@@ -3747,8 +3957,11 @@
       <c r="P44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U44" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>36</v>
       </c>
@@ -3779,8 +3992,11 @@
       <c r="Q45" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U45" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>37</v>
       </c>
@@ -3811,8 +4027,11 @@
       <c r="Q46" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U46" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>38</v>
       </c>
@@ -3843,8 +4062,11 @@
       <c r="Q47" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U47" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>39</v>
       </c>
@@ -3875,8 +4097,11 @@
       <c r="Q48" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U48" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>40</v>
       </c>
@@ -3904,8 +4129,11 @@
       <c r="P49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U49" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>41</v>
       </c>
@@ -3936,8 +4164,11 @@
       <c r="Q50" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U50" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>42</v>
       </c>
@@ -3968,8 +4199,11 @@
       <c r="Q51" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U51" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>43</v>
       </c>
@@ -4000,8 +4234,11 @@
       <c r="Q52" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U52" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>44</v>
       </c>
@@ -4032,8 +4269,11 @@
       <c r="Q53" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U53" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>45</v>
       </c>
@@ -4064,8 +4304,11 @@
       <c r="Q54" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U54" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>46</v>
       </c>
@@ -4096,8 +4339,11 @@
       <c r="Q55" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U55" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>47</v>
       </c>
@@ -4128,8 +4374,11 @@
       <c r="Q56" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U56" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>48</v>
       </c>
@@ -4160,8 +4409,11 @@
       <c r="Q57" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U57" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>49</v>
       </c>
@@ -4192,8 +4444,11 @@
       <c r="Q58" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U58" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>50</v>
       </c>
@@ -4224,8 +4479,11 @@
       <c r="Q59" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U59" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>51</v>
       </c>
@@ -4253,8 +4511,11 @@
       <c r="P60" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U60" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>52</v>
       </c>
@@ -4285,8 +4546,11 @@
       <c r="Q61" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U61" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>53</v>
       </c>
@@ -4317,8 +4581,11 @@
       <c r="Q62" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U62" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>54</v>
       </c>
@@ -4349,8 +4616,11 @@
       <c r="Q63" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U63" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>55</v>
       </c>
@@ -4381,8 +4651,11 @@
       <c r="Q64" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U64" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>56</v>
       </c>
@@ -4413,8 +4686,11 @@
       <c r="Q65" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U65" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>57</v>
       </c>
@@ -4445,8 +4721,11 @@
       <c r="Q66" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U66" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>58</v>
       </c>
@@ -4477,8 +4756,11 @@
       <c r="Q67" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U67" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>59</v>
       </c>
@@ -4509,8 +4791,11 @@
       <c r="Q68" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U68" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>60</v>
       </c>
@@ -4541,8 +4826,11 @@
       <c r="Q69" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U69" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>61</v>
       </c>
@@ -4573,8 +4861,11 @@
       <c r="Q70" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U70" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>62</v>
       </c>
@@ -4605,8 +4896,11 @@
       <c r="Q71" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U71" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>63</v>
       </c>
@@ -4637,8 +4931,11 @@
       <c r="Q72" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U72" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>64</v>
       </c>
@@ -4669,8 +4966,11 @@
       <c r="Q73" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U73" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>65</v>
       </c>
@@ -4701,8 +5001,11 @@
       <c r="Q74" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U74" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>66</v>
       </c>
@@ -4733,8 +5036,11 @@
       <c r="Q75" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U75" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>67</v>
       </c>
@@ -4765,8 +5071,11 @@
       <c r="Q76" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U76" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>68</v>
       </c>
@@ -4797,8 +5106,11 @@
       <c r="Q77" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U77" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>69</v>
       </c>
@@ -4829,8 +5141,11 @@
       <c r="Q78" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U78" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>70</v>
       </c>
@@ -4861,8 +5176,11 @@
       <c r="Q79" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U79" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>71</v>
       </c>
@@ -4893,8 +5211,11 @@
       <c r="Q80" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U80" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>72</v>
       </c>
@@ -4925,8 +5246,11 @@
       <c r="Q81" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U81" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>73</v>
       </c>
@@ -4954,8 +5278,11 @@
       <c r="P82" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U82" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>74</v>
       </c>
@@ -4986,8 +5313,11 @@
       <c r="Q83" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U83" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>75</v>
       </c>
@@ -5018,8 +5348,11 @@
       <c r="Q84" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U84" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>76</v>
       </c>
@@ -5050,8 +5383,11 @@
       <c r="Q85" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U85" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>77</v>
       </c>
@@ -5082,8 +5418,11 @@
       <c r="Q86" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U86" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>78</v>
       </c>
@@ -5114,8 +5453,11 @@
       <c r="Q87" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U87" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>79</v>
       </c>
@@ -5146,8 +5488,11 @@
       <c r="Q88" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U88" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>80</v>
       </c>
@@ -5178,8 +5523,11 @@
       <c r="Q89" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U89" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>81</v>
       </c>
@@ -5210,8 +5558,11 @@
       <c r="Q90" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U90" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>82</v>
       </c>
@@ -5242,8 +5593,11 @@
       <c r="Q91" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U91" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>83</v>
       </c>
@@ -5274,8 +5628,11 @@
       <c r="Q92" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U92" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>84</v>
       </c>
@@ -5306,8 +5663,11 @@
       <c r="Q93" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U93" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>85</v>
       </c>
@@ -5335,8 +5695,11 @@
       <c r="P94" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U94" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>86</v>
       </c>
@@ -5364,8 +5727,11 @@
       <c r="P95" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U95" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>87</v>
       </c>
@@ -5396,8 +5762,11 @@
       <c r="Q96" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U96" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>88</v>
       </c>
@@ -5428,8 +5797,11 @@
       <c r="Q97" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U97" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>89</v>
       </c>
@@ -5460,8 +5832,11 @@
       <c r="Q98" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U98" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>90</v>
       </c>
@@ -5492,8 +5867,11 @@
       <c r="Q99" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U99" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>91</v>
       </c>
@@ -5524,8 +5902,11 @@
       <c r="Q100" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U100" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>92</v>
       </c>
@@ -5556,8 +5937,11 @@
       <c r="Q101" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U101" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>93</v>
       </c>
@@ -5588,8 +5972,11 @@
       <c r="Q102" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U102" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>94</v>
       </c>
@@ -5620,8 +6007,11 @@
       <c r="Q103" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U103" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>95</v>
       </c>
@@ -5652,8 +6042,11 @@
       <c r="Q104" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U104" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>96</v>
       </c>
@@ -5684,8 +6077,11 @@
       <c r="Q105" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U105" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>97</v>
       </c>
@@ -5716,8 +6112,11 @@
       <c r="Q106" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U106" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>98</v>
       </c>
@@ -5748,8 +6147,11 @@
       <c r="Q107" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U107" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>99</v>
       </c>
@@ -5780,8 +6182,11 @@
       <c r="Q108" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U108" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>100</v>
       </c>
@@ -5812,8 +6217,11 @@
       <c r="Q109" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U109" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>101</v>
       </c>
@@ -5844,8 +6252,11 @@
       <c r="Q110" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U110" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>102</v>
       </c>
@@ -5875,6 +6286,9 @@
       </c>
       <c r="Q111" t="s">
         <v>633</v>
+      </c>
+      <c r="U111" t="s">
+        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>